<commit_message>
Country code 2 alfa,StatRec use '-9' when not in FAO 27
Country code 2 alfa (special case e.g. GB-SCT)
StatRec use '-9' when not in FAO 27
Header text 'Short description' -> 'Field name description'
v1.18.3
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="360">
   <si>
     <t>Type</t>
   </si>
@@ -895,15 +895,6 @@
     <t xml:space="preserve">The intended usage at the time of landing. Codes: “Ind” = industry or “HuC” = human consumption or “None” for logbook registered discards. </t>
   </si>
   <si>
-    <t>Total landings value</t>
-  </si>
-  <si>
-    <t>CLtotalLandingsValue</t>
-  </si>
-  <si>
-    <t>CLtotLanVal</t>
-  </si>
-  <si>
     <t>Sales value in Euro of the field official weight 'CLofficialWeight'. If nessesary the estimated value can be reported. Please report the data source in the field 'CLdataSourceOfScientificWeight'. If logbook registered discards, put NA. Exchange rate by month can be found here: http://appsso.eurostat.ec.europa.eu/nui/show.do?dataset=ei_mfrt_m&amp;lang=en</t>
   </si>
   <si>
@@ -961,9 +952,6 @@
   </si>
   <si>
     <t>Incidential by catch mitigation devices: Sorting grid, functional pingers, seal excluder device and turtle excluder device, unknown, None.</t>
-  </si>
-  <si>
-    <t>Ices statistical rectangle (e.g. 41G9), mandatory for FAO area 27. Use ‘99x9’ if unknown. (Use 'NA' if not fishing in ICES area)</t>
   </si>
   <si>
     <t>GSA subarea, mandatory for FAO area 37 (Mediterranean and Black Sea). (Use 'NA' if not fishing in the area)</t>
@@ -1193,12 +1181,137 @@
       <t>GB-ENG, GB-NIR, GB-SCO and GB-WLS.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>official</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> landings value</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CLtotal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Official</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>LandingsValue</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CLtot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Off</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>LanVal</t>
+    </r>
+  </si>
+  <si>
+    <t>Field Name Description</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ICES statistical rectangle (e.g. 41G9), mandatory for FAO area 27. (Use </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>‘-9’ if unknown or if not fishing in ICES area</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>1-25 000 000</t>
+  </si>
+  <si>
+    <r>
+      <t>1-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>100 000 000 000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>100 000 000</t>
+    </r>
+  </si>
+  <si>
+    <t>Ver 18.1.3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1250,6 +1363,14 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1298,7 +1419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1337,6 +1458,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1620,16 +1744,17 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9" style="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1"/>
     <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
@@ -1648,8 +1773,8 @@
       <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>38</v>
+      <c r="C1" s="16" t="s">
+        <v>354</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>41</v>
@@ -1708,10 +1833,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -1756,7 +1881,7 @@
         <v>237</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -1788,7 +1913,7 @@
         <v>238</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -1802,10 +1927,10 @@
         <v>280</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -1820,7 +1945,7 @@
         <v>281</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
@@ -1884,7 +2009,7 @@
         <v>198</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -1916,7 +2041,7 @@
         <v>198</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12" x14ac:dyDescent="0.2">
@@ -1948,7 +2073,7 @@
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.2">
@@ -2076,7 +2201,7 @@
         <v>201</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>306</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2108,7 +2233,7 @@
         <v>202</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2119,13 +2244,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2137,10 +2262,10 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2151,13 +2276,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -2169,10 +2294,10 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -2437,13 +2562,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>4</v>
@@ -2458,7 +2583,7 @@
         <v>279</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2681,13 +2806,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>284</v>
+        <v>351</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>285</v>
+        <v>352</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>286</v>
+        <v>353</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>14</v>
@@ -2700,7 +2825,7 @@
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2737,13 +2862,13 @@
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>14</v>
@@ -2752,11 +2877,11 @@
         <v>17</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2780,11 +2905,11 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2793,13 +2918,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>4</v>
@@ -2812,7 +2937,12 @@
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="13" t="s">
-        <v>294</v>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -2829,8 +2959,8 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,8 +2980,8 @@
       <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>41</v>
+      <c r="D1" s="16" t="s">
+        <v>354</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>40</v>
@@ -2909,10 +3039,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -2957,7 +3087,7 @@
         <v>239</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.25">
@@ -2989,7 +3119,7 @@
         <v>240</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3003,10 +3133,10 @@
         <v>241</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3021,7 +3151,7 @@
         <v>197</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -3053,7 +3183,7 @@
         <v>198</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3213,7 +3343,7 @@
         <v>201</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>306</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -3245,7 +3375,7 @@
         <v>202</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
@@ -3256,13 +3386,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -3274,10 +3404,10 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3288,13 +3418,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -3306,10 +3436,10 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -3323,10 +3453,10 @@
         <v>230</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -3355,10 +3485,10 @@
         <v>242</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -3384,10 +3514,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>275</v>
@@ -3405,7 +3535,7 @@
         <v>276</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -3483,10 +3613,10 @@
         <v>243</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -3515,10 +3645,10 @@
         <v>244</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -3579,7 +3709,7 @@
         <v>166</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>5</v>
@@ -3589,7 +3719,7 @@
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
@@ -3674,7 +3804,7 @@
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="10" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -3711,7 +3841,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>254</v>
@@ -3767,7 +3897,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>272</v>
@@ -3786,7 +3916,7 @@
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="10" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
@@ -3814,7 +3944,7 @@
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="10" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
@@ -3823,7 +3953,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>274</v>
@@ -3842,7 +3972,7 @@
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="10" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -3870,7 +4000,7 @@
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="10" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -3991,7 +4121,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>258</v>
@@ -4006,7 +4136,7 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="10" t="s">
@@ -4118,7 +4248,7 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>64</v>
+        <v>357</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
@@ -4146,7 +4276,7 @@
         <v>5</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>32</v>
+        <v>358</v>
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9" t="s">
@@ -4174,11 +4304,11 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="10" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More clear and descriptive field names for RSE Bias
More clear and descriptive field names for RSE Bias
CL replacing Landing with Weight
Ranges from 0-X
v1.18.4
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -132,9 +132,6 @@
     <t>1-100 000</t>
   </si>
   <si>
-    <t xml:space="preserve">Value RSE </t>
-  </si>
-  <si>
     <t>Qualitative bias</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
   </si>
   <si>
     <t xml:space="preserve">Integer </t>
-  </si>
-  <si>
-    <t>1-2 500 000</t>
   </si>
   <si>
     <t>Scientific kW Days at sea</t>
@@ -606,18 +600,6 @@
     <t>CEnumUniqVes</t>
   </si>
   <si>
-    <t xml:space="preserve">CEeffortRSE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEeffRSE </t>
-  </si>
-  <si>
-    <t>CEqualitativeBias</t>
-  </si>
-  <si>
-    <t>CEqualBias</t>
-  </si>
-  <si>
     <t>Year 1900 to 2050</t>
   </si>
   <si>
@@ -898,26 +880,13 @@
     <t>Sales value in Euro of the field official weight 'CLofficialWeight'. If nessesary the estimated value can be reported. Please report the data source in the field 'CLdataSourceOfScientificWeight'. If logbook registered discards, put NA. Exchange rate by month can be found here: http://appsso.eurostat.ec.europa.eu/nui/show.do?dataset=ei_mfrt_m&amp;lang=en</t>
   </si>
   <si>
-    <t xml:space="preserve">Scientific Landings RSE </t>
-  </si>
-  <si>
-    <t>CLscientificLandingsRSE</t>
-  </si>
-  <si>
     <t>CLsciLanRSE</t>
   </si>
   <si>
     <t>Scientific Landings qualitative bias</t>
   </si>
   <si>
-    <t>CLscientificLandingsQualitativeBias</t>
-  </si>
-  <si>
     <t>CLsciLanQualBias</t>
-  </si>
-  <si>
-    <t>For estimated data: A semi‐quantitative scale ranging from +++ (large overestimate) to −−− (large underestimate) can be used as in Hyder et al 2017 
-For official data: NA</t>
   </si>
   <si>
     <t>Int</t>
@@ -1273,11 +1242,324 @@
     </r>
   </si>
   <si>
-    <t>1-25 000 000</t>
-  </si>
-  <si>
     <r>
       <t>1-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>100 000 000</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">For estimated data: A semi‐quantitative scale ranging from +++ (large overestimate) to −−− (large underestimate) 
+</t>
+  </si>
+  <si>
+    <r>
+      <t>CL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>scientificWeight</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Landing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>QualitativeBias</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Value RSE </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scientific </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">weight </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Landings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">RSE </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CLscientific</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Weight</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Landings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>RSE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>scientificFishingDays</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>effort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">RSE </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>scientificFishingDaysQ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>ualitativeBias</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>sciFishDay</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Effort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">RSE </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>scientificFishingDaysQ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>ualBias</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>-2 500 000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>-25 000 000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
     </r>
     <r>
       <rPr>
@@ -1290,28 +1572,14 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>1-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>100 000 000</t>
-    </r>
-  </si>
-  <si>
-    <t>Ver 18.1.3</t>
+    <t>Ver 18.1.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1371,6 +1639,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1419,7 +1694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1460,6 +1735,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1747,8 +2025,8 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1768,19 +2046,19 @@
   <sheetData>
     <row r="1" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>0</v>
@@ -1792,27 +2070,27 @@
         <v>2</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -1821,7 +2099,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="12" x14ac:dyDescent="0.2">
@@ -1833,10 +2111,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -1854,7 +2132,7 @@
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
@@ -1863,10 +2141,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>4</v>
@@ -1878,15 +2156,15 @@
         <v>6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
@@ -1895,10 +2173,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>4</v>
@@ -1910,27 +2188,27 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -1942,15 +2220,15 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="8">
         <v>5</v>
@@ -1959,10 +2237,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>4</v>
@@ -1974,15 +2252,15 @@
         <v>6</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="8">
         <v>6</v>
@@ -1991,10 +2269,10 @@
         <v>11</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>4</v>
@@ -2006,15 +2284,15 @@
         <v>6</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -2023,10 +2301,10 @@
         <v>12</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>4</v>
@@ -2038,15 +2316,15 @@
         <v>6</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" s="8">
         <v>8</v>
@@ -2055,10 +2333,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>14</v>
@@ -2073,12 +2351,12 @@
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B11" s="8">
         <v>9</v>
@@ -2087,10 +2365,10 @@
         <v>15</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>14</v>
@@ -2105,12 +2383,12 @@
         <v>15</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" s="8">
         <v>10</v>
@@ -2119,10 +2397,10 @@
         <v>16</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>14</v>
@@ -2137,12 +2415,12 @@
         <v>16</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B13" s="8">
         <v>11</v>
@@ -2151,10 +2429,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>4</v>
@@ -2166,15 +2444,15 @@
         <v>6</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B14" s="8">
         <v>12</v>
@@ -2183,10 +2461,10 @@
         <v>19</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -2198,15 +2476,15 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" s="8">
         <v>13</v>
@@ -2215,10 +2493,10 @@
         <v>20</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>21</v>
@@ -2230,27 +2508,27 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B16" s="8">
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2262,27 +2540,27 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B17" s="8">
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -2294,27 +2572,27 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B18" s="8">
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>14</v>
@@ -2326,15 +2604,15 @@
         <v>6</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B19" s="8">
         <v>17</v>
@@ -2343,10 +2621,10 @@
         <v>22</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>4</v>
@@ -2358,15 +2636,15 @@
         <v>6</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B20" s="8">
         <v>18</v>
@@ -2375,10 +2653,10 @@
         <v>23</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>4</v>
@@ -2390,15 +2668,15 @@
         <v>6</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" s="8">
         <v>19</v>
@@ -2407,10 +2685,10 @@
         <v>24</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8" t="s">
@@ -2420,27 +2698,27 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>122</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -2452,15 +2730,15 @@
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B23" s="8">
         <v>21</v>
@@ -2469,10 +2747,10 @@
         <v>25</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>14</v>
@@ -2484,27 +2762,27 @@
         <v>6</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B24" s="8">
         <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>4</v>
@@ -2516,27 +2794,27 @@
         <v>6</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" s="8">
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>4</v>
@@ -2548,27 +2826,27 @@
         <v>6</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26" s="8">
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>4</v>
@@ -2580,27 +2858,27 @@
         <v>6</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B27" s="8">
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>4</v>
@@ -2612,15 +2890,15 @@
         <v>6</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B28" s="8">
         <v>26</v>
@@ -2629,10 +2907,10 @@
         <v>27</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>4</v>
@@ -2644,27 +2922,27 @@
         <v>6</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B29" s="8">
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>4</v>
@@ -2676,27 +2954,27 @@
         <v>6</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B30" s="8">
         <v>28</v>
       </c>
       <c r="C30" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="D30" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>250</v>
-      </c>
       <c r="E30" s="15" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -2708,10 +2986,10 @@
         <v>6</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2723,10 +3001,10 @@
         <v>28</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>14</v>
@@ -2739,7 +3017,7 @@
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2751,10 +3029,10 @@
         <v>30</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>14</v>
@@ -2767,7 +3045,7 @@
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2779,10 +3057,10 @@
         <v>31</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>4</v>
@@ -2794,10 +3072,10 @@
         <v>6</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="96" x14ac:dyDescent="0.2">
@@ -2806,13 +3084,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>14</v>
@@ -2825,7 +3103,7 @@
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2837,10 +3115,10 @@
         <v>33</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>14</v>
@@ -2853,7 +3131,7 @@
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2862,13 +3140,13 @@
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>285</v>
+        <v>350</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>286</v>
+        <v>351</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>14</v>
@@ -2877,11 +3155,11 @@
         <v>17</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2890,13 +3168,13 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>35</v>
+        <v>349</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>14</v>
@@ -2905,11 +3183,11 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2918,13 +3196,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>289</v>
+        <v>348</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>4</v>
@@ -2937,7 +3215,7 @@
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="13" t="s">
-        <v>291</v>
+        <v>347</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2959,8 +3237,8 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,51 +3250,51 @@
   <sheetData>
     <row r="1" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>354</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -3025,12 +3303,12 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -3039,10 +3317,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -3055,24 +3333,24 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>4</v>
@@ -3081,30 +3359,30 @@
         <v>5</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>4</v>
@@ -3116,27 +3394,27 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3148,15 +3426,15 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="8">
         <v>5</v>
@@ -3165,10 +3443,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>4</v>
@@ -3180,15 +3458,15 @@
         <v>6</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="8">
         <v>6</v>
@@ -3197,10 +3475,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>14</v>
@@ -3215,12 +3493,12 @@
         <v>13</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -3229,10 +3507,10 @@
         <v>15</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>14</v>
@@ -3247,12 +3525,12 @@
         <v>15</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" s="8">
         <v>8</v>
@@ -3261,10 +3539,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>14</v>
@@ -3279,12 +3557,12 @@
         <v>16</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B11" s="8">
         <v>9</v>
@@ -3293,10 +3571,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>4</v>
@@ -3308,15 +3586,15 @@
         <v>6</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" s="8">
         <v>10</v>
@@ -3325,10 +3603,10 @@
         <v>19</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>4</v>
@@ -3340,15 +3618,15 @@
         <v>6</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B13" s="8">
         <v>11</v>
@@ -3357,10 +3635,10 @@
         <v>20</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>21</v>
@@ -3372,27 +3650,27 @@
         <v>6</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B14" s="8">
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -3404,27 +3682,27 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" s="8">
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -3436,27 +3714,27 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B16" s="8">
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -3468,27 +3746,27 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B17" s="8">
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -3500,27 +3778,27 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B18" s="8">
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>4</v>
@@ -3532,27 +3810,27 @@
         <v>6</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B19" s="8">
         <v>17</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>4</v>
@@ -3564,27 +3842,27 @@
         <v>6</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B20" s="8">
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>4</v>
@@ -3596,27 +3874,27 @@
         <v>6</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" s="8">
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -3628,27 +3906,27 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -3660,10 +3938,10 @@
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
@@ -3672,26 +3950,26 @@
         <v>21</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F23" s="8" t="s">
+      <c r="G23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="10" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="96.75" x14ac:dyDescent="0.25">
@@ -3700,26 +3978,26 @@
         <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="10" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
@@ -3728,26 +4006,26 @@
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="10" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="K25" s="6"/>
     </row>
@@ -3757,26 +4035,26 @@
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -3785,26 +4063,26 @@
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="10" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -3813,26 +4091,26 @@
         <v>26</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="36" x14ac:dyDescent="0.25">
@@ -3841,13 +4119,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>14</v>
@@ -3856,11 +4134,11 @@
         <v>17</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="10" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.25">
@@ -3869,13 +4147,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>14</v>
@@ -3884,11 +4162,11 @@
         <v>17</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
@@ -3897,26 +4175,26 @@
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="10" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
@@ -3925,26 +4203,26 @@
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="10" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
@@ -3953,26 +4231,26 @@
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="10" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -3981,26 +4259,26 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="10" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4009,26 +4287,26 @@
         <v>33</v>
       </c>
       <c r="C35" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="G35" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4037,26 +4315,26 @@
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4065,26 +4343,26 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4093,26 +4371,26 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="10" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4121,13 +4399,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>14</v>
@@ -4136,11 +4414,11 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="10" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4149,13 +4427,13 @@
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -4164,11 +4442,11 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4177,13 +4455,13 @@
         <v>39</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D41" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>183</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>14</v>
@@ -4192,11 +4470,11 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4205,13 +4483,13 @@
         <v>40</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D42" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E42" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>186</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>14</v>
@@ -4220,11 +4498,11 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4233,13 +4511,13 @@
         <v>41</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>14</v>
@@ -4248,11 +4526,11 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4264,10 +4542,10 @@
         <v>33</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>14</v>
@@ -4276,11 +4554,11 @@
         <v>5</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -4289,13 +4567,13 @@
         <v>43</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>191</v>
+        <v>352</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>192</v>
+        <v>354</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4304,11 +4582,11 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="10" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
@@ -4317,28 +4595,28 @@
         <v>44</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>193</v>
+        <v>353</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>194</v>
+        <v>355</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G46" s="8" t="s">
-        <v>5</v>
+      <c r="G46" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>6</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed headers on CE
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a5362/Google Drive/code/github/public_RDBES/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049751AF-F228-DA4A-A9CC-9D52998E828A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5340"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="26540" windowHeight="13580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial Landing CL" sheetId="3" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="359">
   <si>
     <t>Type</t>
   </si>
@@ -136,9 +137,6 @@
   </si>
   <si>
     <t>Order</t>
-  </si>
-  <si>
-    <t>Short Description</t>
   </si>
   <si>
     <t>Description</t>
@@ -1578,7 +1576,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2018,47 +2016,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="41.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="41.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>0</v>
@@ -2070,27 +2068,27 @@
         <v>2</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -2099,10 +2097,10 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="7"/>
       <c r="B3" s="8">
         <v>1</v>
@@ -2111,10 +2109,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>312</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>313</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -2130,9 +2128,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="52" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
@@ -2141,10 +2139,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>4</v>
@@ -2156,15 +2154,15 @@
         <v>6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="52" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
@@ -2173,10 +2171,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>4</v>
@@ -2188,27 +2186,27 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>310</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>311</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -2220,15 +2218,15 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="91" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="8">
         <v>5</v>
@@ -2237,10 +2235,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>4</v>
@@ -2252,15 +2250,15 @@
         <v>6</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="52" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="8">
         <v>6</v>
@@ -2269,10 +2267,10 @@
         <v>11</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>4</v>
@@ -2284,15 +2282,15 @@
         <v>6</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -2301,10 +2299,10 @@
         <v>12</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>4</v>
@@ -2316,15 +2314,15 @@
         <v>6</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="8">
         <v>8</v>
@@ -2333,10 +2331,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>14</v>
@@ -2351,12 +2349,12 @@
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="8">
         <v>9</v>
@@ -2365,10 +2363,10 @@
         <v>15</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>14</v>
@@ -2383,12 +2381,12 @@
         <v>15</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="8">
         <v>10</v>
@@ -2397,10 +2395,10 @@
         <v>16</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>14</v>
@@ -2415,12 +2413,12 @@
         <v>16</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="91" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="8">
         <v>11</v>
@@ -2429,10 +2427,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>4</v>
@@ -2444,15 +2442,15 @@
         <v>6</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" s="8">
         <v>12</v>
@@ -2461,10 +2459,10 @@
         <v>19</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -2476,15 +2474,15 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="8">
         <v>13</v>
@@ -2493,10 +2491,10 @@
         <v>20</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>21</v>
@@ -2508,27 +2506,27 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="8">
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2540,27 +2538,27 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="J16" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="J16" s="7" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:10" ht="52" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="8">
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>288</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>289</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -2572,27 +2570,27 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="J17" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="J17" s="7" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:10" ht="52" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="8">
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>14</v>
@@ -2604,15 +2602,15 @@
         <v>6</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="8">
         <v>17</v>
@@ -2621,10 +2619,10 @@
         <v>22</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>4</v>
@@ -2636,15 +2634,15 @@
         <v>6</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="8">
         <v>18</v>
@@ -2653,10 +2651,10 @@
         <v>23</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>4</v>
@@ -2668,15 +2666,15 @@
         <v>6</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" s="8">
         <v>19</v>
@@ -2685,10 +2683,10 @@
         <v>24</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8" t="s">
@@ -2698,27 +2696,27 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>120</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -2730,15 +2728,15 @@
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="8">
         <v>21</v>
@@ -2747,10 +2745,10 @@
         <v>25</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>14</v>
@@ -2762,27 +2760,27 @@
         <v>6</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A24" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="8">
         <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>226</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>4</v>
@@ -2794,27 +2792,27 @@
         <v>6</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" s="8">
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>4</v>
@@ -2826,27 +2824,27 @@
         <v>6</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B26" s="8">
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>4</v>
@@ -2858,27 +2856,27 @@
         <v>6</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" s="8">
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>126</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>4</v>
@@ -2890,15 +2888,15 @@
         <v>6</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="8">
         <v>26</v>
@@ -2907,10 +2905,10 @@
         <v>27</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>4</v>
@@ -2922,27 +2920,27 @@
         <v>6</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="8">
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>239</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>240</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>4</v>
@@ -2954,27 +2952,27 @@
         <v>6</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="J29" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="J29" s="13" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="8">
         <v>28</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D30" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="E30" s="15" t="s">
         <v>244</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>245</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -2986,13 +2984,13 @@
         <v>6</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A31" s="7"/>
       <c r="B31" s="8">
         <v>29</v>
@@ -3001,10 +2999,10 @@
         <v>28</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>130</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>14</v>
@@ -3017,10 +3015,10 @@
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="7"/>
       <c r="B32" s="8">
         <v>30</v>
@@ -3029,10 +3027,10 @@
         <v>30</v>
       </c>
       <c r="D32" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>14</v>
@@ -3045,10 +3043,10 @@
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A33" s="7"/>
       <c r="B33" s="8">
         <v>31</v>
@@ -3057,10 +3055,10 @@
         <v>31</v>
       </c>
       <c r="D33" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>133</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>4</v>
@@ -3072,25 +3070,25 @@
         <v>6</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="91" x14ac:dyDescent="0.15">
       <c r="A34" s="7"/>
       <c r="B34" s="8">
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>342</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>343</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>14</v>
@@ -3103,10 +3101,10 @@
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="52" x14ac:dyDescent="0.15">
       <c r="A35" s="7"/>
       <c r="B35" s="8">
         <v>33</v>
@@ -3115,10 +3113,10 @@
         <v>33</v>
       </c>
       <c r="D35" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>14</v>
@@ -3131,22 +3129,22 @@
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A36" s="7"/>
       <c r="B36" s="8">
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>351</v>
-      </c>
       <c r="E36" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>14</v>
@@ -3155,26 +3153,26 @@
         <v>17</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A37" s="7"/>
       <c r="B37" s="8">
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D37" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>14</v>
@@ -3183,26 +3181,26 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A38" s="7"/>
       <c r="B38" s="8">
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>280</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>281</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>4</v>
@@ -3215,12 +3213,12 @@
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="13" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -3230,71 +3228,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>344</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" ht="26" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -3303,12 +3301,12 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -3317,10 +3315,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>314</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>315</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -3333,24 +3331,24 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="65" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>144</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>4</v>
@@ -3359,30 +3357,30 @@
         <v>5</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="52" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>146</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>4</v>
@@ -3394,27 +3392,27 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="65" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>317</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>318</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3426,15 +3424,15 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="39" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="8">
         <v>5</v>
@@ -3443,10 +3441,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>4</v>
@@ -3458,15 +3456,15 @@
         <v>6</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="8">
         <v>6</v>
@@ -3475,10 +3473,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>14</v>
@@ -3493,12 +3491,12 @@
         <v>13</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -3507,10 +3505,10 @@
         <v>15</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>14</v>
@@ -3525,12 +3523,12 @@
         <v>15</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="8">
         <v>8</v>
@@ -3539,10 +3537,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>14</v>
@@ -3557,12 +3555,12 @@
         <v>16</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="84" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="78" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="8">
         <v>9</v>
@@ -3571,10 +3569,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>4</v>
@@ -3586,15 +3584,15 @@
         <v>6</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="27" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="8">
         <v>10</v>
@@ -3603,10 +3601,10 @@
         <v>19</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>156</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>4</v>
@@ -3618,15 +3616,15 @@
         <v>6</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="27" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="8">
         <v>11</v>
@@ -3635,10 +3633,10 @@
         <v>20</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>21</v>
@@ -3650,27 +3648,27 @@
         <v>6</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="27" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" s="8">
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>308</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>309</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -3682,27 +3680,27 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="J14" s="7" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" ht="65" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="8">
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>284</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>285</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -3714,27 +3712,27 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="J15" s="7" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" ht="40" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="8">
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>319</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>320</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -3746,27 +3744,27 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="8">
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -3778,27 +3776,27 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="53" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="8">
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>4</v>
@@ -3810,27 +3808,27 @@
         <v>6</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="40" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="8">
         <v>17</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>159</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>4</v>
@@ -3842,27 +3840,27 @@
         <v>6</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="40" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="8">
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>4</v>
@@ -3874,27 +3872,27 @@
         <v>6</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" s="8">
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>323</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>324</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -3906,27 +3904,27 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="J21" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="J21" s="13" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -3938,194 +3936,194 @@
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="131" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="8">
         <v>21</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="F23" s="8" t="s">
+      <c r="G23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="96.75" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="92" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="8">
         <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="10" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="53" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="8">
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="8">
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>168</v>
-      </c>
       <c r="F26" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="8">
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="10" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="40" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="8">
         <v>26</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>171</v>
-      </c>
       <c r="F28" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="39" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="8">
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>248</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>249</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>14</v>
@@ -4134,26 +4132,26 @@
         <v>17</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="39" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="8">
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>250</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>251</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>14</v>
@@ -4162,250 +4160,250 @@
         <v>17</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="53" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="8">
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>267</v>
-      </c>
       <c r="F31" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="10" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="40" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="8">
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="F32" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="10" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="40" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="8">
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="10" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="40" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
       <c r="B34" s="8">
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>258</v>
-      </c>
       <c r="F34" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="10" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="26" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="8">
         <v>33</v>
       </c>
       <c r="C35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="G35" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="39" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="8">
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D36" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>177</v>
-      </c>
       <c r="F36" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="10" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="26" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="8">
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="39" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
       <c r="B38" s="8">
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D38" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="E38" s="8" t="s">
-        <v>180</v>
-      </c>
       <c r="F38" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="10" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="39" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="8">
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>14</v>
@@ -4414,26 +4412,26 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="10" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="39" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
       <c r="B40" s="8">
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>261</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>262</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -4442,26 +4440,26 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="26" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
       <c r="B41" s="8">
         <v>39</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>14</v>
@@ -4470,26 +4468,26 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="26" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
       <c r="B42" s="8">
         <v>40</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>14</v>
@@ -4498,26 +4496,26 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="26" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
       <c r="B43" s="8">
         <v>41</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>14</v>
@@ -4526,14 +4524,14 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="39" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
       <c r="B44" s="8">
         <v>42</v>
@@ -4542,10 +4540,10 @@
         <v>33</v>
       </c>
       <c r="D44" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>187</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>188</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>14</v>
@@ -4554,26 +4552,26 @@
         <v>5</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="40" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
       <c r="B45" s="8">
         <v>43</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4582,14 +4580,14 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="10" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="40" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
       <c r="B46" s="8">
         <v>44</v>
@@ -4598,10 +4596,10 @@
         <v>35</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>
@@ -4613,10 +4611,10 @@
         <v>6</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update RDBES Data Model CL CE.xlsx
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a5362/Google Drive/code/github/public_RDBES/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\RDBES\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A244F8E-A754-2F4F-BDC9-EEEEB5611CE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="26540" windowHeight="13580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="26535" windowHeight="13575"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial Landing CL" sheetId="3" r:id="rId1"/>
@@ -1576,7 +1575,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2016,33 +2015,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="41.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="41.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>69</v>
       </c>
@@ -2074,7 +2073,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>82</v>
       </c>
@@ -2100,7 +2099,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="8">
         <v>1</v>
@@ -2128,7 +2127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="52" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>88</v>
       </c>
@@ -2160,7 +2159,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="52" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>88</v>
       </c>
@@ -2192,7 +2191,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>88</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="91" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>88</v>
       </c>
@@ -2256,7 +2255,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="52" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>88</v>
       </c>
@@ -2288,7 +2287,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>88</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>88</v>
       </c>
@@ -2352,7 +2351,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>88</v>
       </c>
@@ -2384,7 +2383,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>88</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>88</v>
       </c>
@@ -2448,7 +2447,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>88</v>
       </c>
@@ -2480,7 +2479,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>88</v>
       </c>
@@ -2512,7 +2511,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>88</v>
       </c>
@@ -2544,7 +2543,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="52" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>88</v>
       </c>
@@ -2563,8 +2562,8 @@
       <c r="F17" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>5</v>
+      <c r="G17" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>6</v>
@@ -2576,7 +2575,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="52" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>88</v>
       </c>
@@ -2608,7 +2607,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>88</v>
       </c>
@@ -2640,7 +2639,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>88</v>
       </c>
@@ -2672,7 +2671,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>88</v>
       </c>
@@ -2702,7 +2701,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2734,7 +2733,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>88</v>
       </c>
@@ -2766,7 +2765,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>88</v>
       </c>
@@ -2798,7 +2797,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>88</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>88</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>88</v>
       </c>
@@ -2894,7 +2893,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>88</v>
       </c>
@@ -2926,7 +2925,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>88</v>
       </c>
@@ -2958,7 +2957,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>88</v>
       </c>
@@ -2990,7 +2989,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="8">
         <v>29</v>
@@ -3018,7 +3017,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="8">
         <v>30</v>
@@ -3046,7 +3045,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="8">
         <v>31</v>
@@ -3076,7 +3075,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="91" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="8">
         <v>32</v>
@@ -3104,7 +3103,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="8">
         <v>33</v>
@@ -3132,7 +3131,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="8">
         <v>34</v>
@@ -3160,7 +3159,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="8">
         <v>35</v>
@@ -3188,7 +3187,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="8">
         <v>36</v>
@@ -3216,7 +3215,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>357</v>
       </c>
@@ -3228,7 +3227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -3239,14 +3238,14 @@
       <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="36.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>69</v>
       </c>
@@ -3278,7 +3277,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>82</v>
       </c>
@@ -3304,7 +3303,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>88</v>
       </c>
@@ -3334,7 +3333,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>88</v>
       </c>
@@ -3366,7 +3365,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="52" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>88</v>
       </c>
@@ -3398,7 +3397,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>88</v>
       </c>
@@ -3430,7 +3429,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>88</v>
       </c>
@@ -3462,7 +3461,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>88</v>
       </c>
@@ -3494,7 +3493,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>88</v>
       </c>
@@ -3526,7 +3525,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>88</v>
       </c>
@@ -3558,7 +3557,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>88</v>
       </c>
@@ -3590,7 +3589,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>88</v>
       </c>
@@ -3622,7 +3621,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>88</v>
       </c>
@@ -3654,7 +3653,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>88</v>
       </c>
@@ -3686,7 +3685,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>88</v>
       </c>
@@ -3718,7 +3717,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>88</v>
       </c>
@@ -3750,7 +3749,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>88</v>
       </c>
@@ -3782,7 +3781,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="53" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>88</v>
       </c>
@@ -3814,7 +3813,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="40" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>88</v>
       </c>
@@ -3846,7 +3845,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="40" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>88</v>
       </c>
@@ -3878,7 +3877,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>88</v>
       </c>
@@ -3910,7 +3909,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>88</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="131" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="8">
         <v>21</v>
@@ -3970,7 +3969,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="92" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="96.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="8">
         <v>22</v>
@@ -3998,7 +3997,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="53" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="8">
         <v>23</v>
@@ -4027,7 +4026,7 @@
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="8">
         <v>24</v>
@@ -4055,7 +4054,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="8">
         <v>25</v>
@@ -4083,7 +4082,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="40" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="8">
         <v>26</v>
@@ -4111,7 +4110,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="39" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="8">
         <v>27</v>
@@ -4139,7 +4138,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="39" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="8">
         <v>28</v>
@@ -4167,7 +4166,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="53" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="8">
         <v>29</v>
@@ -4195,7 +4194,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="40" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="8">
         <v>30</v>
@@ -4223,7 +4222,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="8">
         <v>31</v>
@@ -4251,7 +4250,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="8">
         <v>32</v>
@@ -4279,7 +4278,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="8">
         <v>33</v>
@@ -4307,7 +4306,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="39" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="8">
         <v>34</v>
@@ -4335,7 +4334,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="8">
         <v>35</v>
@@ -4363,7 +4362,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="39" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="8">
         <v>36</v>
@@ -4391,7 +4390,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="39" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="8">
         <v>37</v>
@@ -4419,7 +4418,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="39" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="8">
         <v>38</v>
@@ -4447,7 +4446,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="8">
         <v>39</v>
@@ -4475,7 +4474,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="8">
         <v>40</v>
@@ -4503,7 +4502,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="39" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="8">
         <v>41</v>
@@ -4531,7 +4530,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="39" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" s="8">
         <v>42</v>
@@ -4559,7 +4558,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" s="8">
         <v>43</v>
@@ -4587,7 +4586,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="8">
         <v>44</v>

</xml_diff>

<commit_message>
Update national activity description fields
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="26535" windowHeight="13575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="26535" windowHeight="13575"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial Landing CL" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="361">
   <si>
     <t>Type</t>
   </si>
@@ -722,9 +722,6 @@
     <t>Metier6_FishingActivity</t>
   </si>
   <si>
-    <t xml:space="preserve">Fishing activity (like métier) – National level as defined by each country. </t>
-  </si>
-  <si>
     <t>Harbour_LOCODE</t>
   </si>
   <si>
@@ -1796,6 +1793,34 @@
       </rPr>
       <t xml:space="preserve"> sampling.
 Do not provide overlapping data.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Fishing activity (like métier) – National level as defined by each country.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Each code within this vocabulary should have the relevent ISO_3166 country code pre-pended e.g. "DK_OTB_...".  Countries can request new codes to be added to the list by emailing ICES Data Centre.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fishing activity (like métier) – National level as defined by each country. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Each code within this vocabulary should have the relevent ISO_3166 country code pre-pended e.g. "DK_OTB_...".  Countries can request new codes to be added to the list by emailing ICES Data Centre.</t>
     </r>
   </si>
 </sst>
@@ -2254,9 +2279,9 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2282,7 +2307,7 @@
         <v>36</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>39</v>
@@ -2341,10 +2366,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>307</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>308</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -2386,10 +2411,10 @@
         <v>6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -2418,10 +2443,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2432,13 +2457,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>305</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>306</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -2450,10 +2475,10 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
@@ -2517,7 +2542,7 @@
         <v>190</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2549,7 +2574,7 @@
         <v>190</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12" x14ac:dyDescent="0.2">
@@ -2581,7 +2606,7 @@
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.2">
@@ -2709,7 +2734,7 @@
         <v>193</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2741,7 +2766,7 @@
         <v>194</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2752,13 +2777,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>298</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>299</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2770,10 +2795,10 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="J16" s="7" t="s">
         <v>301</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2784,13 +2809,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>286</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -2802,10 +2827,10 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="J17" s="7" t="s">
         <v>283</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -2901,7 +2926,7 @@
         <v>197</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -2931,7 +2956,7 @@
         <v>198</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2998,7 +3023,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>88</v>
       </c>
@@ -3027,7 +3052,7 @@
         <v>225</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>227</v>
+        <v>359</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3038,7 +3063,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>120</v>
@@ -3070,13 +3095,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>4</v>
@@ -3088,10 +3113,10 @@
         <v>6</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3120,7 +3145,7 @@
         <v>6</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>121</v>
@@ -3166,13 +3191,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>237</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>238</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>4</v>
@@ -3184,10 +3209,10 @@
         <v>6</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3198,13 +3223,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D30" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="E30" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>242</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -3216,10 +3241,10 @@
         <v>6</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3314,13 +3339,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>337</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>338</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>14</v>
@@ -3333,7 +3358,7 @@
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -3361,7 +3386,7 @@
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3370,13 +3395,13 @@
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>346</v>
-      </c>
       <c r="E36" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>14</v>
@@ -3385,11 +3410,11 @@
         <v>17</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3398,7 +3423,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>135</v>
@@ -3413,11 +3438,11 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -3426,13 +3451,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>277</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>278</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>4</v>
@@ -3445,12 +3470,12 @@
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -3466,9 +3491,9 @@
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3486,7 +3511,7 @@
         <v>40</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>39</v>
@@ -3547,10 +3572,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>309</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>310</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -3566,7 +3591,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="84" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>88</v>
       </c>
@@ -3592,10 +3617,10 @@
         <v>45</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.25">
@@ -3624,10 +3649,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3638,13 +3663,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>312</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>313</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3659,7 +3684,7 @@
         <v>189</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -3691,7 +3716,7 @@
         <v>190</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3851,7 +3876,7 @@
         <v>193</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -3883,7 +3908,7 @@
         <v>194</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
@@ -3894,13 +3919,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -3912,10 +3937,10 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>301</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3926,13 +3951,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>282</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -3944,13 +3969,13 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="J15" s="7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>88</v>
       </c>
@@ -3961,10 +3986,10 @@
         <v>222</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>314</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>315</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -3979,7 +4004,7 @@
         <v>225</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>227</v>
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
@@ -3990,13 +4015,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -4022,13 +4047,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>4</v>
@@ -4040,10 +4065,10 @@
         <v>6</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -4118,13 +4143,13 @@
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>318</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>319</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -4136,10 +4161,10 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -4150,13 +4175,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>320</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>321</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -4168,10 +4193,10 @@
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
@@ -4217,7 +4242,7 @@
         <v>162</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>5</v>
@@ -4227,7 +4252,7 @@
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
@@ -4312,7 +4337,7 @@
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -4349,13 +4374,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>245</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>246</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>14</v>
@@ -4368,7 +4393,7 @@
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.25">
@@ -4377,13 +4402,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>247</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>248</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>14</v>
@@ -4396,7 +4421,7 @@
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
@@ -4405,13 +4430,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>264</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>49</v>
@@ -4424,7 +4449,7 @@
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
@@ -4433,13 +4458,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>251</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>252</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>49</v>
@@ -4452,7 +4477,7 @@
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
@@ -4461,13 +4486,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>49</v>
@@ -4480,7 +4505,7 @@
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -4489,13 +4514,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>254</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>255</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>49</v>
@@ -4508,7 +4533,7 @@
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4532,7 +4557,7 @@
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
@@ -4560,7 +4585,7 @@
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="10" t="s">
@@ -4588,7 +4613,7 @@
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
@@ -4616,7 +4641,7 @@
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="10" t="s">
@@ -4629,13 +4654,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>14</v>
@@ -4644,11 +4669,11 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4657,13 +4682,13 @@
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>258</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>259</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -4672,11 +4697,11 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4700,7 +4725,7 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="s">
@@ -4728,7 +4753,7 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
@@ -4756,7 +4781,7 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
@@ -4784,7 +4809,7 @@
         <v>5</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9" t="s">
@@ -4800,10 +4825,10 @@
         <v>68</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4812,11 +4837,11 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
@@ -4828,10 +4853,10 @@
         <v>35</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Updated code list names
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="356">
   <si>
     <t>Type</t>
   </si>
@@ -623,9 +623,6 @@
     <t>SpecWoRMS</t>
   </si>
   <si>
-    <t xml:space="preserve">SpecASFIS </t>
-  </si>
-  <si>
     <t>RS_LandingCategory</t>
   </si>
   <si>
@@ -633,12 +630,6 @@
   </si>
   <si>
     <t>RS_CommercialSizeCategoryScale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS_CommercialSizeCategory     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS_VesselLengthCategory       </t>
   </si>
   <si>
     <t>RS_ExplainDifference</t>
@@ -698,15 +689,9 @@
     <t>For estimated data: A semi‐quantitative scale ranging from +++ (large overestimate) to −−− (large underestimate) can be used as in Hyder et al 2017.</t>
   </si>
   <si>
-    <t>LOCODE_Harbour</t>
-  </si>
-  <si>
     <t>CLcommercialSizeCategory</t>
   </si>
   <si>
-    <t>RS_qualitativeBias</t>
-  </si>
-  <si>
     <t>National fishing activity</t>
   </si>
   <si>
@@ -716,9 +701,6 @@
     <t>CLnatFishAct</t>
   </si>
   <si>
-    <t>RS_nationalFishingActivity</t>
-  </si>
-  <si>
     <t>Metier6_FishingActivity</t>
   </si>
   <si>
@@ -728,15 +710,6 @@
     <t>RS_DataTypeOfScientificWE</t>
   </si>
   <si>
-    <t>RS_dataSourceOfScientificWE</t>
-  </si>
-  <si>
-    <t>RS_DataTypeForScientificWE</t>
-  </si>
-  <si>
-    <t>RS_DataSourceForScientificWE</t>
-  </si>
-  <si>
     <t>National Programme behind scientific effort</t>
   </si>
   <si>
@@ -767,9 +740,6 @@
     <t>CLdeepSeaReg</t>
   </si>
   <si>
-    <t>RS_deepSeaRegulation</t>
-  </si>
-  <si>
     <t>Scientific number of hauls/sets</t>
   </si>
   <si>
@@ -839,9 +809,6 @@
     <t>CEIBmitiDev</t>
   </si>
   <si>
-    <t>RS_incidentialByCatchMitigationDevice</t>
-  </si>
-  <si>
     <t>Official vessel kW*Fishing hours.  It is fine to include partial data.</t>
   </si>
   <si>
@@ -852,9 +819,6 @@
   </si>
   <si>
     <t>Sampling scheme</t>
-  </si>
-  <si>
-    <t>RS_SamplingScheme</t>
   </si>
   <si>
     <t>Lan': Landings categorised as above minimum reference size
@@ -1841,13 +1805,34 @@
       </rPr>
       <t>' if not fishing in the area)</t>
     </r>
+  </si>
+  <si>
+    <t>RS_DataSourceOfScientificWE</t>
+  </si>
+  <si>
+    <t>SpecASFIS</t>
+  </si>
+  <si>
+    <t>RS_CommercialSizeCategory</t>
+  </si>
+  <si>
+    <t>RS_NationalFishingActivity</t>
+  </si>
+  <si>
+    <t>RS_VesselLengthCategory</t>
+  </si>
+  <si>
+    <t>YesNoFields</t>
+  </si>
+  <si>
+    <t>RS_QualitativeBias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1920,6 +1905,20 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1968,7 +1967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2013,6 +2012,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2300,7 +2304,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2312,7 +2316,7 @@
     <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1"/>
     <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="19" customWidth="1"/>
     <col min="10" max="10" width="41.7109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.85546875" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
@@ -2326,7 +2330,7 @@
         <v>36</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>39</v>
@@ -2343,7 +2347,7 @@
       <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="16" t="s">
         <v>111</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -2371,7 +2375,7 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="5" t="s">
         <v>86</v>
       </c>
@@ -2385,10 +2389,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -2399,7 +2403,7 @@
       <c r="H3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="17"/>
       <c r="J3" s="8" t="s">
         <v>7</v>
       </c>
@@ -2429,11 +2433,11 @@
       <c r="H4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>228</v>
+      <c r="I4" s="17" t="s">
+        <v>222</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -2461,11 +2465,11 @@
       <c r="H5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>229</v>
+      <c r="I5" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2476,13 +2480,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -2493,11 +2497,11 @@
       <c r="H6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>271</v>
+      <c r="I6" s="17" t="s">
+        <v>189</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
@@ -2525,7 +2529,7 @@
       <c r="H7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="17" t="s">
         <v>191</v>
       </c>
       <c r="J7" s="7" t="s">
@@ -2557,11 +2561,11 @@
       <c r="H8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="17" t="s">
         <v>190</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2589,11 +2593,11 @@
       <c r="H9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="17" t="s">
         <v>190</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12" x14ac:dyDescent="0.2">
@@ -2621,11 +2625,11 @@
       <c r="H10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="17" t="s">
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.2">
@@ -2653,7 +2657,7 @@
       <c r="H11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="17" t="s">
         <v>15</v>
       </c>
       <c r="J11" s="7" t="s">
@@ -2685,7 +2689,7 @@
       <c r="H12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="7" t="s">
@@ -2717,7 +2721,7 @@
       <c r="H13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="17" t="s">
         <v>192</v>
       </c>
       <c r="J13" s="7" t="s">
@@ -2749,11 +2753,11 @@
       <c r="H14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="17" t="s">
         <v>193</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2781,11 +2785,11 @@
       <c r="H15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="17" t="s">
         <v>194</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2796,13 +2800,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2813,11 +2817,11 @@
       <c r="H16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>299</v>
+      <c r="I16" s="17" t="s">
+        <v>287</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2828,13 +2832,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -2845,14 +2849,14 @@
       <c r="H17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>282</v>
+      <c r="I17" s="17" t="s">
+        <v>270</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>88</v>
       </c>
@@ -2877,7 +2881,7 @@
       <c r="H18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="17" t="s">
         <v>195</v>
       </c>
       <c r="J18" s="7" t="s">
@@ -2909,8 +2913,8 @@
       <c r="H19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>196</v>
+      <c r="I19" s="17" t="s">
+        <v>350</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>75</v>
@@ -2941,11 +2945,11 @@
       <c r="H20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="7" t="s">
-        <v>197</v>
+      <c r="I20" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -2971,11 +2975,11 @@
       <c r="H21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>198</v>
+      <c r="I21" s="17" t="s">
+        <v>197</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3003,8 +3007,8 @@
       <c r="H22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>199</v>
+      <c r="I22" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>76</v>
@@ -3021,7 +3025,7 @@
         <v>25</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>119</v>
@@ -3035,8 +3039,8 @@
       <c r="H23" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="7" t="s">
-        <v>200</v>
+      <c r="I23" s="17" t="s">
+        <v>351</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>77</v>
@@ -3050,13 +3054,13 @@
         <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>4</v>
@@ -3067,11 +3071,11 @@
       <c r="H24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="7" t="s">
-        <v>225</v>
+      <c r="I24" s="17" t="s">
+        <v>352</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3082,7 +3086,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>120</v>
@@ -3099,11 +3103,11 @@
       <c r="H25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>226</v>
+      <c r="I25" s="17" t="s">
+        <v>220</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3114,13 +3118,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>4</v>
@@ -3131,11 +3135,11 @@
       <c r="H26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="7" t="s">
-        <v>269</v>
+      <c r="I26" s="17" t="s">
+        <v>258</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3163,8 +3167,8 @@
       <c r="H27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="7" t="s">
-        <v>227</v>
+      <c r="I27" s="17" t="s">
+        <v>221</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>121</v>
@@ -3195,11 +3199,11 @@
       <c r="H28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="7" t="s">
-        <v>201</v>
+      <c r="I28" s="17" t="s">
+        <v>353</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="84" x14ac:dyDescent="0.2">
@@ -3210,13 +3214,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>4</v>
@@ -3227,11 +3231,11 @@
       <c r="H29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I29" s="7" t="s">
-        <v>238</v>
+      <c r="I29" s="17" t="s">
+        <v>229</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3242,13 +3246,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -3259,11 +3263,11 @@
       <c r="H30" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I30" s="15" t="s">
-        <v>242</v>
+      <c r="I30" s="17" t="s">
+        <v>354</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3289,7 +3293,7 @@
       <c r="H31" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="7"/>
+      <c r="I31" s="17"/>
       <c r="J31" s="7" t="s">
         <v>78</v>
       </c>
@@ -3317,7 +3321,7 @@
       <c r="H32" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I32" s="7"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="7" t="s">
         <v>79</v>
       </c>
@@ -3345,8 +3349,8 @@
       <c r="H33" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="7" t="s">
-        <v>202</v>
+      <c r="I33" s="17" t="s">
+        <v>199</v>
       </c>
       <c r="J33" s="7" t="s">
         <v>80</v>
@@ -3358,13 +3362,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>14</v>
@@ -3375,9 +3379,9 @@
       <c r="H34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I34" s="7"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="7" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -3403,9 +3407,9 @@
       <c r="H35" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I35" s="7"/>
+      <c r="I35" s="17"/>
       <c r="J35" s="7" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3414,13 +3418,13 @@
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>14</v>
@@ -3429,11 +3433,11 @@
         <v>17</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="I36" s="7"/>
+        <v>278</v>
+      </c>
+      <c r="I36" s="17"/>
       <c r="J36" s="7" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3442,7 +3446,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>135</v>
@@ -3457,11 +3461,11 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="I37" s="7"/>
+        <v>278</v>
+      </c>
+      <c r="I37" s="17"/>
       <c r="J37" s="7" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -3470,13 +3474,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>4</v>
@@ -3487,14 +3491,16 @@
       <c r="H38" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I38" s="7"/>
+      <c r="I38" s="17" t="s">
+        <v>355</v>
+      </c>
       <c r="J38" s="13" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -3511,14 +3517,15 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="20" customWidth="1"/>
     <col min="10" max="10" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3530,7 +3537,7 @@
         <v>40</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>39</v>
@@ -3547,8 +3554,8 @@
       <c r="H1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>203</v>
+      <c r="I1" s="16" t="s">
+        <v>200</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>37</v>
@@ -3575,7 +3582,7 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="5" t="s">
         <v>86</v>
       </c>
@@ -3591,10 +3598,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -3605,12 +3612,12 @@
       <c r="H3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="8"/>
+      <c r="I3" s="17"/>
       <c r="J3" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="96" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>88</v>
       </c>
@@ -3635,11 +3642,11 @@
       <c r="H4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>230</v>
+      <c r="I4" s="17" t="s">
+        <v>222</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.25">
@@ -3667,11 +3674,11 @@
       <c r="H5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>231</v>
+      <c r="I5" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3682,13 +3689,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3699,11 +3706,11 @@
       <c r="H6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="17" t="s">
         <v>189</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -3731,11 +3738,11 @@
       <c r="H7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="17" t="s">
         <v>190</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3763,7 +3770,7 @@
       <c r="H8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="17" t="s">
         <v>13</v>
       </c>
       <c r="J8" s="9" t="s">
@@ -3795,7 +3802,7 @@
       <c r="H9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="17" t="s">
         <v>15</v>
       </c>
       <c r="J9" s="9" t="s">
@@ -3827,14 +3834,14 @@
       <c r="H10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="17" t="s">
         <v>16</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="84" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>88</v>
       </c>
@@ -3859,7 +3866,7 @@
       <c r="H11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="17" t="s">
         <v>192</v>
       </c>
       <c r="J11" s="12" t="s">
@@ -3891,11 +3898,11 @@
       <c r="H12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="17" t="s">
         <v>193</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -3923,11 +3930,11 @@
       <c r="H13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="17" t="s">
         <v>194</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
@@ -3938,13 +3945,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -3955,11 +3962,11 @@
       <c r="H14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>299</v>
+      <c r="I14" s="17" t="s">
+        <v>287</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3970,13 +3977,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -3987,11 +3994,11 @@
       <c r="H15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>282</v>
+      <c r="I15" s="17" t="s">
+        <v>270</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
@@ -4002,13 +4009,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -4019,11 +4026,11 @@
       <c r="H16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>225</v>
+      <c r="I16" s="17" t="s">
+        <v>352</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
@@ -4034,13 +4041,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -4051,14 +4058,14 @@
       <c r="H17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>226</v>
+      <c r="I17" s="17" t="s">
+        <v>220</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>88</v>
       </c>
@@ -4066,13 +4073,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>4</v>
@@ -4083,11 +4090,11 @@
       <c r="H18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>266</v>
+      <c r="I18" s="17" t="s">
+        <v>258</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -4115,8 +4122,8 @@
       <c r="H19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>219</v>
+      <c r="I19" s="17" t="s">
+        <v>221</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>121</v>
@@ -4147,11 +4154,11 @@
       <c r="H20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="7" t="s">
-        <v>201</v>
+      <c r="I20" s="17" t="s">
+        <v>353</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="96" x14ac:dyDescent="0.25">
@@ -4162,13 +4169,13 @@
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -4179,14 +4186,14 @@
       <c r="H21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>238</v>
+      <c r="I21" s="17" t="s">
+        <v>229</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>88</v>
       </c>
@@ -4194,13 +4201,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -4211,11 +4218,11 @@
       <c r="H22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>242</v>
+      <c r="I22" s="17" t="s">
+        <v>354</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
@@ -4241,9 +4248,9 @@
       <c r="H23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I23" s="9"/>
+      <c r="I23" s="17"/>
       <c r="J23" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="96.75" x14ac:dyDescent="0.25">
@@ -4261,7 +4268,7 @@
         <v>162</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>5</v>
@@ -4269,9 +4276,9 @@
       <c r="H24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I24" s="9"/>
+      <c r="I24" s="17"/>
       <c r="J24" s="10" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
@@ -4297,9 +4304,9 @@
       <c r="H25" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="9"/>
+      <c r="I25" s="17"/>
       <c r="J25" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="K25" s="6"/>
     </row>
@@ -4326,9 +4333,9 @@
       <c r="H26" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I26" s="9"/>
+      <c r="I26" s="17"/>
       <c r="J26" s="10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -4354,9 +4361,9 @@
       <c r="H27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="17"/>
       <c r="J27" s="10" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -4382,9 +4389,9 @@
       <c r="H28" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I28" s="9"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="36" x14ac:dyDescent="0.25">
@@ -4393,13 +4400,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>14</v>
@@ -4410,9 +4417,9 @@
       <c r="H29" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I29" s="9"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="10" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.25">
@@ -4421,13 +4428,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>14</v>
@@ -4438,9 +4445,9 @@
       <c r="H30" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I30" s="9"/>
+      <c r="I30" s="17"/>
       <c r="J30" s="9" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
@@ -4449,13 +4456,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>49</v>
@@ -4466,9 +4473,9 @@
       <c r="H31" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I31" s="9"/>
+      <c r="I31" s="17"/>
       <c r="J31" s="10" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
@@ -4477,13 +4484,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>49</v>
@@ -4494,9 +4501,9 @@
       <c r="H32" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I32" s="9"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="10" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
@@ -4505,13 +4512,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>49</v>
@@ -4522,9 +4529,9 @@
       <c r="H33" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I33" s="9"/>
+      <c r="I33" s="17"/>
       <c r="J33" s="10" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -4533,13 +4540,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>49</v>
@@ -4550,9 +4557,9 @@
       <c r="H34" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I34" s="9"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="10" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4576,11 +4583,11 @@
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="I35" s="9"/>
+        <v>337</v>
+      </c>
+      <c r="I35" s="17"/>
       <c r="J35" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4604,11 +4611,11 @@
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="I36" s="9"/>
+        <v>337</v>
+      </c>
+      <c r="I36" s="17"/>
       <c r="J36" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4632,11 +4639,11 @@
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="I37" s="9"/>
+        <v>337</v>
+      </c>
+      <c r="I37" s="17"/>
       <c r="J37" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4660,11 +4667,11 @@
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="I38" s="9"/>
+        <v>337</v>
+      </c>
+      <c r="I38" s="17"/>
       <c r="J38" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4673,13 +4680,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>14</v>
@@ -4688,11 +4695,11 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="I39" s="9"/>
+        <v>338</v>
+      </c>
+      <c r="I39" s="17"/>
       <c r="J39" s="10" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4701,13 +4708,13 @@
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -4716,11 +4723,11 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="I40" s="9"/>
+        <v>337</v>
+      </c>
+      <c r="I40" s="17"/>
       <c r="J40" s="9" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4744,11 +4751,11 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="I41" s="9"/>
+        <v>337</v>
+      </c>
+      <c r="I41" s="17"/>
       <c r="J41" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4772,11 +4779,11 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="I42" s="9"/>
+        <v>337</v>
+      </c>
+      <c r="I42" s="17"/>
       <c r="J42" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4800,11 +4807,11 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="I43" s="9"/>
+        <v>339</v>
+      </c>
+      <c r="I43" s="17"/>
       <c r="J43" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4828,11 +4835,11 @@
         <v>5</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="I44" s="9"/>
+        <v>327</v>
+      </c>
+      <c r="I44" s="17"/>
       <c r="J44" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -4844,10 +4851,10 @@
         <v>68</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4856,11 +4863,11 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="I45" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="I45" s="17"/>
       <c r="J45" s="10" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
@@ -4872,10 +4879,10 @@
         <v>35</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>
@@ -4886,11 +4893,11 @@
       <c r="H46" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I46" s="8" t="s">
-        <v>221</v>
+      <c r="I46" s="17" t="s">
+        <v>355</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2 x CE field desc updated
Desc CEnumberOfDominantTrips updated with most: 'days at Sea'
Desc CEscientificFishingDays updated with 'official fishing days'
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\RDBES\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBESpublic\RDBES\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="26535" windowHeight="13575"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="26535" windowHeight="13575" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial Landing CL" sheetId="3" r:id="rId1"/>
@@ -656,10 +656,6 @@
 In the case of small-scale fisheries, one landing can equal one day at sea.</t>
   </si>
   <si>
-    <t>Fishing days after reallocation (e.g. based on VMS analysis)
-Can be equal to official days at sea.</t>
-  </si>
-  <si>
     <t>Vessel kW*Days at sea.</t>
   </si>
   <si>
@@ -974,9 +970,6 @@
     <t>CLincidentalByCatchMitigationDevice</t>
   </si>
   <si>
-    <t>If a trip covers more than one area/rectangle/métier/month the area/rectangle/métier/month with the most fishing is used (see example in E/CL documentation). A trip is defined as the period between when a vessel departs from a port (or factory ship) and arrives at a port (or factory ship) for discharge of the catch.</t>
-  </si>
-  <si>
     <t>Number of fishing days following principles agreed on the 2nd Workshop on Transversal Variables*.</t>
   </si>
   <si>
@@ -1861,6 +1854,55 @@
         <family val="2"/>
       </rPr>
       <t>. If logbook registered discards, put NA. Exchange rate by month can be found here: http://appsso.eurostat.ec.europa.eu/nui/show.do?dataset=ei_mfrt_m&amp;lang=en</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fishing days after reallocation (e.g. based on VMS analysis)
+Can be equal to official </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">fishing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>days.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If a trip covers more than one area/rectangle/métier/month the area/rectangle/métier/month with the most </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Days at Sea'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is used (see example in E/CL documentation). A trip is defined as the period between when a vessel departs from a port (or factory ship) and arrives at a port (or factory ship) for discharge of the catch.</t>
     </r>
   </si>
 </sst>
@@ -2338,8 +2380,8 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -2366,7 +2408,7 @@
         <v>36</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>39</v>
@@ -2425,10 +2467,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>292</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>293</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -2470,10 +2512,10 @@
         <v>6</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -2502,10 +2544,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2516,13 +2558,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>290</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>291</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -2537,7 +2579,7 @@
         <v>189</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
@@ -2601,7 +2643,7 @@
         <v>190</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2633,7 +2675,7 @@
         <v>190</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12" x14ac:dyDescent="0.2">
@@ -2665,7 +2707,7 @@
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.2">
@@ -2793,7 +2835,7 @@
         <v>193</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2825,7 +2867,7 @@
         <v>194</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2836,13 +2878,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>283</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>284</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2854,10 +2896,10 @@
         <v>6</v>
       </c>
       <c r="I16" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="J16" s="7" t="s">
         <v>286</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2868,13 +2910,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>271</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>272</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -2886,10 +2928,10 @@
         <v>6</v>
       </c>
       <c r="I17" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="J17" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -2950,7 +2992,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>75</v>
@@ -2985,7 +3027,7 @@
         <v>196</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -3015,7 +3057,7 @@
         <v>197</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3061,7 +3103,7 @@
         <v>25</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>119</v>
@@ -3076,7 +3118,7 @@
         <v>6</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>77</v>
@@ -3090,13 +3132,13 @@
         <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>219</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>4</v>
@@ -3108,10 +3150,10 @@
         <v>6</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3122,7 +3164,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>120</v>
@@ -3140,7 +3182,7 @@
         <v>6</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J25" s="7" t="s">
         <v>201</v>
@@ -3154,13 +3196,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>4</v>
@@ -3172,10 +3214,10 @@
         <v>6</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3204,7 +3246,7 @@
         <v>6</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>121</v>
@@ -3236,7 +3278,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>202</v>
@@ -3250,13 +3292,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>227</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>228</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>4</v>
@@ -3268,10 +3310,10 @@
         <v>6</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3282,13 +3324,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D30" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E30" s="15" t="s">
         <v>231</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>232</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -3300,10 +3342,10 @@
         <v>6</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3398,13 +3440,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>321</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>323</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>14</v>
@@ -3417,7 +3459,7 @@
       </c>
       <c r="I34" s="17"/>
       <c r="J34" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -3445,7 +3487,7 @@
       </c>
       <c r="I35" s="17"/>
       <c r="J35" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3454,13 +3496,13 @@
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>14</v>
@@ -3469,11 +3511,11 @@
         <v>17</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I36" s="17"/>
       <c r="J36" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3482,7 +3524,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>135</v>
@@ -3497,11 +3539,11 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I37" s="17"/>
       <c r="J37" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -3510,13 +3552,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>264</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>4</v>
@@ -3528,15 +3570,15 @@
         <v>6</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -3552,9 +3594,9 @@
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3573,7 +3615,7 @@
         <v>40</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>39</v>
@@ -3634,10 +3676,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>294</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>295</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -3679,10 +3721,10 @@
         <v>45</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.25">
@@ -3711,10 +3753,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3725,13 +3767,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>297</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>298</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3746,7 +3788,7 @@
         <v>189</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -3778,7 +3820,7 @@
         <v>190</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3938,7 +3980,7 @@
         <v>193</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -3970,7 +4012,7 @@
         <v>194</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
@@ -3981,13 +4023,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>288</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>289</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -3999,10 +4041,10 @@
         <v>6</v>
       </c>
       <c r="I14" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>286</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4013,13 +4055,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>268</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -4031,10 +4073,10 @@
         <v>6</v>
       </c>
       <c r="I15" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
@@ -4045,13 +4087,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>300</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -4063,10 +4105,10 @@
         <v>6</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
@@ -4077,13 +4119,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -4095,7 +4137,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>201</v>
@@ -4109,13 +4151,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>4</v>
@@ -4127,10 +4169,10 @@
         <v>6</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -4159,7 +4201,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>121</v>
@@ -4191,7 +4233,7 @@
         <v>6</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>202</v>
@@ -4205,13 +4247,13 @@
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -4223,10 +4265,10 @@
         <v>6</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.25">
@@ -4237,13 +4279,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>305</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>306</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -4255,10 +4297,10 @@
         <v>6</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
@@ -4304,7 +4346,7 @@
         <v>162</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>5</v>
@@ -4314,7 +4356,7 @@
       </c>
       <c r="I24" s="17"/>
       <c r="J24" s="10" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
@@ -4399,7 +4441,7 @@
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -4427,7 +4469,7 @@
       </c>
       <c r="I28" s="17"/>
       <c r="J28" s="10" t="s">
-        <v>206</v>
+        <v>354</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="36" x14ac:dyDescent="0.25">
@@ -4436,13 +4478,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>235</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>14</v>
@@ -4455,7 +4497,7 @@
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.25">
@@ -4464,13 +4506,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>237</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>14</v>
@@ -4483,7 +4525,7 @@
       </c>
       <c r="I30" s="17"/>
       <c r="J30" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
@@ -4492,13 +4534,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>252</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>253</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>49</v>
@@ -4511,7 +4553,7 @@
       </c>
       <c r="I31" s="17"/>
       <c r="J31" s="10" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
@@ -4520,13 +4562,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>241</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>49</v>
@@ -4539,7 +4581,7 @@
       </c>
       <c r="I32" s="17"/>
       <c r="J32" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
@@ -4548,13 +4590,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>49</v>
@@ -4567,7 +4609,7 @@
       </c>
       <c r="I33" s="17"/>
       <c r="J33" s="10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -4576,13 +4618,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>49</v>
@@ -4595,7 +4637,7 @@
       </c>
       <c r="I34" s="17"/>
       <c r="J34" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4619,11 +4661,11 @@
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I35" s="17"/>
       <c r="J35" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4647,11 +4689,11 @@
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I36" s="17"/>
       <c r="J36" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4675,11 +4717,11 @@
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I37" s="17"/>
       <c r="J37" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4703,11 +4745,11 @@
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I38" s="17"/>
       <c r="J38" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4716,13 +4758,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>14</v>
@@ -4731,11 +4773,11 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I39" s="17"/>
       <c r="J39" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4744,13 +4786,13 @@
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>247</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>248</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -4759,11 +4801,11 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I40" s="17"/>
       <c r="J40" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4787,11 +4829,11 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I41" s="17"/>
       <c r="J41" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4815,11 +4857,11 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I42" s="17"/>
       <c r="J42" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4843,11 +4885,11 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I43" s="17"/>
       <c r="J43" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -4871,11 +4913,11 @@
         <v>5</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I44" s="17"/>
       <c r="J44" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
@@ -4887,10 +4929,10 @@
         <v>68</v>
       </c>
       <c r="D45" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>334</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4899,11 +4941,11 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I45" s="17"/>
       <c r="J45" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
@@ -4915,10 +4957,10 @@
         <v>35</v>
       </c>
       <c r="D46" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>333</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>335</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>
@@ -4930,10 +4972,10 @@
         <v>6</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New version 1.19 no significant change since Sep. 2020
New version 1.19 no significant change since Sep. 2020
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBESpublic\RDBES\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7B7B24-8E28-4815-A783-C2A3645387CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="26535" windowHeight="13575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial Landing CL" sheetId="3" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="357">
   <si>
     <t>Type</t>
   </si>
@@ -132,12 +133,12 @@
     <t>1-100 000</t>
   </si>
   <si>
-    <t>Qualitative bias</t>
-  </si>
-  <si>
     <t>Order</t>
   </si>
   <si>
+    <t>Short Description</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -229,9 +230,6 @@
   </si>
   <si>
     <t>GT Fishing hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Effort RSE </t>
   </si>
   <si>
     <t>Unique combination of fields</t>
@@ -273,6 +271,9 @@
     <t>The estimated scientific weight. Can be the same as official weight or adjusted.</t>
   </si>
   <si>
+    <t>Number of the active unique vessels within the aggregation level. This field should not be aggregated or use for any other purpose that check the number of vessels at the aggregation level of the data.</t>
+  </si>
+  <si>
     <t>Explaining the differences between official weight and scientific weight. Can be “Sample data”, “Unallocated catches”, “Area misreporing”, “Correction for overweight in boxes”.</t>
   </si>
   <si>
@@ -602,9 +603,6 @@
 Division in Mediterranean and Black Seas (e.g. 37.1.1) and NAFO (e.g. 21.1A).</t>
   </si>
   <si>
-    <t>RS_NationalProgram</t>
-  </si>
-  <si>
     <t>ISO_3166</t>
   </si>
   <si>
@@ -623,6 +621,9 @@
     <t>SpecWoRMS</t>
   </si>
   <si>
+    <t xml:space="preserve">SpecASFIS </t>
+  </si>
+  <si>
     <t>RS_LandingCategory</t>
   </si>
   <si>
@@ -630,6 +631,12 @@
   </si>
   <si>
     <t>RS_CommercialSizeCategoryScale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS_CommercialSizeCategory     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS_VesselLengthCategory       </t>
   </si>
   <si>
     <t>RS_ExplainDifference</t>
@@ -685,9 +692,15 @@
     <t>For estimated data: A semi‐quantitative scale ranging from +++ (large overestimate) to −−− (large underestimate) can be used as in Hyder et al 2017.</t>
   </si>
   <si>
+    <t>LOCODE_Harbour</t>
+  </si>
+  <si>
     <t>CLcommercialSizeCategory</t>
   </si>
   <si>
+    <t>RS_qualitativeBias</t>
+  </si>
+  <si>
     <t>National fishing activity</t>
   </si>
   <si>
@@ -697,16 +710,28 @@
     <t>CLnatFishAct</t>
   </si>
   <si>
+    <t>RS_nationalFishingActivity</t>
+  </si>
+  <si>
     <t>Metier6_FishingActivity</t>
   </si>
   <si>
+    <t xml:space="preserve">Fishing activity (like métier) – National level as defined by each country. </t>
+  </si>
+  <si>
     <t>Harbour_LOCODE</t>
   </si>
   <si>
     <t>RS_DataTypeOfScientificWE</t>
   </si>
   <si>
-    <t>National Programme behind scientific effort</t>
+    <t>RS_dataSourceOfScientificWE</t>
+  </si>
+  <si>
+    <t>RS_DataTypeForScientificWE</t>
+  </si>
+  <si>
+    <t>RS_DataSourceForScientificWE</t>
   </si>
   <si>
     <t xml:space="preserve"> Metier 6 fishing activity</t>
@@ -727,6 +752,9 @@
     <t>RS_FishingTechnique</t>
   </si>
   <si>
+    <t>Indicating which fishing technique there have been used. For EU FDI data.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indicating if the fishery is in the deep sea EU regulation ‘Yes’ or not ‘No’. For EU FDI data. </t>
   </si>
   <si>
@@ -736,6 +764,9 @@
     <t>CLdeepSeaReg</t>
   </si>
   <si>
+    <t>RS_deepSeaRegulation</t>
+  </si>
+  <si>
     <t>Scientific number of hauls/sets</t>
   </si>
   <si>
@@ -805,6 +836,9 @@
     <t>CEIBmitiDev</t>
   </si>
   <si>
+    <t>RS_incidentialByCatchMitigationDevice</t>
+  </si>
+  <si>
     <t>Official vessel kW*Fishing hours.  It is fine to include partial data.</t>
   </si>
   <si>
@@ -815,6 +849,9 @@
   </si>
   <si>
     <t>Sampling scheme</t>
+  </si>
+  <si>
+    <t>RS_SamplingScheme</t>
   </si>
   <si>
     <t>Lan': Landings categorised as above minimum reference size
@@ -825,13 +862,7 @@
     <t xml:space="preserve">The intended usage at the time of landing. Codes: “Ind” = industry or “HuC” = human consumption or “None” for logbook registered discards. </t>
   </si>
   <si>
-    <t>CLsciLanRSE</t>
-  </si>
-  <si>
-    <t>Scientific Landings qualitative bias</t>
-  </si>
-  <si>
-    <t>CLsciLanQualBias</t>
+    <t>Sales value in Euro of the field official weight 'CLofficialWeight'. If nessesary the estimated value can be reported. Please report the data source in the field 'CLdataSourceOfScientificWeight'. If logbook registered discards, put NA. Exchange rate by month can be found here: http://appsso.eurostat.ec.europa.eu/nui/show.do?dataset=ei_mfrt_m&amp;lang=en</t>
   </si>
   <si>
     <t>Int</t>
@@ -868,17 +899,13 @@
     <t>Incidential by catch mitigation devices: Sorting grid, functional pingers, seal excluder device and turtle excluder device, unknown, None.</t>
   </si>
   <si>
-    <t>Sampling scheme behind scientific weight e.g. national program (from code list).</t>
+    <t>GSA subarea, mandatory for FAO area 37 (Mediterranean and Black Sea). (Use 'NA' if not fishing in the area)</t>
   </si>
   <si>
     <t>0-999</t>
   </si>
   <si>
     <t>Relative Standard Error of the estimated value of landings. Report as percentage (%).
-For official data: Do not fill in this field</t>
-  </si>
-  <si>
-    <t>Relative Standard Error of the scientific landings. Report as percentage (%).
 For official data: Do not fill in this field</t>
   </si>
   <si>
@@ -887,6 +914,16 @@
 </t>
   </si>
   <si>
+    <t>“Official”: for data coming from official data (e.g. logbooks, sales notes, declarative forms).
+“Estimate”: for data coming from estimates based on sampling
+Do not provide overlapping data.</t>
+  </si>
+  <si>
+    <t>“Official”: for data coming from official data (e.g. logbooks, sales notes, declarative forms).
+“Estimate”: for data coming from estimates based on sampling
+Dot not provide overlapping data.</t>
+  </si>
+  <si>
     <t>Relative Standard Error of the estimated effort. Report as percentage (%).
 For official data: Do not fill in this field</t>
   </si>
@@ -937,12 +974,6 @@
     <t>CLIBmitiDev</t>
   </si>
   <si>
-    <t>CEnationalProgramBehScientificEffort</t>
-  </si>
-  <si>
-    <t>CEnatProgSciEff</t>
-  </si>
-  <si>
     <t>CEnationalFishingActivity</t>
   </si>
   <si>
@@ -997,428 +1028,85 @@
     <t>Official kW fishing hours</t>
   </si>
   <si>
-    <r>
-      <t>ISO 3166 typically alpha-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>2 codes, but also e.g. GB-SCT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>. In the special case where a vessel lands the catch in country A, but the catch is transported directly to country B, it should be registered as if it had been landed in country B.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ISO 3166 alpha-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>2 codes, but also e.g. GB-SCT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>. The flag country of the vessel. This may be different from the landing country (see description of landing country).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Country code using ISO 3166 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">typically </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">alpha-2. The flag country of the vessel. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">E.g. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>GB-ENG, GB-NIR, GB-SCO and GB-WLS.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Total </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>official</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> landings value</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>CLtotal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Official</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>LandingsValue</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>CLtot</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Off</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>LanVal</t>
-    </r>
-  </si>
-  <si>
     <t>Field Name Description</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ICES statistical rectangle (e.g. 41G9), mandatory for FAO area 27. (Use </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>‘-9’ if unknown or if not fishing in ICES area</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>100 000 000</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">For estimated data: A semi‐quantitative scale ranging from +++ (large overestimate) to −−− (large underestimate) 
 </t>
   </si>
   <si>
+    <t xml:space="preserve"> Value RSE </t>
+  </si>
+  <si>
+    <t>Ver 18.1.4</t>
+  </si>
+  <si>
+    <t>CEsamplingScheme</t>
+  </si>
+  <si>
+    <t>CEsampScheme</t>
+  </si>
+  <si>
+    <t>Total official landings value</t>
+  </si>
+  <si>
+    <t>CLtotalOfficialLandingsValue</t>
+  </si>
+  <si>
+    <t>CLtotOffLanVal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scientific weight RSE </t>
+  </si>
+  <si>
+    <t>CLscientificWeightRSE</t>
+  </si>
+  <si>
+    <t>CLscientificWeightQualitativeBias</t>
+  </si>
+  <si>
+    <t>Sampling scheme behind scientific weight e.g. national program (from code list). The countries should send an email to RDBsupport@ices.dk and request their codes for their national programs/sampling schemes.</t>
+  </si>
+  <si>
+    <t>ISO 3166 typically alpha-2 codes, but also e.g. GB-SCT. In the special case where a vessel lands the catch in country A, but the catch is transported directly to country B, it should be registered as if it had been landed in country B.</t>
+  </si>
+  <si>
+    <t>ISO 3166 alpha-2 codes, but also e.g. GB-SCT. The flag country of the vessel. This may be different from the landing country (see description of landing country).</t>
+  </si>
+  <si>
+    <t>ICES statistical rectangle (e.g. 41G9), mandatory for FAO area 27. (Use ‘-9’ if unknown or if not fishing in ICES area)</t>
+  </si>
+  <si>
+    <t>Relative Standard Error of the scientific weight/landings. Report as percentage (%).
+For official data: Do not fill in this field</t>
+  </si>
+  <si>
+    <t>Scientific weight qualitative bias</t>
+  </si>
+  <si>
+    <t>CLsciWeightRSE</t>
+  </si>
+  <si>
+    <t>CLsciWeightQualBias</t>
+  </si>
+  <si>
+    <t>Country code using ISO 3166 typically alpha-2. The flag country of the vessel. E.g. GB-ENG, GB-NIR, GB-SCO and GB-WLS.</t>
+  </si>
+  <si>
+    <t>If a trip covers more than one area/rectangle/métier/month the area/rectangle/métier/month with the most 'Days at Sea' is used (see example in E/CL documentation). A trip is defined as the period between when a vessel departs from a port (or factory ship) and arrives at a port (or factory ship) for discharge of the catch.</t>
+  </si>
+  <si>
+    <t>Fishing days after reallocation (e.g. based on VMS analysis)
+Can be equal to official fishing days.</t>
+  </si>
+  <si>
     <r>
-      <t>CL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>scientificWeight</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Landing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>QualitativeBias</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> Value RSE </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Scientific </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">weight </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Landings</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">RSE </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>CLscientific</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Weight</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Landings</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>RSE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>CE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>scientificFishingDays</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>effort</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">RSE </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>CE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>scientificFishingDaysQ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>ualitativeBias</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>CE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>sciFishDay</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Effort</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">RSE </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>CE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>scientificFishingDaysQ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>ualBias</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
       <t>0</t>
     </r>
     <r>
       <rPr>
         <strike/>
         <sz val="9"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri Light"/>
         <family val="2"/>
       </rPr>
@@ -1435,19 +1123,12 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
       <t>0</t>
     </r>
     <r>
       <rPr>
         <strike/>
         <sz val="9"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri Light"/>
         <family val="2"/>
       </rPr>
@@ -1464,19 +1145,12 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
       <t>0</t>
     </r>
     <r>
       <rPr>
         <strike/>
         <sz val="9"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri Light"/>
         <family val="2"/>
       </rPr>
@@ -1488,429 +1162,33 @@
         <rFont val="Calibri Light"/>
         <family val="2"/>
       </rPr>
-      <t>-</t>
+      <t>-100 000 000 000</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>100 000 000 000</t>
-    </r>
-  </si>
-  <si>
-    <t>Ver 18.1.4</t>
-  </si>
-  <si>
-    <t>Number of active unique vessels within the aggregation level. This field should not be aggregated or use for any other purpose that check the number of vessels at the aggregation level of the data.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Indicating which fishing technique there have been used. For EU FDI data.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>This indicates the fishing technique of the vessel for that year - the fishing technique value is typically used by economists and covers that vessel's activity for the whole year.  This is the same definition as used in the EU Fisheries Depdendent Information data call.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Indicating which fishing technique there have been used. For EU FDI data.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>This indicates the fishing technique of the vessel for that year - the fishing technique value is typically used by economists and covers that vessel's activity for the whole year.  This is the same definition as used in the EU Fisheries Depdendent Information data call.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">“Official”: for data coming from official </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>sources</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> such </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">as those defined by the Control Regulation </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(e.g. logbooks, sales notes, declarative forms).  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>This could also include official estimates of weights or values.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-“Estimate”: for data coming from </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>scientific</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> estimates based on </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>scientific</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> sampling.
-Do not provide overlapping data.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">“Official”: for data coming from official </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>sources</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> such </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">as those defined by the Control Regulation </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(e.g. logbooks, sales notes, declarative forms).  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>This could also include official estimates of effort.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-“Estimate”: for data coming from </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>scientific</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> estimates based on </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>scientific</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> sampling.
-Do not provide overlapping data.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Fishing activity (like métier) – National level as defined by each country.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Each code within this vocabulary should have the relevent ISO_3166 country code pre-pended e.g. "DK_OTB_...".  Countries can request new codes to be added to the list by emailing ICES Data Centre.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fishing activity (like métier) – National level as defined by each country. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Each code within this vocabulary should have the relevent ISO_3166 country code pre-pended e.g. "DK_OTB_...".  Countries can request new codes to be added to the list by emailing ICES Data Centre.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>GSA subarea, mandatory for FAO area 37 (Mediterranean and Black Sea). (Use '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>NotApplicable</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>' if not fishing in the area)</t>
-    </r>
-  </si>
-  <si>
-    <t>RS_DataSourceOfScientificWE</t>
-  </si>
-  <si>
-    <t>SpecASFIS</t>
-  </si>
-  <si>
-    <t>RS_CommercialSizeCategory</t>
-  </si>
-  <si>
-    <t>RS_NationalFishingActivity</t>
-  </si>
-  <si>
-    <t>RS_VesselLengthCategory</t>
-  </si>
-  <si>
-    <t>YesNoFields</t>
-  </si>
-  <si>
-    <t>RS_QualitativeBias</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sales value in Euro of the field official weight 'CLofficialWeight'. If nessesary the estimated value can be reported. Please report the data source in the field </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>CLdataSourceLandingsValue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>'CLdataSourceOfScientificWeight'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>. If logbook registered discards, put NA. Exchange rate by month can be found here: http://appsso.eurostat.ec.europa.eu/nui/show.do?dataset=ei_mfrt_m&amp;lang=en</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fishing days after reallocation (e.g. based on VMS analysis)
-Can be equal to official </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">fishing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>days.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If a trip covers more than one area/rectangle/métier/month the area/rectangle/métier/month with the most </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Days at Sea'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is used (see example in E/CL documentation). A trip is defined as the period between when a vessel departs from a port (or factory ship) and arrives at a port (or factory ship) for discharge of the catch.</t>
-    </r>
+  </si>
+  <si>
+    <t>CEscientificFishingDaysQualitativeBias</t>
+  </si>
+  <si>
+    <t>CEscientificFishingDaysQualBias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEscientificFishingDaysRSE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEsciFishDayRSE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fishing days RSE </t>
+  </si>
+  <si>
+    <t>Fishing days qualitative bias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1957,15 +1235,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1973,29 +1244,8 @@
     <font>
       <strike/>
       <sz val="9"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="9"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2045,7 +1295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2084,17 +1334,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2374,41 +1616,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.73046875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.73046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.86328125" style="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="19" customWidth="1"/>
-    <col min="10" max="10" width="41.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.59765625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="41.73046875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.86328125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>39</v>
@@ -2425,14 +1667,14 @@
       <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="3" t="s">
         <v>111</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>82</v>
       </c>
@@ -2453,12 +1695,12 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="18"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="8">
         <v>1</v>
@@ -2467,10 +1709,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -2481,12 +1723,12 @@
       <c r="H3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="17"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>88</v>
       </c>
@@ -2511,14 +1753,14 @@
       <c r="H4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>221</v>
+      <c r="I4" s="8" t="s">
+        <v>227</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>88</v>
       </c>
@@ -2543,14 +1785,14 @@
       <c r="H5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>346</v>
+      <c r="I5" s="8" t="s">
+        <v>228</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>88</v>
       </c>
@@ -2558,13 +1800,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -2575,14 +1817,14 @@
       <c r="H6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>189</v>
+      <c r="I6" s="8" t="s">
+        <v>270</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>88</v>
       </c>
@@ -2607,14 +1849,14 @@
       <c r="H7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>191</v>
+      <c r="I7" s="7" t="s">
+        <v>190</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>88</v>
       </c>
@@ -2639,14 +1881,14 @@
       <c r="H8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>190</v>
+      <c r="I8" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>88</v>
       </c>
@@ -2671,14 +1913,14 @@
       <c r="H9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>190</v>
+      <c r="I9" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>88</v>
       </c>
@@ -2703,14 +1945,14 @@
       <c r="H10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>88</v>
       </c>
@@ -2735,14 +1977,14 @@
       <c r="H11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>88</v>
       </c>
@@ -2767,14 +2009,14 @@
       <c r="H12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>88</v>
       </c>
@@ -2799,14 +2041,14 @@
       <c r="H13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="17" t="s">
-        <v>192</v>
+      <c r="I13" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>88</v>
       </c>
@@ -2831,14 +2073,14 @@
       <c r="H14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="17" t="s">
-        <v>193</v>
+      <c r="I14" s="7" t="s">
+        <v>192</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>88</v>
       </c>
@@ -2863,14 +2105,14 @@
       <c r="H15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>194</v>
+      <c r="I15" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>88</v>
       </c>
@@ -2878,13 +2120,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2895,14 +2137,14 @@
       <c r="H16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="17" t="s">
-        <v>285</v>
+      <c r="I16" s="7" t="s">
+        <v>296</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>88</v>
       </c>
@@ -2910,31 +2152,31 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="17" t="s">
-        <v>17</v>
+      <c r="G17" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="17" t="s">
-        <v>268</v>
+      <c r="I17" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>88</v>
       </c>
@@ -2959,14 +2201,14 @@
       <c r="H18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="17" t="s">
-        <v>195</v>
+      <c r="I18" s="7" t="s">
+        <v>194</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>88</v>
       </c>
@@ -2991,14 +2233,14 @@
       <c r="H19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="17" t="s">
-        <v>347</v>
+      <c r="I19" s="7" t="s">
+        <v>195</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>88</v>
       </c>
@@ -3023,14 +2265,14 @@
       <c r="H20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="7" t="s">
         <v>196</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>88</v>
       </c>
@@ -3053,14 +2295,14 @@
       <c r="H21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="7" t="s">
         <v>197</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -3085,14 +2327,14 @@
       <c r="H22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="7" t="s">
         <v>198</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>88</v>
       </c>
@@ -3103,13 +2345,13 @@
         <v>25</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>119</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>17</v>
@@ -3117,14 +2359,14 @@
       <c r="H23" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="17" t="s">
-        <v>348</v>
+      <c r="I23" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>88</v>
       </c>
@@ -3132,13 +2374,13 @@
         <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>4</v>
@@ -3149,14 +2391,14 @@
       <c r="H24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="17" t="s">
-        <v>349</v>
+      <c r="I24" s="7" t="s">
+        <v>223</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>88</v>
       </c>
@@ -3164,7 +2406,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>120</v>
@@ -3181,14 +2423,14 @@
       <c r="H25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I25" s="17" t="s">
-        <v>219</v>
+      <c r="I25" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>88</v>
       </c>
@@ -3196,13 +2438,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>306</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>295</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>4</v>
@@ -3213,14 +2455,14 @@
       <c r="H26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="17" t="s">
-        <v>257</v>
+      <c r="I26" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>88</v>
       </c>
@@ -3245,14 +2487,14 @@
       <c r="H27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="17" t="s">
-        <v>220</v>
+      <c r="I27" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>88</v>
       </c>
@@ -3277,14 +2519,14 @@
       <c r="H28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="17" t="s">
-        <v>350</v>
+      <c r="I28" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>88</v>
       </c>
@@ -3292,13 +2534,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>4</v>
@@ -3309,14 +2551,14 @@
       <c r="H29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I29" s="17" t="s">
-        <v>228</v>
+      <c r="I29" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>88</v>
       </c>
@@ -3324,13 +2566,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>230</v>
+        <v>233</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>239</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -3341,14 +2583,14 @@
       <c r="H30" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I30" s="17" t="s">
-        <v>351</v>
+      <c r="I30" s="15" t="s">
+        <v>241</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A31" s="7"/>
       <c r="B31" s="8">
         <v>29</v>
@@ -3371,12 +2613,12 @@
       <c r="H31" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="17"/>
+      <c r="I31" s="7"/>
       <c r="J31" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
       <c r="B32" s="8">
         <v>30</v>
@@ -3399,12 +2641,12 @@
       <c r="H32" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I32" s="17"/>
+      <c r="I32" s="7"/>
       <c r="J32" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="8">
         <v>31</v>
@@ -3427,26 +2669,26 @@
       <c r="H33" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="17" t="s">
-        <v>199</v>
+      <c r="I33" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="J33" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="8">
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>14</v>
@@ -3457,12 +2699,12 @@
       <c r="H34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I34" s="17"/>
+      <c r="I34" s="7"/>
       <c r="J34" s="7" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A35" s="7"/>
       <c r="B35" s="8">
         <v>33</v>
@@ -3485,24 +2727,24 @@
       <c r="H35" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I35" s="17"/>
+      <c r="I35" s="7"/>
       <c r="J35" s="7" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A36" s="7"/>
       <c r="B36" s="8">
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>261</v>
+        <v>343</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>14</v>
@@ -3511,14 +2753,14 @@
         <v>17</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="I36" s="17"/>
+        <v>286</v>
+      </c>
+      <c r="I36" s="7"/>
       <c r="J36" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A37" s="7"/>
       <c r="B37" s="8">
         <v>35</v>
@@ -3539,26 +2781,26 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="I37" s="17"/>
+        <v>286</v>
+      </c>
+      <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A38" s="7"/>
       <c r="B38" s="8">
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>262</v>
+        <v>342</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>263</v>
+        <v>344</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>4</v>
@@ -3569,16 +2811,14 @@
       <c r="H38" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I38" s="17" t="s">
-        <v>352</v>
-      </c>
+      <c r="I38" s="7"/>
       <c r="J38" s="13" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -3588,37 +2828,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" customWidth="1"/>
+    <col min="5" max="5" width="15.265625" customWidth="1"/>
+    <col min="10" max="10" width="36.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>322</v>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>39</v>
+        <v>325</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>38</v>
@@ -3632,14 +2872,14 @@
       <c r="H1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>200</v>
+      <c r="I1" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>82</v>
       </c>
@@ -3660,12 +2900,12 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="18"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>88</v>
       </c>
@@ -3676,10 +2916,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -3690,12 +2930,12 @@
       <c r="H3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="17"/>
+      <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="96" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>88</v>
       </c>
@@ -3720,14 +2960,14 @@
       <c r="H4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>221</v>
+      <c r="I4" s="8" t="s">
+        <v>229</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>88</v>
       </c>
@@ -3752,28 +2992,28 @@
       <c r="H5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>346</v>
+      <c r="I5" s="8" t="s">
+        <v>230</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>88</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>297</v>
+      <c r="C6" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>330</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3784,14 +3024,14 @@
       <c r="H6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>189</v>
+      <c r="I6" s="8" t="s">
+        <v>270</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>88</v>
       </c>
@@ -3816,14 +3056,14 @@
       <c r="H7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>190</v>
+      <c r="I7" s="9" t="s">
+        <v>189</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>88</v>
       </c>
@@ -3848,14 +3088,14 @@
       <c r="H8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>88</v>
       </c>
@@ -3880,14 +3120,14 @@
       <c r="H9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="9" t="s">
         <v>15</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>88</v>
       </c>
@@ -3912,14 +3152,14 @@
       <c r="H10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="9" t="s">
         <v>16</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="84" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="69.75" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>88</v>
       </c>
@@ -3944,14 +3184,14 @@
       <c r="H11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>192</v>
+      <c r="I11" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>88</v>
       </c>
@@ -3976,14 +3216,14 @@
       <c r="H12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>193</v>
+      <c r="I12" s="7" t="s">
+        <v>192</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>88</v>
       </c>
@@ -4008,14 +3248,14 @@
       <c r="H13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="17" t="s">
-        <v>194</v>
+      <c r="I13" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
         <v>88</v>
       </c>
@@ -4023,13 +3263,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -4040,14 +3280,14 @@
       <c r="H14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="17" t="s">
-        <v>285</v>
+      <c r="I14" s="7" t="s">
+        <v>296</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>88</v>
       </c>
@@ -4055,13 +3295,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -4072,14 +3312,14 @@
       <c r="H15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>268</v>
+      <c r="I15" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>88</v>
       </c>
@@ -4087,13 +3327,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -4104,14 +3344,14 @@
       <c r="H16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="17" t="s">
-        <v>349</v>
+      <c r="I16" s="7" t="s">
+        <v>223</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="1" customFormat="1" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>88</v>
       </c>
@@ -4119,13 +3359,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -4136,14 +3376,14 @@
       <c r="H17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="17" t="s">
-        <v>219</v>
+      <c r="I17" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>88</v>
       </c>
@@ -4151,13 +3391,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>4</v>
@@ -4168,14 +3408,14 @@
       <c r="H18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="17" t="s">
-        <v>257</v>
+      <c r="I18" s="7" t="s">
+        <v>265</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>88</v>
       </c>
@@ -4200,14 +3440,14 @@
       <c r="H19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="17" t="s">
-        <v>220</v>
+      <c r="I19" s="7" t="s">
+        <v>217</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>88</v>
       </c>
@@ -4232,14 +3472,14 @@
       <c r="H20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="17" t="s">
-        <v>350</v>
+      <c r="I20" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="96" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="24" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>88</v>
       </c>
@@ -4247,13 +3487,13 @@
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -4264,14 +3504,14 @@
       <c r="H21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="17" t="s">
-        <v>228</v>
+      <c r="I21" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>88</v>
       </c>
@@ -4279,13 +3519,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -4296,14 +3536,14 @@
       <c r="H22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="17" t="s">
-        <v>351</v>
+      <c r="I22" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="117" x14ac:dyDescent="0.45">
       <c r="A23" s="9"/>
       <c r="B23" s="8">
         <v>21</v>
@@ -4326,12 +3566,12 @@
       <c r="H23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I23" s="17"/>
+      <c r="I23" s="9"/>
       <c r="J23" s="10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="96.75" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="82.15" x14ac:dyDescent="0.45">
       <c r="A24" s="9"/>
       <c r="B24" s="8">
         <v>22</v>
@@ -4346,7 +3586,7 @@
         <v>162</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>5</v>
@@ -4354,12 +3594,12 @@
       <c r="H24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I24" s="17"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="10" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A25" s="9"/>
       <c r="B25" s="8">
         <v>23</v>
@@ -4382,13 +3622,13 @@
       <c r="H25" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="17"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="24" x14ac:dyDescent="0.45">
       <c r="A26" s="9"/>
       <c r="B26" s="8">
         <v>24</v>
@@ -4411,12 +3651,12 @@
       <c r="H26" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I26" s="17"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="24" x14ac:dyDescent="0.45">
       <c r="A27" s="9"/>
       <c r="B27" s="8">
         <v>25</v>
@@ -4439,12 +3679,12 @@
       <c r="H27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I27" s="17"/>
+      <c r="I27" s="9"/>
       <c r="J27" s="10" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A28" s="9"/>
       <c r="B28" s="8">
         <v>26</v>
@@ -4467,24 +3707,24 @@
       <c r="H28" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I28" s="17"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="10" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A29" s="9"/>
       <c r="B29" s="8">
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>14</v>
@@ -4495,24 +3735,24 @@
       <c r="H29" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I29" s="17"/>
+      <c r="I29" s="9"/>
       <c r="J29" s="10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A30" s="9"/>
       <c r="B30" s="8">
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>14</v>
@@ -4523,24 +3763,24 @@
       <c r="H30" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I30" s="17"/>
+      <c r="I30" s="9"/>
       <c r="J30" s="9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A31" s="9"/>
       <c r="B31" s="8">
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>49</v>
@@ -4551,24 +3791,24 @@
       <c r="H31" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I31" s="17"/>
+      <c r="I31" s="9"/>
       <c r="J31" s="10" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A32" s="9"/>
       <c r="B32" s="8">
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>49</v>
@@ -4579,24 +3819,24 @@
       <c r="H32" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I32" s="17"/>
+      <c r="I32" s="9"/>
       <c r="J32" s="10" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A33" s="9"/>
       <c r="B33" s="8">
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>49</v>
@@ -4607,24 +3847,24 @@
       <c r="H33" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I33" s="17"/>
+      <c r="I33" s="9"/>
       <c r="J33" s="10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A34" s="9"/>
       <c r="B34" s="8">
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>49</v>
@@ -4635,12 +3875,12 @@
       <c r="H34" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I34" s="17"/>
+      <c r="I34" s="9"/>
       <c r="J34" s="10" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A35" s="9"/>
       <c r="B35" s="8">
         <v>33</v>
@@ -4661,14 +3901,14 @@
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="I35" s="17"/>
+        <v>348</v>
+      </c>
+      <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A36" s="9"/>
       <c r="B36" s="8">
         <v>34</v>
@@ -4689,14 +3929,14 @@
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="I36" s="17"/>
+        <v>348</v>
+      </c>
+      <c r="I36" s="9"/>
       <c r="J36" s="10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A37" s="9"/>
       <c r="B37" s="8">
         <v>35</v>
@@ -4717,14 +3957,14 @@
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="I37" s="17"/>
+        <v>348</v>
+      </c>
+      <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A38" s="9"/>
       <c r="B38" s="8">
         <v>36</v>
@@ -4745,26 +3985,26 @@
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="I38" s="17"/>
+        <v>348</v>
+      </c>
+      <c r="I38" s="9"/>
       <c r="J38" s="10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A39" s="9"/>
       <c r="B39" s="8">
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>14</v>
@@ -4773,26 +4013,26 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="I39" s="17"/>
+        <v>349</v>
+      </c>
+      <c r="I39" s="9"/>
       <c r="J39" s="10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A40" s="9"/>
       <c r="B40" s="8">
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -4801,14 +4041,14 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="I40" s="17"/>
+        <v>348</v>
+      </c>
+      <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A41" s="9"/>
       <c r="B41" s="8">
         <v>39</v>
@@ -4829,14 +4069,14 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="I41" s="17"/>
+        <v>348</v>
+      </c>
+      <c r="I41" s="9"/>
       <c r="J41" s="9" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A42" s="9"/>
       <c r="B42" s="8">
         <v>40</v>
@@ -4857,14 +4097,14 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="I42" s="17"/>
+        <v>348</v>
+      </c>
+      <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A43" s="9"/>
       <c r="B43" s="8">
         <v>41</v>
@@ -4885,14 +4125,14 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="I43" s="17"/>
+        <v>350</v>
+      </c>
+      <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A44" s="9"/>
       <c r="B44" s="8">
         <v>42</v>
@@ -4913,26 +4153,26 @@
         <v>5</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="I44" s="17"/>
+        <v>32</v>
+      </c>
+      <c r="I44" s="9"/>
       <c r="J44" s="9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A45" s="9"/>
       <c r="B45" s="8">
         <v>43</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>68</v>
+        <v>355</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>332</v>
+        <v>354</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4941,41 +4181,41 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="I45" s="17"/>
+        <v>286</v>
+      </c>
+      <c r="I45" s="9"/>
       <c r="J45" s="10" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A46" s="9"/>
       <c r="B46" s="8">
         <v>44</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>35</v>
+        <v>356</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>333</v>
+        <v>352</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G46" s="17" t="s">
+      <c r="G46" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I46" s="17" t="s">
-        <v>352</v>
+      <c r="I46" s="8" t="s">
+        <v>219</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New version 1.19.1 new field added CLregDisCategory
'When 'RegDis' have been selected in the CLcatchCategory, Logbook registered discard category can be specified
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7B7B24-8E28-4815-A783-C2A3645387CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406EE25A-479C-4DCC-B38F-6761E18AFDD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="363">
   <si>
     <t>Type</t>
   </si>
@@ -1182,6 +1182,24 @@
   </si>
   <si>
     <t>Fishing days qualitative bias</t>
+  </si>
+  <si>
+    <t>CLregDisCategory</t>
+  </si>
+  <si>
+    <t>CLregDisCat</t>
+  </si>
+  <si>
+    <t>RS_regDisCategory</t>
+  </si>
+  <si>
+    <t>(New)</t>
+  </si>
+  <si>
+    <t>Logbook registered discard category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When 'RegDis' have been selected in the CLcatchCategory, Logbook registered discard category can be specified </t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1336,6 +1354,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1620,11 +1641,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -2288,7 +2309,9 @@
       <c r="E21" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="G21" s="8" t="s">
         <v>5</v>
       </c>
@@ -2303,20 +2326,20 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
-        <v>88</v>
+      <c r="A22" s="17" t="s">
+        <v>360</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>117</v>
+        <v>361</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>116</v>
+        <v>357</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>118</v>
+        <v>358</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -2328,10 +2351,10 @@
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>75</v>
+        <v>359</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2342,13 +2365,13 @@
         <v>21</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>218</v>
+        <v>116</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>4</v>
@@ -2360,10 +2383,10 @@
         <v>6</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2374,13 +2397,13 @@
         <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>220</v>
+        <v>25</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>222</v>
+        <v>119</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>4</v>
@@ -2392,10 +2415,10 @@
         <v>6</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>225</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2406,31 +2429,31 @@
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>120</v>
+        <v>221</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>120</v>
+        <v>222</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>6</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>88</v>
       </c>
@@ -2438,13 +2461,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>283</v>
+        <v>231</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>315</v>
+        <v>120</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>306</v>
+        <v>120</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>4</v>
@@ -2456,10 +2479,10 @@
         <v>6</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>268</v>
+        <v>224</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>284</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2470,28 +2493,28 @@
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>122</v>
+        <v>283</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>123</v>
+        <v>315</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>124</v>
+        <v>306</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>6</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>226</v>
+        <v>268</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>121</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2502,31 +2525,31 @@
         <v>26</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>6</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>88</v>
       </c>
@@ -2534,28 +2557,28 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>232</v>
+        <v>27</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>234</v>
+        <v>125</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>235</v>
+        <v>126</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>6</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="J29" s="13" t="s">
-        <v>237</v>
+        <v>200</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2565,14 +2588,14 @@
       <c r="B30" s="8">
         <v>28</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>233</v>
+      <c r="C30" s="8" t="s">
+        <v>232</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>240</v>
+        <v>234</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -2583,39 +2606,43 @@
       <c r="H30" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I30" s="15" t="s">
-        <v>241</v>
+      <c r="I30" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
+      <c r="A31" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="B31" s="8">
         <v>29</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>28</v>
+      <c r="C31" s="15" t="s">
+        <v>233</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>128</v>
+        <v>239</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>240</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7" t="s">
-        <v>77</v>
+        <v>6</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2624,13 +2651,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>14</v>
@@ -2643,80 +2670,80 @@
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="8">
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>201</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="I33" s="7"/>
       <c r="J33" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="8">
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>331</v>
+        <v>31</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>332</v>
+        <v>131</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>333</v>
+        <v>132</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I34" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>201</v>
+      </c>
       <c r="J34" s="7" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A35" s="7"/>
       <c r="B35" s="8">
         <v>33</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>33</v>
+        <v>331</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>133</v>
+        <v>332</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>134</v>
+        <v>333</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>14</v>
@@ -2725,39 +2752,39 @@
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A36" s="7"/>
       <c r="B36" s="8">
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>334</v>
+        <v>33</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>335</v>
+        <v>133</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>343</v>
+        <v>134</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>286</v>
+        <v>34</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="s">
-        <v>341</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2766,13 +2793,13 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>135</v>
+        <v>335</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>136</v>
+        <v>343</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>14</v>
@@ -2785,7 +2812,7 @@
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>287</v>
+        <v>341</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2794,30 +2821,58 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>336</v>
+        <v>135</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>344</v>
+        <v>136</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>6</v>
+        <v>286</v>
       </c>
       <c r="I38" s="7"/>
-      <c r="J38" s="13" t="s">
+      <c r="J38" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8">
+        <v>37</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I39" s="7"/>
+      <c r="J39" s="13" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+    <row r="41" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>328</v>
       </c>
     </row>
@@ -3319,7 +3374,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Changes and updates of specially code types, see the yellow marks, Ver. 1.19.2
Changes and updates of specially code types, see the yellow marks, Ver. 1.19.2
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406EE25A-479C-4DCC-B38F-6761E18AFDD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D0DBAB-75EB-4AAE-AAD8-95DCF9ED1CA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="364">
   <si>
     <t>Type</t>
   </si>
@@ -630,9 +630,6 @@
     <t>RS_CatchCategory</t>
   </si>
   <si>
-    <t>RS_CommercialSizeCategoryScale</t>
-  </si>
-  <si>
     <t xml:space="preserve">RS_CommercialSizeCategory     </t>
   </si>
   <si>
@@ -845,9 +842,6 @@
     <t>Official number of hauls or settings of gear. It is fine to include partial data.</t>
   </si>
   <si>
-    <t>RS_incidentialByCatchMitigateD</t>
-  </si>
-  <si>
     <t>Sampling scheme</t>
   </si>
   <si>
@@ -1036,9 +1030,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Value RSE </t>
-  </si>
-  <si>
-    <t>Ver 18.1.4</t>
   </si>
   <si>
     <t>CEsamplingScheme</t>
@@ -1190,9 +1181,6 @@
     <t>CLregDisCat</t>
   </si>
   <si>
-    <t>RS_regDisCategory</t>
-  </si>
-  <si>
     <t>(New)</t>
   </si>
   <si>
@@ -1200,6 +1188,21 @@
   </si>
   <si>
     <t xml:space="preserve">When 'RegDis' have been selected in the CLcatchCategory, Logbook registered discard category can be specified </t>
+  </si>
+  <si>
+    <t>regDisCategory</t>
+  </si>
+  <si>
+    <t>CommercialSizeCategoryScale</t>
+  </si>
+  <si>
+    <t>ByCatchMitigateDev</t>
+  </si>
+  <si>
+    <t>RS_QualitativeBias</t>
+  </si>
+  <si>
+    <t>Ver 1.19.2</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1269,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1282,6 +1285,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1313,7 +1322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1357,6 +1366,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1643,9 +1655,9 @@
   </sheetPr>
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -1657,7 +1669,7 @@
     <col min="5" max="5" width="11.86328125" style="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1"/>
     <col min="8" max="8" width="12.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.73046875" style="1" customWidth="1"/>
     <col min="10" max="10" width="41.73046875" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.86328125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
@@ -1671,7 +1683,7 @@
         <v>35</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>39</v>
@@ -1730,10 +1742,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -1775,10 +1787,10 @@
         <v>6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -1807,10 +1819,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -1821,13 +1833,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -1839,10 +1851,10 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
@@ -1906,7 +1918,7 @@
         <v>189</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -1938,7 +1950,7 @@
         <v>189</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
@@ -1970,7 +1982,7 @@
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
@@ -2098,7 +2110,7 @@
         <v>192</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2130,7 +2142,7 @@
         <v>193</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2141,13 +2153,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>295</v>
-      </c>
       <c r="E16" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2159,10 +2171,10 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -2173,13 +2185,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -2191,10 +2203,10 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -2290,7 +2302,7 @@
         <v>196</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2322,24 +2334,24 @@
         <v>197</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -2350,11 +2362,11 @@
       <c r="H22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="18" t="s">
         <v>359</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2382,8 +2394,8 @@
       <c r="H23" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="7" t="s">
-        <v>198</v>
+      <c r="I23" s="18" t="s">
+        <v>360</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>75</v>
@@ -2400,7 +2412,7 @@
         <v>25</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>119</v>
@@ -2415,7 +2427,7 @@
         <v>6</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>76</v>
@@ -2429,13 +2441,13 @@
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>221</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>222</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>4</v>
@@ -2447,10 +2459,10 @@
         <v>6</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2461,7 +2473,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>120</v>
@@ -2479,10 +2491,10 @@
         <v>6</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2493,13 +2505,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>4</v>
@@ -2510,11 +2522,11 @@
       <c r="H27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="7" t="s">
-        <v>268</v>
+      <c r="I27" s="18" t="s">
+        <v>361</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2543,7 +2555,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>121</v>
@@ -2575,10 +2587,10 @@
         <v>6</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2589,13 +2601,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>235</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -2607,10 +2619,10 @@
         <v>6</v>
       </c>
       <c r="I30" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="J30" s="13" t="s">
         <v>236</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2621,13 +2633,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>239</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>240</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>4</v>
@@ -2639,10 +2651,10 @@
         <v>6</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2701,7 +2713,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="8">
         <v>32</v>
@@ -2725,7 +2737,7 @@
         <v>6</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J34" s="7" t="s">
         <v>80</v>
@@ -2737,13 +2749,13 @@
         <v>33</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>14</v>
@@ -2756,7 +2768,7 @@
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -2793,13 +2805,13 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>14</v>
@@ -2808,11 +2820,11 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2821,7 +2833,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>135</v>
@@ -2836,11 +2848,11 @@
         <v>17</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2849,13 +2861,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>4</v>
@@ -2866,14 +2878,16 @@
       <c r="H39" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="7"/>
+      <c r="I39" s="18" t="s">
+        <v>362</v>
+      </c>
       <c r="J39" s="13" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>328</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -2890,15 +2904,16 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="4" max="4" width="15.73046875" customWidth="1"/>
     <col min="5" max="5" width="15.265625" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
     <col min="10" max="10" width="36.86328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2913,7 +2928,7 @@
         <v>36</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>38</v>
@@ -2928,7 +2943,7 @@
         <v>43</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>37</v>
@@ -2971,10 +2986,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -3016,10 +3031,10 @@
         <v>45</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.45">
@@ -3048,10 +3063,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.45">
@@ -3062,13 +3077,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3080,10 +3095,10 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
@@ -3115,7 +3130,7 @@
         <v>189</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
@@ -3275,7 +3290,7 @@
         <v>192</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -3307,7 +3322,7 @@
         <v>193</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -3318,13 +3333,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -3336,10 +3351,10 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
@@ -3350,13 +3365,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>275</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>277</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -3368,10 +3383,10 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
@@ -3382,13 +3397,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -3400,10 +3415,10 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="34.9" x14ac:dyDescent="0.35">
@@ -3414,13 +3429,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -3432,13 +3447,13 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="46.5" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>88</v>
       </c>
@@ -3446,28 +3461,28 @@
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E18" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>265</v>
-      </c>
       <c r="J18" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
@@ -3496,7 +3511,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>121</v>
@@ -3528,13 +3543,13 @@
         <v>6</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="24" x14ac:dyDescent="0.45">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>88</v>
       </c>
@@ -3542,13 +3557,13 @@
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -3560,10 +3575,10 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="J21" s="13" t="s">
         <v>236</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.45">
@@ -3574,13 +3589,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -3592,10 +3607,10 @@
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="117" x14ac:dyDescent="0.45">
@@ -3623,7 +3638,7 @@
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="82.15" x14ac:dyDescent="0.45">
@@ -3641,7 +3656,7 @@
         <v>162</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>5</v>
@@ -3651,7 +3666,7 @@
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="10" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3679,7 +3694,7 @@
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K25" s="6"/>
     </row>
@@ -3708,7 +3723,7 @@
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="24" x14ac:dyDescent="0.45">
@@ -3736,7 +3751,7 @@
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
@@ -3764,7 +3779,7 @@
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="10" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
@@ -3773,13 +3788,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>14</v>
@@ -3792,7 +3807,7 @@
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
@@ -3801,13 +3816,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>245</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>246</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>14</v>
@@ -3820,7 +3835,7 @@
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3829,13 +3844,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>261</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>262</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>49</v>
@@ -3848,7 +3863,7 @@
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3857,13 +3872,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>249</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>250</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>49</v>
@@ -3876,7 +3891,7 @@
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -3885,13 +3900,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>49</v>
@@ -3904,7 +3919,7 @@
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -3913,13 +3928,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>252</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>253</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>49</v>
@@ -3932,7 +3947,7 @@
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -3956,11 +3971,11 @@
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -3984,11 +3999,11 @@
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4012,11 +4027,11 @@
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -4040,11 +4055,11 @@
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -4053,13 +4068,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>14</v>
@@ -4068,11 +4083,11 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4081,13 +4096,13 @@
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>256</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>257</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -4096,11 +4111,11 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4124,11 +4139,11 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4152,11 +4167,11 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4180,11 +4195,11 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
@@ -4212,7 +4227,7 @@
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -4221,13 +4236,13 @@
         <v>43</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4236,11 +4251,11 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -4249,13 +4264,13 @@
         <v>44</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>
@@ -4267,10 +4282,10 @@
         <v>6</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ver 1.19.3 Changes and updates of specially code types, see the yellow marks
Changes and updates of code types, see the yellow marks, latest RS_deepSeaRegulation have been replaced by YesNoFields.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D0DBAB-75EB-4AAE-AAD8-95DCF9ED1CA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0263D1D0-8DAC-4335-9E1A-BB728922054D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -695,9 +695,6 @@
     <t>CLcommercialSizeCategory</t>
   </si>
   <si>
-    <t>RS_qualitativeBias</t>
-  </si>
-  <si>
     <t>National fishing activity</t>
   </si>
   <si>
@@ -722,9 +719,6 @@
     <t>RS_DataTypeOfScientificWE</t>
   </si>
   <si>
-    <t>RS_dataSourceOfScientificWE</t>
-  </si>
-  <si>
     <t>RS_DataTypeForScientificWE</t>
   </si>
   <si>
@@ -759,9 +753,6 @@
   </si>
   <si>
     <t>CLdeepSeaReg</t>
-  </si>
-  <si>
-    <t>RS_deepSeaRegulation</t>
   </si>
   <si>
     <t>Scientific number of hauls/sets</t>
@@ -1190,19 +1181,28 @@
     <t xml:space="preserve">When 'RegDis' have been selected in the CLcatchCategory, Logbook registered discard category can be specified </t>
   </si>
   <si>
-    <t>regDisCategory</t>
-  </si>
-  <si>
     <t>CommercialSizeCategoryScale</t>
   </si>
   <si>
-    <t>ByCatchMitigateDev</t>
-  </si>
-  <si>
     <t>RS_QualitativeBias</t>
   </si>
   <si>
-    <t>Ver 1.19.2</t>
+    <t>YesNoFields</t>
+  </si>
+  <si>
+    <t>RegDisCategory</t>
+  </si>
+  <si>
+    <t>RS_DataSourceOfScientificWE</t>
+  </si>
+  <si>
+    <t>BycatchMitigateDevice</t>
+  </si>
+  <si>
+    <t>RS_NationalFishingActivity</t>
+  </si>
+  <si>
+    <t>Ver 1.19.3</t>
   </si>
 </sst>
 </file>
@@ -1322,7 +1322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1370,6 +1370,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1657,7 +1658,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -1669,7 +1670,7 @@
     <col min="5" max="5" width="11.86328125" style="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1"/>
     <col min="8" max="8" width="12.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.73046875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="41.73046875" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.86328125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
@@ -1683,7 +1684,7 @@
         <v>35</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>39</v>
@@ -1742,10 +1743,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -1787,10 +1788,10 @@
         <v>6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -1819,10 +1820,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>227</v>
+        <v>360</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -1833,13 +1834,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -1851,10 +1852,10 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
@@ -1918,7 +1919,7 @@
         <v>189</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -1950,7 +1951,7 @@
         <v>189</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
@@ -1982,7 +1983,7 @@
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
@@ -2110,7 +2111,7 @@
         <v>192</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2142,7 +2143,7 @@
         <v>193</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2153,13 +2154,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2171,10 +2172,10 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -2185,28 +2186,28 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>276</v>
-      </c>
       <c r="J17" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -2302,7 +2303,7 @@
         <v>196</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2334,24 +2335,24 @@
         <v>197</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -2366,7 +2367,7 @@
         <v>359</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2395,7 +2396,7 @@
         <v>6</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>75</v>
@@ -2441,13 +2442,13 @@
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>221</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>4</v>
@@ -2459,10 +2460,10 @@
         <v>6</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2473,7 +2474,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>120</v>
@@ -2491,7 +2492,7 @@
         <v>6</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J26" s="7" t="s">
         <v>202</v>
@@ -2505,13 +2506,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>4</v>
@@ -2526,7 +2527,7 @@
         <v>361</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2555,7 +2556,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>121</v>
@@ -2601,13 +2602,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>233</v>
-      </c>
       <c r="E30" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -2619,10 +2620,10 @@
         <v>6</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2633,13 +2634,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>4</v>
@@ -2650,11 +2651,11 @@
       <c r="H31" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I31" s="15" t="s">
-        <v>240</v>
+      <c r="I31" s="19" t="s">
+        <v>358</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2749,13 +2750,13 @@
         <v>33</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>14</v>
@@ -2768,7 +2769,7 @@
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -2805,13 +2806,13 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>14</v>
@@ -2820,11 +2821,11 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2833,7 +2834,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>135</v>
@@ -2848,11 +2849,11 @@
         <v>17</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2861,13 +2862,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>4</v>
@@ -2879,10 +2880,10 @@
         <v>6</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
@@ -2904,9 +2905,9 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2928,7 +2929,7 @@
         <v>36</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>38</v>
@@ -2986,10 +2987,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -3031,10 +3032,10 @@
         <v>45</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.45">
@@ -3063,10 +3064,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.45">
@@ -3077,13 +3078,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3095,10 +3096,10 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
@@ -3130,7 +3131,7 @@
         <v>189</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
@@ -3290,7 +3291,7 @@
         <v>192</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -3322,7 +3323,7 @@
         <v>193</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -3333,13 +3334,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -3351,10 +3352,10 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
@@ -3365,13 +3366,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -3383,10 +3384,10 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
@@ -3397,13 +3398,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -3415,10 +3416,10 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>222</v>
+        <v>362</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="34.9" x14ac:dyDescent="0.35">
@@ -3429,13 +3430,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -3447,7 +3448,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>202</v>
@@ -3461,13 +3462,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>4</v>
@@ -3479,10 +3480,10 @@
         <v>6</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
@@ -3557,13 +3558,13 @@
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -3575,13 +3576,13 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.45">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>88</v>
       </c>
@@ -3589,13 +3590,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -3606,11 +3607,11 @@
       <c r="H22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>240</v>
+      <c r="I22" s="18" t="s">
+        <v>358</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="117" x14ac:dyDescent="0.45">
@@ -3656,7 +3657,7 @@
         <v>162</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>5</v>
@@ -3666,7 +3667,7 @@
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="10" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3751,7 +3752,7 @@
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="10" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
@@ -3779,7 +3780,7 @@
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="10" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
@@ -3788,13 +3789,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>14</v>
@@ -3807,7 +3808,7 @@
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
@@ -3816,13 +3817,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>244</v>
-      </c>
       <c r="E30" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>14</v>
@@ -3835,7 +3836,7 @@
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3844,13 +3845,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>49</v>
@@ -3863,7 +3864,7 @@
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="10" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3872,13 +3873,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>49</v>
@@ -3891,7 +3892,7 @@
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="10" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -3900,13 +3901,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>49</v>
@@ -3919,7 +3920,7 @@
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="10" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -3928,13 +3929,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>49</v>
@@ -3947,7 +3948,7 @@
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="10" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -3971,7 +3972,7 @@
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
@@ -3999,7 +4000,7 @@
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="10" t="s">
@@ -4027,7 +4028,7 @@
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
@@ -4055,7 +4056,7 @@
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="10" t="s">
@@ -4068,13 +4069,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>14</v>
@@ -4083,11 +4084,11 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="10" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4096,13 +4097,13 @@
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -4111,11 +4112,11 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4139,7 +4140,7 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="s">
@@ -4167,7 +4168,7 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
@@ -4195,7 +4196,7 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
@@ -4236,13 +4237,13 @@
         <v>43</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4251,11 +4252,11 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -4264,13 +4265,13 @@
         <v>44</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>
@@ -4282,7 +4283,7 @@
         <v>6</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>218</v>
+        <v>357</v>
       </c>
       <c r="J46" s="10" t="s">
         <v>215</v>

</xml_diff>

<commit_message>
Ver. 1.19.4. Correting typos for CE Vocabulary code types
Ver. 1.19.4. Correting typos for CE Vocabulary code types for: RS_DataTypeOfScientificWE, RS_DataSourceOfScientificWE, BycatchMitigateDevice, Harbour_LOCODE and headers Field Name Description and Field Name.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0263D1D0-8DAC-4335-9E1A-BB728922054D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60182542-F5F8-403E-A0E5-A22FB5A8DE43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Commercial Landing CL" sheetId="3" r:id="rId1"/>
     <sheet name="Commercial Effort CE" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="361">
   <si>
     <t>Type</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>Order</t>
-  </si>
-  <si>
-    <t>Short Description</t>
   </si>
   <si>
     <t>Description</t>
@@ -689,9 +686,6 @@
     <t>For estimated data: A semi‐quantitative scale ranging from +++ (large overestimate) to −−− (large underestimate) can be used as in Hyder et al 2017.</t>
   </si>
   <si>
-    <t>LOCODE_Harbour</t>
-  </si>
-  <si>
     <t>CLcommercialSizeCategory</t>
   </si>
   <si>
@@ -719,12 +713,6 @@
     <t>RS_DataTypeOfScientificWE</t>
   </si>
   <si>
-    <t>RS_DataTypeForScientificWE</t>
-  </si>
-  <si>
-    <t>RS_DataSourceForScientificWE</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Metier 6 fishing activity</t>
   </si>
   <si>
@@ -822,9 +810,6 @@
   </si>
   <si>
     <t>CEIBmitiDev</t>
-  </si>
-  <si>
-    <t>RS_incidentialByCatchMitigationDevice</t>
   </si>
   <si>
     <t>Official vessel kW*Fishing hours.  It is fine to include partial data.</t>
@@ -1202,7 +1187,13 @@
     <t>RS_NationalFishingActivity</t>
   </si>
   <si>
-    <t>Ver 1.19.3</t>
+    <t>BycatchMitigationDevice</t>
+  </si>
+  <si>
+    <t>Field name Description</t>
+  </si>
+  <si>
+    <t>Ver 1.19.4</t>
   </si>
 </sst>
 </file>
@@ -1322,7 +1313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1371,6 +1362,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1678,19 +1672,19 @@
   <sheetData>
     <row r="1" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>0</v>
@@ -1702,27 +1696,27 @@
         <v>2</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -1731,7 +1725,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
@@ -1743,10 +1737,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -1764,7 +1758,7 @@
     </row>
     <row r="4" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
@@ -1773,10 +1767,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>4</v>
@@ -1788,15 +1782,15 @@
         <v>6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
@@ -1805,10 +1799,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>4</v>
@@ -1820,27 +1814,27 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -1852,15 +1846,15 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="8">
         <v>5</v>
@@ -1869,10 +1863,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>4</v>
@@ -1884,15 +1878,15 @@
         <v>6</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="8">
         <v>6</v>
@@ -1901,10 +1895,10 @@
         <v>11</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>4</v>
@@ -1916,15 +1910,15 @@
         <v>6</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -1933,10 +1927,10 @@
         <v>12</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>4</v>
@@ -1948,15 +1942,15 @@
         <v>6</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="8">
         <v>8</v>
@@ -1965,10 +1959,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>14</v>
@@ -1983,12 +1977,12 @@
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="8">
         <v>9</v>
@@ -1997,10 +1991,10 @@
         <v>15</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>14</v>
@@ -2015,12 +2009,12 @@
         <v>15</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="8">
         <v>10</v>
@@ -2029,10 +2023,10 @@
         <v>16</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>14</v>
@@ -2047,12 +2041,12 @@
         <v>16</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="8">
         <v>11</v>
@@ -2061,10 +2055,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>4</v>
@@ -2076,15 +2070,15 @@
         <v>6</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="8">
         <v>12</v>
@@ -2093,10 +2087,10 @@
         <v>19</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -2108,15 +2102,15 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="8">
         <v>13</v>
@@ -2125,10 +2119,10 @@
         <v>20</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>21</v>
@@ -2140,27 +2134,27 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="8">
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2172,27 +2166,27 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="8">
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>275</v>
-      </c>
       <c r="E17" s="8" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -2204,27 +2198,27 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="8">
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>14</v>
@@ -2236,15 +2230,15 @@
         <v>6</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="8">
         <v>17</v>
@@ -2253,10 +2247,10 @@
         <v>22</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>4</v>
@@ -2268,15 +2262,15 @@
         <v>6</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="8">
         <v>18</v>
@@ -2285,10 +2279,10 @@
         <v>23</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>4</v>
@@ -2300,15 +2294,15 @@
         <v>6</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="8">
         <v>19</v>
@@ -2317,11 +2311,11 @@
         <v>24</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>114</v>
-      </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
       </c>
@@ -2332,27 +2326,27 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -2364,27 +2358,27 @@
         <v>6</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="8">
         <v>21</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>4</v>
@@ -2396,15 +2390,15 @@
         <v>6</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="8">
         <v>22</v>
@@ -2413,10 +2407,10 @@
         <v>25</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>4</v>
@@ -2428,27 +2422,27 @@
         <v>6</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" s="8">
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>4</v>
@@ -2460,27 +2454,27 @@
         <v>6</v>
       </c>
       <c r="I25" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="J25" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" s="8">
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>4</v>
@@ -2492,27 +2486,27 @@
         <v>6</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" s="8">
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>4</v>
@@ -2524,27 +2518,27 @@
         <v>6</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28" s="8">
         <v>26</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>124</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>4</v>
@@ -2556,15 +2550,15 @@
         <v>6</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="8">
         <v>27</v>
@@ -2573,11 +2567,11 @@
         <v>27</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>126</v>
-      </c>
       <c r="F29" s="8" t="s">
         <v>4</v>
       </c>
@@ -2588,27 +2582,27 @@
         <v>6</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" s="8">
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -2620,27 +2614,27 @@
         <v>6</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" s="8">
         <v>29</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>4</v>
@@ -2652,10 +2646,10 @@
         <v>6</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2667,10 +2661,10 @@
         <v>28</v>
       </c>
       <c r="D32" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>14</v>
@@ -2683,7 +2677,7 @@
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2695,10 +2689,10 @@
         <v>30</v>
       </c>
       <c r="D33" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>130</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>14</v>
@@ -2711,7 +2705,7 @@
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2723,11 +2717,11 @@
         <v>31</v>
       </c>
       <c r="D34" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>132</v>
-      </c>
       <c r="F34" s="8" t="s">
         <v>4</v>
       </c>
@@ -2738,10 +2732,10 @@
         <v>6</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
@@ -2750,13 +2744,13 @@
         <v>33</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>14</v>
@@ -2769,7 +2763,7 @@
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -2781,10 +2775,10 @@
         <v>33</v>
       </c>
       <c r="D36" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>133</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>14</v>
@@ -2797,7 +2791,7 @@
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2806,13 +2800,13 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>14</v>
@@ -2821,11 +2815,11 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2834,13 +2828,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D38" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>14</v>
@@ -2849,11 +2843,11 @@
         <v>17</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2862,13 +2856,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>4</v>
@@ -2880,15 +2874,15 @@
         <v>6</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -2904,10 +2898,10 @@
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2920,51 +2914,51 @@
   <sheetData>
     <row r="1" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -2973,12 +2967,12 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -2987,10 +2981,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -3003,57 +2997,57 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>226</v>
+      <c r="I4" s="20" t="s">
+        <v>223</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>144</v>
-      </c>
       <c r="F5" s="8" t="s">
         <v>4</v>
       </c>
@@ -3063,28 +3057,28 @@
       <c r="H5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>227</v>
+      <c r="I5" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3096,15 +3090,15 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="8">
         <v>5</v>
@@ -3113,10 +3107,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>4</v>
@@ -3128,15 +3122,15 @@
         <v>6</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="8">
         <v>6</v>
@@ -3145,10 +3139,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>14</v>
@@ -3163,12 +3157,12 @@
         <v>13</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -3177,10 +3171,10 @@
         <v>15</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>14</v>
@@ -3195,12 +3189,12 @@
         <v>15</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="8">
         <v>8</v>
@@ -3209,10 +3203,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>14</v>
@@ -3227,12 +3221,12 @@
         <v>16</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="69.75" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="8">
         <v>9</v>
@@ -3241,10 +3235,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>4</v>
@@ -3256,15 +3250,15 @@
         <v>6</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="8">
         <v>10</v>
@@ -3273,11 +3267,11 @@
         <v>19</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="F12" s="8" t="s">
         <v>4</v>
       </c>
@@ -3288,15 +3282,15 @@
         <v>6</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="8">
         <v>11</v>
@@ -3305,10 +3299,10 @@
         <v>20</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>21</v>
@@ -3320,27 +3314,27 @@
         <v>6</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="8">
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>293</v>
-      </c>
       <c r="E14" s="8" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -3352,27 +3346,27 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="8">
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -3384,27 +3378,27 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="8">
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -3416,27 +3410,27 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="8">
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -3448,27 +3442,27 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="46.5" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="8">
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>4</v>
@@ -3479,29 +3473,29 @@
       <c r="H18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>261</v>
+      <c r="I18" s="18" t="s">
+        <v>358</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="8">
         <v>17</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>157</v>
-      </c>
       <c r="F19" s="8" t="s">
         <v>4</v>
       </c>
@@ -3511,28 +3505,28 @@
       <c r="H19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>216</v>
+      <c r="I19" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="8">
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>4</v>
@@ -3544,27 +3538,27 @@
         <v>6</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="8">
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -3576,27 +3570,27 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -3608,10 +3602,10 @@
         <v>6</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="117" x14ac:dyDescent="0.45">
@@ -3620,26 +3614,26 @@
         <v>21</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="F23" s="8" t="s">
+      <c r="G23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="82.15" x14ac:dyDescent="0.45">
@@ -3648,26 +3642,26 @@
         <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="10" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3676,26 +3670,26 @@
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K25" s="6"/>
     </row>
@@ -3705,26 +3699,26 @@
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="F26" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="24" x14ac:dyDescent="0.45">
@@ -3733,26 +3727,26 @@
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="10" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
@@ -3761,26 +3755,26 @@
         <v>26</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>169</v>
-      </c>
       <c r="F28" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="10" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
@@ -3789,13 +3783,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>14</v>
@@ -3804,11 +3798,11 @@
         <v>17</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="10" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
@@ -3817,13 +3811,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>242</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>14</v>
@@ -3832,11 +3826,11 @@
         <v>17</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3845,26 +3839,26 @@
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="10" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3873,26 +3867,26 @@
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="10" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -3901,26 +3895,26 @@
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="10" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -3929,26 +3923,26 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="10" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -3957,26 +3951,26 @@
         <v>33</v>
       </c>
       <c r="C35" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="G35" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -3985,26 +3979,26 @@
         <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>175</v>
-      </c>
       <c r="F36" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4013,26 +4007,26 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -4041,26 +4035,26 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D38" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="E38" s="8" t="s">
-        <v>178</v>
-      </c>
       <c r="F38" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -4069,13 +4063,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>14</v>
@@ -4084,11 +4078,11 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="10" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4097,13 +4091,13 @@
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -4112,11 +4106,11 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4125,13 +4119,13 @@
         <v>39</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>14</v>
@@ -4140,11 +4134,11 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4153,13 +4147,13 @@
         <v>40</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>14</v>
@@ -4168,11 +4162,11 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4181,13 +4175,13 @@
         <v>41</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>14</v>
@@ -4196,11 +4190,11 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
@@ -4212,10 +4206,10 @@
         <v>33</v>
       </c>
       <c r="D44" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>185</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>186</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>14</v>
@@ -4228,7 +4222,7 @@
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -4237,13 +4231,13 @@
         <v>43</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4252,11 +4246,11 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="10" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -4265,13 +4259,13 @@
         <v>44</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>
@@ -4283,10 +4277,10 @@
         <v>6</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V.1.19.5 Codes in descriptions and typos corrected
BycatchMitigationDevice update codes in description (to AttAcoustic from pingers, etc.)

CLtotalOfficialLandingsValue description updated with 'CLdataSourceOfScientificValue'

CEdataTypeForScientificEffort, CEdataSourceForScientificEffort, 
CEincidentalByCatchMitigationDevice and CElandingLocationvocabulary code type typo corrected.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60182542-F5F8-403E-A0E5-A22FB5A8DE43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA47BD8-0898-4C9B-BF0A-0929C33E0C40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9360" windowHeight="5205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial Landing CL" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="360">
   <si>
     <t>Type</t>
   </si>
@@ -238,12 +238,6 @@
 “Other”: if value of landings are estimated from other sources</t>
   </si>
   <si>
-    <t>1-4.</t>
-  </si>
-  <si>
-    <t>1-12.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Most detailed FAO area (http://www.fao.org/fishery/area/search/en). 
 E.g. ICES division 27.4.c, subdivisions in the Baltic Sea (e.g. 27.3.d.25). 
 Division in Mediterranean and Black Seas (e.g. 37.1.1) and NAFO (e.g. 21.1A). 
@@ -592,9 +586,6 @@
     <t>CEnumUniqVes</t>
   </si>
   <si>
-    <t>Year 1900 to 2050</t>
-  </si>
-  <si>
     <t>Most detailed FAO area (http://www.fao.org/fishery/area/search/en). 
 E.g. ICES division 27.4.c, subdivisions in the Baltic Sea (e.g. 27.3.d.25). 
 Division in Mediterranean and Black Seas (e.g. 37.1.1) and NAFO (e.g. 21.1A).</t>
@@ -832,9 +823,6 @@
     <t xml:space="preserve">The intended usage at the time of landing. Codes: “Ind” = industry or “HuC” = human consumption or “None” for logbook registered discards. </t>
   </si>
   <si>
-    <t>Sales value in Euro of the field official weight 'CLofficialWeight'. If nessesary the estimated value can be reported. Please report the data source in the field 'CLdataSourceOfScientificWeight'. If logbook registered discards, put NA. Exchange rate by month can be found here: http://appsso.eurostat.ec.europa.eu/nui/show.do?dataset=ei_mfrt_m&amp;lang=en</t>
-  </si>
-  <si>
     <t>Int</t>
   </si>
   <si>
@@ -860,16 +848,7 @@
     <t>CLeconZoneIndi</t>
   </si>
   <si>
-    <t>1900 - 2050.</t>
-  </si>
-  <si>
     <t>Incidential by catch mitigation device</t>
-  </si>
-  <si>
-    <t>Incidential by catch mitigation devices: Sorting grid, functional pingers, seal excluder device and turtle excluder device, unknown, None.</t>
-  </si>
-  <si>
-    <t>GSA subarea, mandatory for FAO area 37 (Mediterranean and Black Sea). (Use 'NA' if not fishing in the area)</t>
   </si>
   <si>
     <t>0-999</t>
@@ -1157,9 +1136,6 @@
     <t>CLregDisCat</t>
   </si>
   <si>
-    <t>(New)</t>
-  </si>
-  <si>
     <t>Logbook registered discard category</t>
   </si>
   <si>
@@ -1181,9 +1157,6 @@
     <t>RS_DataSourceOfScientificWE</t>
   </si>
   <si>
-    <t>BycatchMitigateDevice</t>
-  </si>
-  <si>
     <t>RS_NationalFishingActivity</t>
   </si>
   <si>
@@ -1193,7 +1166,31 @@
     <t>Field name Description</t>
   </si>
   <si>
-    <t>Ver 1.19.4</t>
+    <t>1-12. The month is determined by the landing date.</t>
+  </si>
+  <si>
+    <t>1-4.The quarter is determined by the landing date.</t>
+  </si>
+  <si>
+    <t>1-4. The quarter is determined by the landing date.</t>
+  </si>
+  <si>
+    <t>1900 - 2050. The year is determined by the landing date.</t>
+  </si>
+  <si>
+    <t>Year 1900 to 2050. The year is determined by the landing date.</t>
+  </si>
+  <si>
+    <t>GSA subarea, mandatory for FAO area 37 (Mediterranean and Black Sea). (Use 'NotApplicable' if not fishing in the area)</t>
+  </si>
+  <si>
+    <t>Sales value in Euro of the field official weight 'CLofficialWeight'. If nessesary the estimated value can be reported. Please report the data source in the field 'CLdataSourceOfScientificValue'. If logbook registered discards, put NA. Exchange rate by month can be found here: http://appsso.eurostat.ec.europa.eu/nui/show.do?dataset=ei_mfrt_m&amp;lang=en</t>
+  </si>
+  <si>
+    <t>Incidential bycatch mitigation devices: AttAcoustic, AttAltProf, AttExclDev, AttLight, unknown, None, etc.</t>
+  </si>
+  <si>
+    <t>Ver 1.19.5</t>
   </si>
 </sst>
 </file>
@@ -1355,15 +1352,15 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1664,7 +1661,7 @@
     <col min="5" max="5" width="11.86328125" style="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1"/>
     <col min="8" max="8" width="12.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.265625" style="1" customWidth="1"/>
     <col min="10" max="10" width="41.73046875" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.86328125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
@@ -1678,7 +1675,7 @@
         <v>35</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>38</v>
@@ -1696,7 +1693,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>36</v>
@@ -1704,19 +1701,19 @@
     </row>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -1725,7 +1722,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
@@ -1737,10 +1734,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -1758,7 +1755,7 @@
     </row>
     <row r="4" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
@@ -1767,10 +1764,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>4</v>
@@ -1782,15 +1779,15 @@
         <v>6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
@@ -1799,11 +1796,11 @@
         <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="F5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1814,27 +1811,27 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -1846,15 +1843,15 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="8">
         <v>5</v>
@@ -1863,10 +1860,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>4</v>
@@ -1878,7 +1875,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>68</v>
@@ -1886,7 +1883,7 @@
     </row>
     <row r="8" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="8">
         <v>6</v>
@@ -1895,10 +1892,10 @@
         <v>11</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>4</v>
@@ -1910,15 +1907,15 @@
         <v>6</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -1927,10 +1924,10 @@
         <v>12</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>4</v>
@@ -1942,15 +1939,15 @@
         <v>6</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B10" s="8">
         <v>8</v>
@@ -1959,10 +1956,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>14</v>
@@ -1977,12 +1974,12 @@
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>272</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" s="8">
         <v>9</v>
@@ -1991,10 +1988,10 @@
         <v>15</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>14</v>
@@ -2009,12 +2006,12 @@
         <v>15</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>69</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B12" s="8">
         <v>10</v>
@@ -2023,10 +2020,10 @@
         <v>16</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>14</v>
@@ -2041,12 +2038,12 @@
         <v>16</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>70</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B13" s="8">
         <v>11</v>
@@ -2055,10 +2052,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>4</v>
@@ -2070,15 +2067,15 @@
         <v>6</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B14" s="8">
         <v>12</v>
@@ -2087,10 +2084,10 @@
         <v>19</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -2102,15 +2099,15 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="8">
         <v>13</v>
@@ -2119,10 +2116,10 @@
         <v>20</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>21</v>
@@ -2134,27 +2131,27 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>275</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B16" s="8">
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -2166,59 +2163,59 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B17" s="8">
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="J17" s="7" t="s">
         <v>265</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B18" s="8">
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>14</v>
@@ -2230,15 +2227,15 @@
         <v>6</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" s="8">
         <v>17</v>
@@ -2247,10 +2244,10 @@
         <v>22</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>4</v>
@@ -2262,15 +2259,15 @@
         <v>6</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B20" s="8">
         <v>18</v>
@@ -2279,10 +2276,10 @@
         <v>23</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>4</v>
@@ -2294,15 +2291,15 @@
         <v>6</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" s="8">
         <v>19</v>
@@ -2311,10 +2308,10 @@
         <v>24</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -2326,59 +2323,59 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A22" s="17" t="s">
-        <v>348</v>
-      </c>
-      <c r="B22" s="8">
+      <c r="A22" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="19">
         <v>20</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="17" t="s">
         <v>346</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>354</v>
-      </c>
       <c r="J22" s="14" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" s="8">
         <v>21</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>117</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>4</v>
@@ -2389,16 +2386,16 @@
       <c r="H23" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="18" t="s">
-        <v>351</v>
+      <c r="I23" s="17" t="s">
+        <v>343</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B24" s="8">
         <v>22</v>
@@ -2407,10 +2404,10 @@
         <v>25</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>4</v>
@@ -2422,27 +2419,27 @@
         <v>6</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B25" s="8">
         <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>4</v>
@@ -2454,27 +2451,27 @@
         <v>6</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B26" s="8">
         <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>4</v>
@@ -2486,27 +2483,27 @@
         <v>6</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B27" s="8">
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>4</v>
@@ -2517,28 +2514,28 @@
       <c r="H27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>274</v>
+      <c r="I27" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B28" s="8">
         <v>26</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>123</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>4</v>
@@ -2550,15 +2547,15 @@
         <v>6</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B29" s="8">
         <v>27</v>
@@ -2567,10 +2564,10 @@
         <v>27</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>4</v>
@@ -2582,27 +2579,27 @@
         <v>6</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B30" s="8">
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>228</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>4</v>
@@ -2614,27 +2611,27 @@
         <v>6</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B31" s="8">
         <v>29</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>4</v>
@@ -2645,11 +2642,11 @@
       <c r="H31" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I31" s="19" t="s">
-        <v>353</v>
+      <c r="I31" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2661,10 +2658,10 @@
         <v>28</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>14</v>
@@ -2677,7 +2674,7 @@
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2689,10 +2686,10 @@
         <v>30</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>14</v>
@@ -2705,7 +2702,7 @@
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2717,10 +2714,10 @@
         <v>31</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>4</v>
@@ -2732,10 +2729,10 @@
         <v>6</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
@@ -2744,13 +2741,13 @@
         <v>33</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>14</v>
@@ -2762,8 +2759,8 @@
         <v>32</v>
       </c>
       <c r="I35" s="7"/>
-      <c r="J35" s="7" t="s">
-        <v>263</v>
+      <c r="J35" s="17" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -2775,10 +2772,10 @@
         <v>33</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>14</v>
@@ -2791,7 +2788,7 @@
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2800,13 +2797,13 @@
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>14</v>
@@ -2815,11 +2812,11 @@
         <v>17</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2828,13 +2825,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>14</v>
@@ -2843,11 +2840,11 @@
         <v>17</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
@@ -2856,13 +2853,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>4</v>
@@ -2873,16 +2870,16 @@
       <c r="H39" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="18" t="s">
-        <v>352</v>
+      <c r="I39" s="17" t="s">
+        <v>344</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -2898,17 +2895,17 @@
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="4" max="4" width="15.73046875" customWidth="1"/>
     <col min="5" max="5" width="15.265625" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.265625" customWidth="1"/>
     <col min="10" max="10" width="36.86328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2920,7 +2917,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>38</v>
@@ -2938,7 +2935,7 @@
         <v>42</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>36</v>
@@ -2946,19 +2943,19 @@
     </row>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -2967,12 +2964,12 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -2981,10 +2978,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>4</v>
@@ -2997,12 +2994,12 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
@@ -3011,10 +3008,10 @@
         <v>43</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>4</v>
@@ -3025,16 +3022,16 @@
       <c r="H4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>223</v>
+      <c r="I4" s="19" t="s">
+        <v>220</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
@@ -3043,10 +3040,10 @@
         <v>45</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>4</v>
@@ -3057,28 +3054,28 @@
       <c r="H5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="20" t="s">
-        <v>355</v>
+      <c r="I5" s="19" t="s">
+        <v>347</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>4</v>
@@ -3090,15 +3087,15 @@
         <v>6</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="8">
         <v>5</v>
@@ -3107,11 +3104,11 @@
         <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>148</v>
-      </c>
       <c r="F7" s="8" t="s">
         <v>4</v>
       </c>
@@ -3122,15 +3119,15 @@
         <v>6</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="8">
         <v>6</v>
@@ -3139,10 +3136,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>14</v>
@@ -3157,12 +3154,12 @@
         <v>13</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>186</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -3171,10 +3168,10 @@
         <v>15</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>14</v>
@@ -3189,12 +3186,12 @@
         <v>15</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>69</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B10" s="8">
         <v>8</v>
@@ -3203,10 +3200,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>14</v>
@@ -3221,12 +3218,12 @@
         <v>16</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>70</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="69.75" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" s="8">
         <v>9</v>
@@ -3235,10 +3232,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>4</v>
@@ -3250,15 +3247,15 @@
         <v>6</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B12" s="8">
         <v>10</v>
@@ -3267,10 +3264,10 @@
         <v>19</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>4</v>
@@ -3282,15 +3279,15 @@
         <v>6</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B13" s="8">
         <v>11</v>
@@ -3299,10 +3296,10 @@
         <v>20</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>21</v>
@@ -3314,27 +3311,27 @@
         <v>6</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>275</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B14" s="8">
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>4</v>
@@ -3346,27 +3343,27 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="8">
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>4</v>
@@ -3378,27 +3375,27 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B16" s="8">
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>4</v>
@@ -3410,27 +3407,27 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B17" s="8">
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>4</v>
@@ -3442,27 +3439,27 @@
         <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="46.5" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B18" s="8">
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>4</v>
@@ -3473,28 +3470,28 @@
       <c r="H18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="I18" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="J18" s="17" t="s">
         <v>358</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" s="8">
         <v>17</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>4</v>
@@ -3505,16 +3502,16 @@
       <c r="H19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="18" t="s">
-        <v>222</v>
+      <c r="I19" s="17" t="s">
+        <v>219</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B20" s="8">
         <v>18</v>
@@ -3523,10 +3520,10 @@
         <v>46</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>4</v>
@@ -3538,27 +3535,27 @@
         <v>6</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" s="8">
         <v>19</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>4</v>
@@ -3570,27 +3567,27 @@
         <v>6</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -3601,11 +3598,11 @@
       <c r="H22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="18" t="s">
-        <v>353</v>
+      <c r="I22" s="17" t="s">
+        <v>345</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="117" x14ac:dyDescent="0.45">
@@ -3617,10 +3614,10 @@
         <v>47</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>48</v>
@@ -3633,7 +3630,7 @@
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="82.15" x14ac:dyDescent="0.45">
@@ -3645,13 +3642,13 @@
         <v>50</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>161</v>
-      </c>
       <c r="F24" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>5</v>
@@ -3661,7 +3658,7 @@
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="10" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3673,10 +3670,10 @@
         <v>52</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>48</v>
@@ -3689,7 +3686,7 @@
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K25" s="6"/>
     </row>
@@ -3702,10 +3699,10 @@
         <v>54</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>48</v>
@@ -3718,7 +3715,7 @@
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="24" x14ac:dyDescent="0.45">
@@ -3730,10 +3727,10 @@
         <v>55</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>48</v>
@@ -3746,7 +3743,7 @@
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="10" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
@@ -3758,10 +3755,10 @@
         <v>56</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>48</v>
@@ -3774,7 +3771,7 @@
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="10" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
@@ -3783,13 +3780,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>14</v>
@@ -3802,7 +3799,7 @@
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
@@ -3811,13 +3808,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>237</v>
-      </c>
       <c r="E30" s="8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>14</v>
@@ -3830,7 +3827,7 @@
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3839,13 +3836,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>48</v>
@@ -3858,7 +3855,7 @@
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="10" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
@@ -3867,13 +3864,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>48</v>
@@ -3886,7 +3883,7 @@
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="10" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -3895,13 +3892,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>48</v>
@@ -3914,7 +3911,7 @@
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="10" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -3923,13 +3920,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>48</v>
@@ -3942,7 +3939,7 @@
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="10" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -3954,10 +3951,10 @@
         <v>59</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>60</v>
@@ -3966,11 +3963,11 @@
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -3982,10 +3979,10 @@
         <v>61</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>60</v>
@@ -3994,11 +3991,11 @@
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4010,10 +4007,10 @@
         <v>62</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>60</v>
@@ -4022,11 +4019,11 @@
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -4038,10 +4035,10 @@
         <v>63</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>60</v>
@@ -4050,11 +4047,11 @@
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="24" x14ac:dyDescent="0.45">
@@ -4063,13 +4060,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>14</v>
@@ -4078,11 +4075,11 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4091,13 +4088,13 @@
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -4106,11 +4103,11 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4122,10 +4119,10 @@
         <v>64</v>
       </c>
       <c r="D41" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>14</v>
@@ -4134,11 +4131,11 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4150,10 +4147,10 @@
         <v>65</v>
       </c>
       <c r="D42" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>181</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>14</v>
@@ -4162,11 +4159,11 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
@@ -4178,10 +4175,10 @@
         <v>66</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>14</v>
@@ -4190,11 +4187,11 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
@@ -4206,10 +4203,10 @@
         <v>33</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>14</v>
@@ -4222,7 +4219,7 @@
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -4231,13 +4228,13 @@
         <v>43</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4246,11 +4243,11 @@
         <v>17</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="10" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
@@ -4259,13 +4256,13 @@
         <v>44</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>
@@ -4277,10 +4274,10 @@
         <v>6</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "small format edits"
This reverts commit 997db37ad3ffca74eb87f9863ee0c0b16a4b46c7.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\ICES\ices-tools-dev\RDBES\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA47BD8-0898-4C9B-BF0A-0929C33E0C40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9360" windowHeight="5205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9360" windowHeight="5205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial Landing CL" sheetId="3" r:id="rId1"/>
     <sheet name="Commercial Effort CE" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -999,6 +1000,9 @@
   </si>
   <si>
     <t>CLtotOffLanVal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scientific weight RSE </t>
   </si>
   <si>
     <t>CLscientificWeightRSE</t>
@@ -1188,14 +1192,11 @@
   <si>
     <t>Ver 1.19.5</t>
   </si>
-  <si>
-    <t>Scientific weight RSE</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1640,33 +1641,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.73046875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.73046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.86328125" style="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="41.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="41.73046875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.86328125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>67</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>79</v>
       </c>
@@ -1724,7 +1725,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="8">
         <v>1</v>
@@ -1752,7 +1753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>85</v>
       </c>
@@ -1784,7 +1785,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>85</v>
       </c>
@@ -1810,13 +1811,13 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>85</v>
       </c>
@@ -1845,10 +1846,10 @@
         <v>257</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>85</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>85</v>
       </c>
@@ -1909,10 +1910,10 @@
         <v>185</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>85</v>
       </c>
@@ -1941,10 +1942,10 @@
         <v>185</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>85</v>
       </c>
@@ -1973,10 +1974,10 @@
         <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>85</v>
       </c>
@@ -2005,10 +2006,10 @@
         <v>15</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>85</v>
       </c>
@@ -2037,10 +2038,10 @@
         <v>16</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>85</v>
       </c>
@@ -2072,7 +2073,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>85</v>
       </c>
@@ -2101,10 +2102,10 @@
         <v>188</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>85</v>
       </c>
@@ -2133,10 +2134,10 @@
         <v>189</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>85</v>
       </c>
@@ -2168,7 +2169,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>85</v>
       </c>
@@ -2200,7 +2201,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>85</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>85</v>
       </c>
@@ -2264,7 +2265,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>85</v>
       </c>
@@ -2296,7 +2297,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>85</v>
       </c>
@@ -2328,7 +2329,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
         <v>85</v>
       </c>
@@ -2336,13 +2337,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>340</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>338</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>339</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>4</v>
@@ -2354,13 +2355,13 @@
         <v>6</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>85</v>
       </c>
@@ -2386,13 +2387,13 @@
         <v>6</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>85</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>85</v>
       </c>
@@ -2456,7 +2457,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>85</v>
       </c>
@@ -2488,7 +2489,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>85</v>
       </c>
@@ -2514,13 +2515,13 @@
         <v>6</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>85</v>
       </c>
@@ -2552,7 +2553,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>85</v>
       </c>
@@ -2584,7 +2585,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>85</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>85</v>
       </c>
@@ -2642,13 +2643,13 @@
         <v>6</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
       <c r="B32" s="8">
         <v>30</v>
@@ -2676,7 +2677,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="8">
         <v>31</v>
@@ -2704,7 +2705,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="8">
         <v>32</v>
@@ -2734,7 +2735,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
       <c r="A35" s="7"/>
       <c r="B35" s="8">
         <v>33</v>
@@ -2759,10 +2760,10 @@
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="17" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A36" s="7"/>
       <c r="B36" s="8">
         <v>34</v>
@@ -2790,19 +2791,19 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A37" s="7"/>
       <c r="B37" s="8">
         <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>359</v>
+        <v>316</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>14</v>
@@ -2815,10 +2816,10 @@
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A38" s="7"/>
       <c r="B38" s="8">
         <v>36</v>
@@ -2846,19 +2847,19 @@
         <v>270</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A39" s="7"/>
       <c r="B39" s="8">
         <v>37</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>4</v>
@@ -2870,15 +2871,15 @@
         <v>6</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="J39" s="13" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -2888,7 +2889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -2900,15 +2901,15 @@
       <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" customWidth="1"/>
+    <col min="5" max="5" width="15.265625" customWidth="1"/>
+    <col min="9" max="9" width="15.265625" customWidth="1"/>
+    <col min="10" max="10" width="36.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>67</v>
       </c>
@@ -2916,7 +2917,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>38</v>
@@ -2940,7 +2941,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>79</v>
       </c>
@@ -2966,7 +2967,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>85</v>
       </c>
@@ -2996,7 +2997,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>85</v>
       </c>
@@ -3028,7 +3029,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>85</v>
       </c>
@@ -3054,13 +3055,13 @@
         <v>6</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>85</v>
       </c>
@@ -3089,10 +3090,10 @@
         <v>257</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>85</v>
       </c>
@@ -3121,10 +3122,10 @@
         <v>185</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>85</v>
       </c>
@@ -3153,10 +3154,10 @@
         <v>13</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>85</v>
       </c>
@@ -3185,10 +3186,10 @@
         <v>15</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>85</v>
       </c>
@@ -3217,10 +3218,10 @@
         <v>16</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="84" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="69.75" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>85</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>85</v>
       </c>
@@ -3281,10 +3282,10 @@
         <v>188</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>85</v>
       </c>
@@ -3313,10 +3314,10 @@
         <v>189</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
         <v>85</v>
       </c>
@@ -3348,7 +3349,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>85</v>
       </c>
@@ -3380,7 +3381,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>85</v>
       </c>
@@ -3406,13 +3407,13 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" s="1" customFormat="1" ht="34.9" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>85</v>
       </c>
@@ -3444,7 +3445,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="46.5" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>85</v>
       </c>
@@ -3470,13 +3471,13 @@
         <v>6</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>85</v>
       </c>
@@ -3508,7 +3509,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>85</v>
       </c>
@@ -3540,7 +3541,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>85</v>
       </c>
@@ -3572,7 +3573,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>85</v>
       </c>
@@ -3598,13 +3599,13 @@
         <v>6</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="J22" s="13" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="117" x14ac:dyDescent="0.45">
       <c r="A23" s="9"/>
       <c r="B23" s="8">
         <v>21</v>
@@ -3632,7 +3633,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="96.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="82.15" x14ac:dyDescent="0.45">
       <c r="A24" s="9"/>
       <c r="B24" s="8">
         <v>22</v>
@@ -3657,10 +3658,10 @@
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="10" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A25" s="9"/>
       <c r="B25" s="8">
         <v>23</v>
@@ -3689,7 +3690,7 @@
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="24" x14ac:dyDescent="0.45">
       <c r="A26" s="9"/>
       <c r="B26" s="8">
         <v>24</v>
@@ -3717,7 +3718,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="24" x14ac:dyDescent="0.45">
       <c r="A27" s="9"/>
       <c r="B27" s="8">
         <v>25</v>
@@ -3745,7 +3746,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A28" s="9"/>
       <c r="B28" s="8">
         <v>26</v>
@@ -3770,10 +3771,10 @@
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="10" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A29" s="9"/>
       <c r="B29" s="8">
         <v>27</v>
@@ -3801,7 +3802,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A30" s="9"/>
       <c r="B30" s="8">
         <v>28</v>
@@ -3829,7 +3830,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A31" s="9"/>
       <c r="B31" s="8">
         <v>29</v>
@@ -3857,7 +3858,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A32" s="9"/>
       <c r="B32" s="8">
         <v>30</v>
@@ -3885,7 +3886,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A33" s="9"/>
       <c r="B33" s="8">
         <v>31</v>
@@ -3913,7 +3914,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A34" s="9"/>
       <c r="B34" s="8">
         <v>32</v>
@@ -3941,7 +3942,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A35" s="9"/>
       <c r="B35" s="8">
         <v>33</v>
@@ -3962,14 +3963,14 @@
         <v>5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A36" s="9"/>
       <c r="B36" s="8">
         <v>34</v>
@@ -3990,14 +3991,14 @@
         <v>5</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="10" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A37" s="9"/>
       <c r="B37" s="8">
         <v>35</v>
@@ -4018,14 +4019,14 @@
         <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A38" s="9"/>
       <c r="B38" s="8">
         <v>36</v>
@@ -4046,14 +4047,14 @@
         <v>5</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="10" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A39" s="9"/>
       <c r="B39" s="8">
         <v>37</v>
@@ -4074,14 +4075,14 @@
         <v>17</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A40" s="9"/>
       <c r="B40" s="8">
         <v>38</v>
@@ -4102,14 +4103,14 @@
         <v>17</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A41" s="9"/>
       <c r="B41" s="8">
         <v>39</v>
@@ -4130,14 +4131,14 @@
         <v>5</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A42" s="9"/>
       <c r="B42" s="8">
         <v>40</v>
@@ -4158,14 +4159,14 @@
         <v>5</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A43" s="9"/>
       <c r="B43" s="8">
         <v>41</v>
@@ -4186,14 +4187,14 @@
         <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A44" s="9"/>
       <c r="B44" s="8">
         <v>42</v>
@@ -4221,19 +4222,19 @@
         <v>210</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A45" s="9"/>
       <c r="B45" s="8">
         <v>43</v>
       </c>
       <c r="C45" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>336</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>335</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4249,19 +4250,19 @@
         <v>274</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A46" s="9"/>
       <c r="B46" s="8">
         <v>44</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>4</v>
@@ -4273,7 +4274,7 @@
         <v>6</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="J46" s="10" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
Ver 1.19.26 CL, CE FDI fields' code types are updated
MeshSizeRange  to: FDI_MESH_SIZE_RANGE   //vocab.ices.dk/?ref=1748
SupraRegion  to: FDI_SUPRA_REGION      //vocab.ices.dk/?ref=1749
GeographicalIndicator  to: FDI_GEO_INDICATOR     //vocab.ices.dk/?ref=1750
SpecificConditionsTechnical  to: FDI_SPECON_TECH     //vocab.ices.dk/?ref=1751
FDIconfidentialityCode  to: FDI_CONFIDENTIALITY //vocab.ices.dk/?ref=1752
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCA08F6-61B4-42AA-83DC-96C4E25AF445}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9019F43A-AFC0-4C28-8F5A-25AA14D578B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10185" windowHeight="4815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1560,9 +1560,6 @@
     <t>CLmesSizRan</t>
   </si>
   <si>
-    <t>MeshSizeRange</t>
-  </si>
-  <si>
     <t>Mesh size range</t>
   </si>
   <si>
@@ -1584,9 +1581,6 @@
     <t>Supra Region</t>
   </si>
   <si>
-    <t>SupraRegion</t>
-  </si>
-  <si>
     <t xml:space="preserve">Supra Region. E.g. 'NAO' for Baltic Sea, North Sea, Eastern Arctic, North of Azores, East Greenland, NAFO, Extended North-Western waters (ICES areas V, VI and VII), Southern Western waters, CECAF areas around Madera and the Canary Islands14 (FAO areas 34.1.1, 34.1.2, 34.2.0). </t>
   </si>
   <si>
@@ -1608,9 +1602,6 @@
     <t>CLspecificConditionsTechnical</t>
   </si>
   <si>
-    <t>SpecificConditionsTechnical</t>
-  </si>
-  <si>
     <t>CEspecificConditionsTechnical</t>
   </si>
   <si>
@@ -1626,9 +1617,6 @@
     <t>Geographical indicator</t>
   </si>
   <si>
-    <t>GeographicalIndicator</t>
-  </si>
-  <si>
     <t>Geographical indicator code to distinguish fishing fleets operating in outermost regions and fleets operating exclusively in non-EU waters (international waters and third countries including those with fishing partner agreements). E.g. 'NGI' for No geographical indicator - EU waters, i.e. EEZ of any EU member state, 'NEU' for Non EU waters - More than 50% of activity occurs in non-EU waters.</t>
   </si>
   <si>
@@ -1645,9 +1633,6 @@
   </si>
   <si>
     <t>FDI confidentiality code</t>
-  </si>
-  <si>
-    <t>FDIconfidentialityCode</t>
   </si>
   <si>
     <t xml:space="preserve">Supra Region. E.g. 'NAO' for Baltic Sea, North Sea, Eastern Arctic, North of Azores, East Greenland, NAFO, Extended North-Western waters (ICES areas V, VI and VII), Southern Western waters, CECAF areas around Madera and the Canary Islands14 (FAO areas 34.1.1, 34.1.2, 34.2.0). For EU FDI data.  </t>
@@ -1856,9 +1841,6 @@
     </r>
   </si>
   <si>
-    <t>Ver 1.19.25</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Explaining the differences between official weight and scientific weight. Can be e.g. </t>
     </r>
@@ -2034,6 +2016,29 @@
       </rPr>
       <t>Trips</t>
     </r>
+  </si>
+  <si>
+    <t>FDI_SUPRA_REGION
+//vocab.ices.dk/?ref=1749</t>
+  </si>
+  <si>
+    <t>FDI_MESH_SIZE_RANGE
+//vocab.ices.dk/?ref=1748</t>
+  </si>
+  <si>
+    <t>FDI_GEO_INDICATOR
+//vocab.ices.dk/?ref=1750</t>
+  </si>
+  <si>
+    <t>FDI_SPECON_TECH
+//vocab.ices.dk/?ref=1751</t>
+  </si>
+  <si>
+    <t>FDI_CONFIDENTIALITY
+//vocab.ices.dk/?ref=1752</t>
+  </si>
+  <si>
+    <t>Ver 1.19.26</t>
   </si>
 </sst>
 </file>
@@ -2214,7 +2219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2308,6 +2313,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2596,27 +2604,27 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.73046875" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="25"/>
-    <col min="3" max="3" width="15.73046875" style="25" customWidth="1"/>
-    <col min="4" max="4" width="23.59765625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="13.1328125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="25" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="25" customWidth="1"/>
     <col min="6" max="6" width="9" style="25"/>
-    <col min="7" max="7" width="6.06640625" style="25" customWidth="1"/>
-    <col min="8" max="8" width="12.265625" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.265625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="41.73046875" style="32" customWidth="1"/>
-    <col min="11" max="11" width="36.86328125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="6" style="25" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="41.7109375" style="32" customWidth="1"/>
+    <col min="11" max="11" width="36.85546875" style="25" customWidth="1"/>
     <col min="12" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>63</v>
       </c>
@@ -2649,7 +2657,7 @@
       </c>
       <c r="L1" s="26"/>
     </row>
-    <row r="2" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>73</v>
       </c>
@@ -2676,7 +2684,7 @@
       </c>
       <c r="L2" s="26"/>
     </row>
-    <row r="3" spans="1:12" ht="11.65" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4">
         <v>1</v>
@@ -2705,7 +2713,7 @@
       </c>
       <c r="L3" s="26"/>
     </row>
-    <row r="4" spans="1:12" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>79</v>
       </c>
@@ -2739,7 +2747,7 @@
       <c r="K4" s="21"/>
       <c r="L4" s="26"/>
     </row>
-    <row r="5" spans="1:12" ht="58.15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>79</v>
       </c>
@@ -2773,7 +2781,7 @@
       <c r="K5" s="28"/>
       <c r="L5" s="26"/>
     </row>
-    <row r="6" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>79</v>
       </c>
@@ -2806,7 +2814,7 @@
       </c>
       <c r="L6" s="26"/>
     </row>
-    <row r="7" spans="1:12" ht="81.400000000000006" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
@@ -2839,7 +2847,7 @@
       </c>
       <c r="L7" s="26"/>
     </row>
-    <row r="8" spans="1:12" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>79</v>
       </c>
@@ -2872,7 +2880,7 @@
       </c>
       <c r="L8" s="26"/>
     </row>
-    <row r="9" spans="1:12" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>79</v>
       </c>
@@ -2905,7 +2913,7 @@
       </c>
       <c r="L9" s="26"/>
     </row>
-    <row r="10" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
@@ -2938,7 +2946,7 @@
       </c>
       <c r="L10" s="26"/>
     </row>
-    <row r="11" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>79</v>
       </c>
@@ -2971,7 +2979,7 @@
       </c>
       <c r="L11" s="26"/>
     </row>
-    <row r="12" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>79</v>
       </c>
@@ -3004,7 +3012,7 @@
       </c>
       <c r="L12" s="26"/>
     </row>
-    <row r="13" spans="1:12" ht="81.400000000000006" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="84" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>79</v>
       </c>
@@ -3037,7 +3045,7 @@
       </c>
       <c r="L13" s="26"/>
     </row>
-    <row r="14" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>79</v>
       </c>
@@ -3070,7 +3078,7 @@
       </c>
       <c r="L14" s="26"/>
     </row>
-    <row r="15" spans="1:12" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="4">
         <v>13</v>
@@ -3102,7 +3110,7 @@
       <c r="K15" s="19"/>
       <c r="L15" s="26"/>
     </row>
-    <row r="16" spans="1:12" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>79</v>
       </c>
@@ -3110,33 +3118,33 @@
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>495</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>500</v>
       </c>
       <c r="K16" s="35"/>
       <c r="L16" s="26"/>
     </row>
-    <row r="17" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>79</v>
       </c>
@@ -3169,7 +3177,7 @@
       </c>
       <c r="L17" s="26"/>
     </row>
-    <row r="18" spans="1:12" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>79</v>
       </c>
@@ -3202,7 +3210,7 @@
       </c>
       <c r="L18" s="26"/>
     </row>
-    <row r="19" spans="1:12" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>79</v>
       </c>
@@ -3235,7 +3243,7 @@
       </c>
       <c r="L19" s="26"/>
     </row>
-    <row r="20" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>79</v>
       </c>
@@ -3268,7 +3276,7 @@
       </c>
       <c r="L20" s="26"/>
     </row>
-    <row r="21" spans="1:12" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>79</v>
       </c>
@@ -3301,7 +3309,7 @@
       </c>
       <c r="L21" s="26"/>
     </row>
-    <row r="22" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4">
         <v>20</v>
@@ -3328,11 +3336,11 @@
         <v>444</v>
       </c>
       <c r="J22" s="33" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="L22" s="26"/>
     </row>
-    <row r="23" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -3365,7 +3373,7 @@
       </c>
       <c r="L23" s="26"/>
     </row>
-    <row r="24" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="4">
         <v>22</v>
@@ -3396,7 +3404,7 @@
       </c>
       <c r="L24" s="26"/>
     </row>
-    <row r="25" spans="1:12" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>79</v>
       </c>
@@ -3429,7 +3437,7 @@
       </c>
       <c r="L25" s="26"/>
     </row>
-    <row r="26" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>79</v>
       </c>
@@ -3462,7 +3470,7 @@
       </c>
       <c r="L26" s="26"/>
     </row>
-    <row r="27" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>79</v>
       </c>
@@ -3495,7 +3503,7 @@
       </c>
       <c r="L27" s="26"/>
     </row>
-    <row r="28" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
@@ -3528,7 +3536,7 @@
       </c>
       <c r="L28" s="26"/>
     </row>
-    <row r="29" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>79</v>
       </c>
@@ -3561,7 +3569,7 @@
       </c>
       <c r="L29" s="26"/>
     </row>
-    <row r="30" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>79</v>
       </c>
@@ -3594,7 +3602,7 @@
       </c>
       <c r="L30" s="26"/>
     </row>
-    <row r="31" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>79</v>
       </c>
@@ -3627,7 +3635,7 @@
       </c>
       <c r="L31" s="26"/>
     </row>
-    <row r="32" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>79</v>
       </c>
@@ -3660,7 +3668,7 @@
       </c>
       <c r="L32" s="26"/>
     </row>
-    <row r="33" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>79</v>
       </c>
@@ -3693,7 +3701,7 @@
       </c>
       <c r="L33" s="26"/>
     </row>
-    <row r="34" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>79</v>
       </c>
@@ -3726,7 +3734,7 @@
       </c>
       <c r="L34" s="26"/>
     </row>
-    <row r="35" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>79</v>
       </c>
@@ -3760,7 +3768,7 @@
       <c r="K35" s="19"/>
       <c r="L35" s="26"/>
     </row>
-    <row r="36" spans="1:12" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
         <v>79</v>
       </c>
@@ -3768,7 +3776,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>452</v>
@@ -3785,16 +3793,16 @@
       <c r="H36" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I36" s="4" t="s">
-        <v>454</v>
+      <c r="I36" s="12" t="s">
+        <v>512</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K36" s="35"/>
       <c r="L36" s="26"/>
     </row>
-    <row r="37" spans="1:12" ht="58.15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A37" s="33" t="s">
         <v>79</v>
       </c>
@@ -3802,14 +3810,14 @@
         <v>35</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D37" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>460</v>
-      </c>
       <c r="F37" s="4" t="s">
         <v>4</v>
       </c>
@@ -3819,16 +3827,16 @@
       <c r="H37" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I37" s="4" t="s">
-        <v>462</v>
+      <c r="I37" s="12" t="s">
+        <v>511</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="K37" s="35"/>
       <c r="L37" s="26"/>
     </row>
-    <row r="38" spans="1:12" ht="81.400000000000006" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A38" s="33" t="s">
         <v>79</v>
       </c>
@@ -3836,13 +3844,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>4</v>
@@ -3853,16 +3861,16 @@
       <c r="H38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I38" s="4" t="s">
-        <v>476</v>
+      <c r="I38" s="12" t="s">
+        <v>513</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="K38" s="35"/>
       <c r="L38" s="26"/>
     </row>
-    <row r="39" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="33" t="s">
         <v>79</v>
       </c>
@@ -3870,13 +3878,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>469</v>
-      </c>
       <c r="E39" s="4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>4</v>
@@ -3887,16 +3895,16 @@
       <c r="H39" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="4" t="s">
-        <v>470</v>
+      <c r="I39" s="12" t="s">
+        <v>514</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="K39" s="35"/>
       <c r="L39" s="26"/>
     </row>
-    <row r="40" spans="1:12" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>79</v>
       </c>
@@ -3928,37 +3936,37 @@
         <v>299</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="4">
         <v>39</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>515</v>
+      </c>
+      <c r="J41" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="4">
         <v>40</v>
@@ -3986,7 +3994,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="4">
         <v>41</v>
@@ -4014,7 +4022,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="4">
         <v>42</v>
@@ -4041,22 +4049,22 @@
         <v>420</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="54.85" customHeight="1" x14ac:dyDescent="0.35">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="4">
         <v>43</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>4</v>
@@ -4069,10 +4077,10 @@
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="37" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="4">
         <v>44</v>
@@ -4100,7 +4108,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="4">
         <v>45</v>
@@ -4128,7 +4136,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="58.15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="4">
         <v>46</v>
@@ -4158,7 +4166,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="4">
         <v>47</v>
@@ -4183,10 +4191,10 @@
       </c>
       <c r="I49" s="4"/>
       <c r="J49" s="4" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="4">
         <v>48</v>
@@ -4214,7 +4222,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="58.15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="4">
         <v>49</v>
@@ -4244,7 +4252,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="4">
         <v>50</v>
@@ -4269,10 +4277,10 @@
       </c>
       <c r="I52" s="4"/>
       <c r="J52" s="12" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="4">
         <v>51</v>
@@ -4297,10 +4305,10 @@
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="12" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="58.15" x14ac:dyDescent="0.35">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="4">
         <v>52</v>
@@ -4330,7 +4338,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="4">
         <v>53</v>
@@ -4358,7 +4366,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="4">
         <v>54</v>
@@ -4386,7 +4394,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="4">
         <v>55</v>
@@ -4412,7 +4420,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="4">
         <v>56</v>
@@ -4442,7 +4450,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
       <c r="B59" s="4">
         <v>57</v>
@@ -4467,10 +4475,10 @@
         <v>310</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
       <c r="B60" s="4">
         <v>58</v>
@@ -4496,9 +4504,9 @@
         <v>312</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -4515,25 +4523,25 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A15" sqref="A15:J15"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.53125" customWidth="1"/>
-    <col min="4" max="4" width="20.1328125" customWidth="1"/>
-    <col min="5" max="5" width="15.265625" customWidth="1"/>
-    <col min="6" max="6" width="9.73046875" customWidth="1"/>
-    <col min="7" max="7" width="6.06640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="23.265625" customWidth="1"/>
-    <col min="10" max="10" width="40.265625" customWidth="1"/>
-    <col min="12" max="12" width="12.73046875" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" customWidth="1"/>
+    <col min="10" max="10" width="40.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>63</v>
       </c>
@@ -4565,7 +4573,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>73</v>
       </c>
@@ -4591,7 +4599,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>79</v>
       </c>
@@ -4621,7 +4629,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>79</v>
       </c>
@@ -4629,10 +4637,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>130</v>
@@ -4655,7 +4663,7 @@
       <c r="K4" s="19"/>
       <c r="L4" s="20"/>
     </row>
-    <row r="5" spans="1:12" ht="58.15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>79</v>
       </c>
@@ -4663,10 +4671,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>131</v>
@@ -4689,7 +4697,7 @@
       <c r="K5" s="19"/>
       <c r="L5" s="20"/>
     </row>
-    <row r="6" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>79</v>
       </c>
@@ -4722,7 +4730,7 @@
       </c>
       <c r="L6" s="20"/>
     </row>
-    <row r="7" spans="1:12" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>79</v>
       </c>
@@ -4755,7 +4763,7 @@
       </c>
       <c r="L7" s="20"/>
     </row>
-    <row r="8" spans="1:12" ht="24" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>79</v>
       </c>
@@ -4788,7 +4796,7 @@
       </c>
       <c r="L8" s="20"/>
     </row>
-    <row r="9" spans="1:12" ht="24" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>79</v>
       </c>
@@ -4821,7 +4829,7 @@
       </c>
       <c r="L9" s="20"/>
     </row>
-    <row r="10" spans="1:12" ht="24" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
@@ -4854,7 +4862,7 @@
       </c>
       <c r="L10" s="20"/>
     </row>
-    <row r="11" spans="1:12" ht="69.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" ht="72" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>79</v>
       </c>
@@ -4887,7 +4895,7 @@
       </c>
       <c r="L11" s="20"/>
     </row>
-    <row r="12" spans="1:12" ht="24" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>79</v>
       </c>
@@ -4920,7 +4928,7 @@
       </c>
       <c r="L12" s="20"/>
     </row>
-    <row r="13" spans="1:12" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" ht="48" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4">
         <v>11</v>
@@ -4952,7 +4960,7 @@
       <c r="K13" s="19"/>
       <c r="L13" s="20"/>
     </row>
-    <row r="14" spans="1:12" s="13" customFormat="1" ht="69.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" s="13" customFormat="1" ht="84" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>79</v>
       </c>
@@ -4960,33 +4968,33 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>499</v>
-      </c>
       <c r="J14" s="4" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="K14" s="35"/>
       <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="1:12" ht="24" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>79</v>
       </c>
@@ -5018,7 +5026,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="24" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>79</v>
       </c>
@@ -5050,7 +5058,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="14" customFormat="1" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>79</v>
       </c>
@@ -5082,7 +5090,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="14" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>79</v>
       </c>
@@ -5114,7 +5122,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>79</v>
       </c>
@@ -5146,7 +5154,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4">
         <v>18</v>
@@ -5155,7 +5163,7 @@
         <v>441</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>443</v>
@@ -5177,7 +5185,7 @@
       </c>
       <c r="L20" s="14"/>
     </row>
-    <row r="21" spans="1:12" s="1" customFormat="1" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>79</v>
       </c>
@@ -5210,7 +5218,7 @@
       </c>
       <c r="L21" s="13"/>
     </row>
-    <row r="22" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
@@ -5243,7 +5251,7 @@
       </c>
       <c r="L22" s="13"/>
     </row>
-    <row r="23" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>79</v>
       </c>
@@ -5276,7 +5284,7 @@
       </c>
       <c r="L23" s="13"/>
     </row>
-    <row r="24" spans="1:12" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>79</v>
       </c>
@@ -5309,7 +5317,7 @@
       </c>
       <c r="L24" s="13"/>
     </row>
-    <row r="25" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>79</v>
       </c>
@@ -5343,7 +5351,7 @@
       <c r="K25" s="11"/>
       <c r="L25" s="13"/>
     </row>
-    <row r="26" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>79</v>
       </c>
@@ -5375,7 +5383,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="13" customFormat="1" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" s="13" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
         <v>79</v>
       </c>
@@ -5383,31 +5391,31 @@
         <v>25</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>512</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="13" customFormat="1" ht="58.15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:12" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
         <v>79</v>
       </c>
@@ -5415,31 +5423,31 @@
         <v>26</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>463</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="38" t="s">
+        <v>511</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="E28" s="35" t="s">
-        <v>465</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I28" s="35" t="s">
-        <v>462</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="13" customFormat="1" ht="81.400000000000006" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:12" s="13" customFormat="1" ht="96" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
         <v>79</v>
       </c>
@@ -5447,14 +5455,14 @@
         <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>479</v>
-      </c>
       <c r="F29" s="4" t="s">
         <v>4</v>
       </c>
@@ -5464,14 +5472,14 @@
       <c r="H29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I29" s="4" t="s">
-        <v>476</v>
+      <c r="I29" s="12" t="s">
+        <v>513</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="13" customFormat="1" ht="46.5" x14ac:dyDescent="0.45">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
         <v>79</v>
       </c>
@@ -5479,13 +5487,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>4</v>
@@ -5496,14 +5504,14 @@
       <c r="H30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I30" s="4" t="s">
-        <v>470</v>
+      <c r="I30" s="12" t="s">
+        <v>514</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="39.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>79</v>
       </c>
@@ -5536,19 +5544,19 @@
       </c>
       <c r="L31" s="15"/>
     </row>
-    <row r="32" spans="1:12" s="13" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" s="13" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="4">
         <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>431</v>
@@ -5561,20 +5569,20 @@
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="8" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="L32" s="15"/>
     </row>
-    <row r="33" spans="1:12" ht="107.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" ht="107.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="4">
         <v>31</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>147</v>
@@ -5594,7 +5602,7 @@
       </c>
       <c r="L33" s="13"/>
     </row>
-    <row r="34" spans="1:12" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="4">
         <v>32</v>
@@ -5624,7 +5632,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="13"/>
     </row>
-    <row r="35" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="4">
         <v>33</v>
@@ -5653,7 +5661,7 @@
       </c>
       <c r="L35" s="13"/>
     </row>
-    <row r="36" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="4">
         <v>34</v>
@@ -5682,7 +5690,7 @@
       </c>
       <c r="L36" s="15"/>
     </row>
-    <row r="37" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="4">
         <v>35</v>
@@ -5711,7 +5719,7 @@
       </c>
       <c r="L37" s="15"/>
     </row>
-    <row r="38" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="4">
         <v>36</v>
@@ -5740,7 +5748,7 @@
       </c>
       <c r="L38" s="13"/>
     </row>
-    <row r="39" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="4">
         <v>37</v>
@@ -5769,7 +5777,7 @@
       </c>
       <c r="L39" s="13"/>
     </row>
-    <row r="40" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="4">
         <v>38</v>
@@ -5798,7 +5806,7 @@
       </c>
       <c r="L40" s="13"/>
     </row>
-    <row r="41" spans="1:12" ht="46.5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" ht="48" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="4">
         <v>39</v>
@@ -5827,7 +5835,7 @@
       </c>
       <c r="L41" s="13"/>
     </row>
-    <row r="42" spans="1:12" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" ht="48" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="4">
         <v>40</v>
@@ -5855,7 +5863,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="4">
         <v>41</v>
@@ -5883,7 +5891,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="4">
         <v>42</v>
@@ -5911,7 +5919,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="4">
         <v>43</v>
@@ -5939,7 +5947,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="4">
         <v>44</v>
@@ -5967,7 +5975,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="4">
         <v>45</v>
@@ -5995,7 +6003,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="37.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="4">
         <v>46</v>
@@ -6023,7 +6031,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="4">
         <v>47</v>
@@ -6051,7 +6059,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="4">
         <v>48</v>
@@ -6079,7 +6087,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="4">
         <v>49</v>
@@ -6107,7 +6115,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="4">
         <v>50</v>
@@ -6135,7 +6143,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="4">
         <v>51</v>
@@ -6163,7 +6171,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="4">
         <v>52</v>
@@ -6191,7 +6199,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="4">
         <v>53</v>
@@ -6219,7 +6227,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="4">
         <v>54</v>
@@ -6247,7 +6255,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="14" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
       <c r="B57" s="4">
         <v>55</v>
@@ -6275,7 +6283,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="14" customFormat="1" ht="58.15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="4">
         <v>56</v>
@@ -6305,7 +6313,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="14" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" s="14" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="4">
         <v>57</v>
@@ -6333,7 +6341,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="46.5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10" ht="48" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4">
         <v>58</v>
@@ -6361,7 +6369,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="13" customFormat="1" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" s="13" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="4">
         <v>59</v>
@@ -6391,7 +6399,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="13" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10" s="13" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="4">
         <v>60</v>
@@ -6416,10 +6424,10 @@
         <v>310</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="69.75" x14ac:dyDescent="0.45">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="72" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="4">
         <v>61</v>

</xml_diff>

<commit_message>
No format change - yellow colour removed
There is no format change for February 2026. The yellow colour is removed.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CL CE.xlsx
+++ b/Documents/RDBES Data Model CL CE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29725"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\RDBES_Core_Group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icesit-my.sharepoint.com/personal/henrikkn_ices_dk/Documents/RDBES/Data model/BACKUPs Data model Published/2026 02 02 After yellow removed no change/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC6FAD1-7F3B-4805-A2D1-D4D95CB5526A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{BEC6FAD1-7F3B-4805-A2D1-D4D95CB5526A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AA9AB20-1BAB-4BCC-95AB-D58C33E560B9}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="63195" yWindow="930" windowWidth="20925" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial Landing CL" sheetId="3" r:id="rId1"/>
@@ -1713,46 +1713,6 @@
     <t>For passive nets, the scientific number of meter multiplied with hours the gear is fishing. This reflect the gear effort.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Allowed codes are: “Official” and "Estimated"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-“Official”: Official data, which can be 1) census data (e.g. control regulation data as logbooks, sales notes, declarative forms eventually combined) or 2) official sampling data. 
-“Estimate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>”: Data coming from scientific estimates based on scientific sampling or scientific reevaluation and not officially registered and/or reported. Do not provide overlapping data.</t>
-    </r>
-  </si>
-  <si>
     <t>DataSource
 //vocab.ices.dk/?ref=1768</t>
   </si>
@@ -1844,27 +1804,6 @@
   </si>
   <si>
     <t>CLencryptedVesselIds</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Data Source of scientific weight. When DataBasisOfScientificWeight is  “Official”, Allowed codes are:  "CombOD", "Logb", "OthDF", "SalN". When When DataBasisOfScientificWeight is  “Estimated”, Allowed codes are: "SampDS", "SampDC", "Exprt", "OthDF", "CombOD". </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Data Source of scientific effort. When DataBasisOfScientificEffort is  “Official”, allowed codes are:  "CombOD", "Logb", "OthDF", "SalN". When DataBasisOfScientificEffort is  “Estimated”, allowed codes are: "SampDS", "SampDC", "Exprt", "Logb", "CombOD". </t>
@@ -1899,7 +1838,16 @@
     </r>
   </si>
   <si>
-    <t>Ver 1.19.35</t>
+    <t>Allowed codes are: “Official” and "Estimated"
+“Official”: Official data, which can be 1) census data (e.g. control regulation data as logbooks, sales notes, declarative forms eventually combined) or 2) official sampling data. 
+“Estimated”: Data coming from scientific estimates based on scientific sampling or scientific reevaluation and not officially registered and/or reported. Do not provide overlapping data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Source of scientific weight. When DataBasisOfScientificWeight is  “Official”, Allowed codes are:  "CombOD", "Logb", "OthDF", "SalN". When When DataBasisOfScientificWeight is  “Estimated”, Allowed codes are: "SampDS", "SampDC", "Exprt", "OthDF", "CombOD". 
+</t>
+  </si>
+  <si>
+    <t>Ver 1.19.36</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +1938,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2002,14 +1950,8 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2041,25 +1983,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2075,9 +2004,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2126,18 +2052,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2419,14 +2354,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:DB63"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.65"/>
@@ -2440,44 +2372,139 @@
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.26953125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="41.7265625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="41.7265625" style="10" customWidth="1"/>
     <col min="11" max="11" width="36.81640625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="36.75" x14ac:dyDescent="0.65">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:106" ht="36.75" x14ac:dyDescent="0.65">
+      <c r="A1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30"/>
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30"/>
+      <c r="BN1" s="30"/>
+      <c r="BO1" s="30"/>
+      <c r="BP1" s="30"/>
+      <c r="BQ1" s="30"/>
+      <c r="BR1" s="30"/>
+      <c r="BS1" s="30"/>
+      <c r="BT1" s="30"/>
+      <c r="BU1" s="30"/>
+      <c r="BV1" s="30"/>
+      <c r="BW1" s="30"/>
+      <c r="BX1" s="30"/>
+      <c r="BY1" s="30"/>
+      <c r="BZ1" s="30"/>
+      <c r="CA1" s="30"/>
+      <c r="CB1" s="30"/>
+      <c r="CC1" s="30"/>
+      <c r="CD1" s="30"/>
+      <c r="CE1" s="30"/>
+      <c r="CF1" s="30"/>
+      <c r="CG1" s="30"/>
+      <c r="CH1" s="30"/>
+      <c r="CI1" s="30"/>
+      <c r="CJ1" s="30"/>
+      <c r="CK1" s="30"/>
+      <c r="CL1" s="30"/>
+      <c r="CM1" s="30"/>
+      <c r="CN1" s="30"/>
+      <c r="CO1" s="30"/>
+      <c r="CP1" s="30"/>
+      <c r="CQ1" s="30"/>
+      <c r="CR1" s="30"/>
+      <c r="CS1" s="30"/>
+      <c r="CT1" s="30"/>
+      <c r="CU1" s="30"/>
+      <c r="CV1" s="30"/>
+      <c r="CW1" s="30"/>
+      <c r="CX1" s="30"/>
+      <c r="CY1" s="30"/>
+      <c r="CZ1" s="30"/>
+      <c r="DA1" s="30"/>
+      <c r="DB1" s="30"/>
+    </row>
+    <row r="2" spans="1:106" ht="24.5" x14ac:dyDescent="0.65">
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
@@ -2503,7 +2530,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="12.25" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:106" ht="12.25" x14ac:dyDescent="0.65">
       <c r="A3" s="3"/>
       <c r="B3" s="4">
         <v>1</v>
@@ -2531,73 +2558,73 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="98" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:106" ht="110.25" x14ac:dyDescent="0.65">
       <c r="A4" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>496</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>499</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>506</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="C4" s="23" t="s">
+        <v>495</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>498</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>505</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>494</v>
+      <c r="H4" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>493</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>492</v>
-      </c>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" ht="93" customHeight="1" x14ac:dyDescent="0.65">
+        <v>522</v>
+      </c>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="1:106" ht="93" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>493</v>
+      <c r="H5" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>492</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>519</v>
-      </c>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:11" ht="49" x14ac:dyDescent="0.65">
+        <v>523</v>
+      </c>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:106" ht="49" x14ac:dyDescent="0.65">
       <c r="A6" s="3" t="s">
         <v>77</v>
       </c>
@@ -2629,7 +2656,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="98" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:106" ht="98" x14ac:dyDescent="0.65">
       <c r="A7" s="3" t="s">
         <v>77</v>
       </c>
@@ -2661,7 +2688,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="73.5" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:106" ht="85.75" x14ac:dyDescent="0.65">
       <c r="A8" s="3" t="s">
         <v>77</v>
       </c>
@@ -2693,7 +2720,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="36.75" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:106" ht="36.75" x14ac:dyDescent="0.65">
       <c r="A9" s="3" t="s">
         <v>77</v>
       </c>
@@ -2725,7 +2752,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:106" ht="24.5" x14ac:dyDescent="0.65">
       <c r="A10" s="3" t="s">
         <v>77</v>
       </c>
@@ -2757,7 +2784,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:106" ht="24.5" x14ac:dyDescent="0.65">
       <c r="A11" s="3" t="s">
         <v>77</v>
       </c>
@@ -2789,7 +2816,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:106" ht="24.5" x14ac:dyDescent="0.65">
       <c r="A12" s="3" t="s">
         <v>77</v>
       </c>
@@ -2821,7 +2848,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="85.75" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:106" ht="85.75" x14ac:dyDescent="0.65">
       <c r="A13" s="3" t="s">
         <v>77</v>
       </c>
@@ -2853,7 +2880,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:106" ht="36.75" x14ac:dyDescent="0.65">
       <c r="A14" s="3" t="s">
         <v>77</v>
       </c>
@@ -2885,21 +2912,21 @@
         <v>251</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
-      <c r="A15" s="24" t="s">
+    <row r="15" spans="1:106" ht="24.5" x14ac:dyDescent="0.65">
+      <c r="A15" s="28" t="s">
         <v>77</v>
       </c>
       <c r="B15" s="25">
         <v>13</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F15" s="25" t="s">
         <v>4</v>
@@ -2911,42 +2938,42 @@
         <v>6</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="122.5" x14ac:dyDescent="0.65">
-      <c r="A16" s="24" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="16" spans="1:106" ht="134.75" x14ac:dyDescent="0.65">
+      <c r="A16" s="28" t="s">
         <v>77</v>
       </c>
       <c r="B16" s="25">
         <v>14</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="F16" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="25" t="s">
         <v>6</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>493</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>521</v>
+        <v>492</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>519</v>
       </c>
       <c r="K16" s="6"/>
     </row>
@@ -2954,7 +2981,7 @@
       <c r="A17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="23">
         <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -2981,13 +3008,13 @@
       <c r="J17" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="K17" s="12"/>
+      <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" ht="36.75" x14ac:dyDescent="0.65">
       <c r="A18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="23">
         <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -3019,7 +3046,7 @@
       <c r="A19" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="23">
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -3051,7 +3078,7 @@
       <c r="A20" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="23">
         <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -3083,7 +3110,7 @@
       <c r="A21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="23">
         <v>19</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -3115,7 +3142,7 @@
       <c r="A22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22" s="23">
         <v>20</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -3144,10 +3171,10 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="49" x14ac:dyDescent="0.65">
-      <c r="A23" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="25">
+      <c r="A23" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="23">
         <v>21</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -3175,11 +3202,11 @@
         <v>472</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="49" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:11" ht="61.25" x14ac:dyDescent="0.65">
       <c r="A24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="23">
         <v>22</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -3209,7 +3236,7 @@
     </row>
     <row r="25" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
       <c r="A25" s="3"/>
-      <c r="B25" s="25">
+      <c r="B25" s="23">
         <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -3241,7 +3268,7 @@
       <c r="A26" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="25">
+      <c r="B26" s="23">
         <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -3265,7 +3292,7 @@
       <c r="I26" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="J26" s="22" t="s">
+      <c r="J26" s="21" t="s">
         <v>489</v>
       </c>
     </row>
@@ -3273,7 +3300,7 @@
       <c r="A27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="23">
         <v>25</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -3297,15 +3324,15 @@
       <c r="I27" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="J27" s="12" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.65">
-      <c r="A28" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="25">
+      <c r="A28" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="23">
         <v>26</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -3329,15 +3356,15 @@
       <c r="I28" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="12" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:11" ht="36.75" x14ac:dyDescent="0.65">
       <c r="A29" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="23">
         <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -3369,7 +3396,7 @@
       <c r="A30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="25">
+      <c r="B30" s="23">
         <v>28</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -3401,7 +3428,7 @@
       <c r="A31" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="23">
         <v>29</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -3433,7 +3460,7 @@
       <c r="A32" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B32" s="23">
         <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -3465,7 +3492,7 @@
       <c r="A33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="23">
         <v>31</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -3497,7 +3524,7 @@
       <c r="A34" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="23">
         <v>32</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -3529,7 +3556,7 @@
       <c r="A35" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="25">
+      <c r="B35" s="23">
         <v>33</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -3557,11 +3584,11 @@
         <v>355</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
+    <row r="36" spans="1:11" ht="36.75" x14ac:dyDescent="0.65">
       <c r="A36" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="23">
         <v>34</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -3585,7 +3612,7 @@
       <c r="I36" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="J36" s="15" t="s">
+      <c r="J36" s="14" t="s">
         <v>357</v>
       </c>
       <c r="K36" s="6"/>
@@ -3594,7 +3621,7 @@
       <c r="A37" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="25">
+      <c r="B37" s="23">
         <v>35</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -3621,13 +3648,13 @@
       <c r="J37" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="K37" s="12"/>
+      <c r="K37" s="11"/>
     </row>
     <row r="38" spans="1:11" ht="73.5" x14ac:dyDescent="0.65">
       <c r="A38" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="25">
+      <c r="B38" s="23">
         <v>36</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -3654,13 +3681,13 @@
       <c r="J38" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="K38" s="12"/>
+      <c r="K38" s="11"/>
     </row>
     <row r="39" spans="1:11" ht="98" x14ac:dyDescent="0.65">
       <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="25">
+      <c r="B39" s="23">
         <v>37</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -3687,13 +3714,13 @@
       <c r="J39" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="K39" s="12"/>
+      <c r="K39" s="11"/>
     </row>
     <row r="40" spans="1:11" ht="61.25" x14ac:dyDescent="0.65">
       <c r="A40" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="25">
+      <c r="B40" s="23">
         <v>38</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -3720,22 +3747,22 @@
       <c r="J40" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="K40" s="12"/>
+      <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:11" ht="36.75" x14ac:dyDescent="0.65">
       <c r="A41" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="25">
+      <c r="B41" s="23">
         <v>39</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="15" t="s">
         <v>182</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="15" t="s">
         <v>187</v>
       </c>
       <c r="F41" s="4" t="s">
@@ -3747,7 +3774,7 @@
       <c r="H41" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I41" s="17" t="s">
+      <c r="I41" s="16" t="s">
         <v>294</v>
       </c>
       <c r="J41" s="4" t="s">
@@ -3756,7 +3783,7 @@
     </row>
     <row r="42" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
       <c r="A42" s="3"/>
-      <c r="B42" s="25">
+      <c r="B42" s="23">
         <v>40</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -3784,9 +3811,9 @@
         <v>452</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
+    <row r="43" spans="1:11" ht="36.75" x14ac:dyDescent="0.65">
       <c r="A43" s="3"/>
-      <c r="B43" s="25">
+      <c r="B43" s="23">
         <v>41</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -3801,7 +3828,7 @@
       <c r="F43" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="G43" s="25" t="s">
+      <c r="G43" s="23" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="4" t="s">
@@ -3812,9 +3839,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
+    <row r="44" spans="1:11" ht="36.75" x14ac:dyDescent="0.65">
       <c r="A44" s="3"/>
-      <c r="B44" s="25">
+      <c r="B44" s="23">
         <v>42</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -3840,9 +3867,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="49" x14ac:dyDescent="0.65">
+    <row r="45" spans="1:11" ht="61.25" x14ac:dyDescent="0.65">
       <c r="A45" s="3"/>
-      <c r="B45" s="25">
+      <c r="B45" s="23">
         <v>43</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -3872,7 +3899,7 @@
     </row>
     <row r="46" spans="1:11" ht="55" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A46" s="3"/>
-      <c r="B46" s="25">
+      <c r="B46" s="23">
         <v>44</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -3894,13 +3921,13 @@
         <v>31</v>
       </c>
       <c r="I46" s="4"/>
-      <c r="J46" s="18" t="s">
+      <c r="J46" s="17" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="24.5" x14ac:dyDescent="0.65">
       <c r="A47" s="3"/>
-      <c r="B47" s="25">
+      <c r="B47" s="23">
         <v>45</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -3928,7 +3955,7 @@
     </row>
     <row r="48" spans="1:11" ht="49" x14ac:dyDescent="0.65">
       <c r="A48" s="3"/>
-      <c r="B48" s="25">
+      <c r="B48" s="23">
         <v>46</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -3956,7 +3983,7 @@
     </row>
     <row r="49" spans="1:10" ht="73.5" x14ac:dyDescent="0.65">
       <c r="A49" s="3"/>
-      <c r="B49" s="25">
+      <c r="B49" s="23">
         <v>47</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -3986,7 +4013,7 @@
     </row>
     <row r="50" spans="1:10" ht="49" x14ac:dyDescent="0.65">
       <c r="A50" s="3"/>
-      <c r="B50" s="25">
+      <c r="B50" s="23">
         <v>48</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -4014,7 +4041,7 @@
     </row>
     <row r="51" spans="1:10" ht="49" x14ac:dyDescent="0.65">
       <c r="A51" s="3"/>
-      <c r="B51" s="25">
+      <c r="B51" s="23">
         <v>49</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -4042,7 +4069,7 @@
     </row>
     <row r="52" spans="1:10" ht="61.25" x14ac:dyDescent="0.65">
       <c r="A52" s="3"/>
-      <c r="B52" s="25">
+      <c r="B52" s="23">
         <v>50</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -4072,7 +4099,7 @@
     </row>
     <row r="53" spans="1:10" ht="49" x14ac:dyDescent="0.65">
       <c r="A53" s="3"/>
-      <c r="B53" s="25">
+      <c r="B53" s="23">
         <v>51</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -4100,7 +4127,7 @@
     </row>
     <row r="54" spans="1:10" ht="49" x14ac:dyDescent="0.65">
       <c r="A54" s="3"/>
-      <c r="B54" s="25">
+      <c r="B54" s="23">
         <v>52</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -4128,7 +4155,7 @@
     </row>
     <row r="55" spans="1:10" ht="61.25" x14ac:dyDescent="0.65">
       <c r="A55" s="3"/>
-      <c r="B55" s="25">
+      <c r="B55" s="23">
         <v>53</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -4158,7 +4185,7 @@
     </row>
     <row r="56" spans="1:10" ht="36.75" x14ac:dyDescent="0.65">
       <c r="A56" s="3"/>
-      <c r="B56" s="25">
+      <c r="B56" s="23">
         <v>54</v>
       </c>
       <c r="C56" s="4" t="s">
@@ -4186,7 +4213,7 @@
     </row>
     <row r="57" spans="1:10" ht="36.75" x14ac:dyDescent="0.65">
       <c r="A57" s="3"/>
-      <c r="B57" s="25">
+      <c r="B57" s="23">
         <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -4214,7 +4241,7 @@
     </row>
     <row r="58" spans="1:10" ht="24.5" x14ac:dyDescent="0.65">
       <c r="A58" s="3"/>
-      <c r="B58" s="25">
+      <c r="B58" s="23">
         <v>56</v>
       </c>
       <c r="C58" s="4" t="s">
@@ -4240,7 +4267,7 @@
     </row>
     <row r="59" spans="1:10" ht="49" x14ac:dyDescent="0.65">
       <c r="A59" s="3"/>
-      <c r="B59" s="25">
+      <c r="B59" s="23">
         <v>57</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -4269,8 +4296,8 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A60" s="19"/>
-      <c r="B60" s="25">
+      <c r="A60" s="18"/>
+      <c r="B60" s="23">
         <v>58</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -4292,20 +4319,20 @@
       <c r="I60" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="J60" s="20" t="s">
+      <c r="J60" s="19" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A61" s="19"/>
-      <c r="B61" s="25">
+      <c r="A61" s="18"/>
+      <c r="B61" s="23">
         <v>59</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>290</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>419</v>
@@ -4318,7 +4345,7 @@
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="5"/>
-      <c r="J61" s="20" t="s">
+      <c r="J61" s="19" t="s">
         <v>296</v>
       </c>
     </row>
@@ -4335,15 +4362,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A15" sqref="A15:J15"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4360,34 +4384,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="37.25" x14ac:dyDescent="0.75">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4418,7 +4442,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="30.65" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B3" s="4">
@@ -4448,73 +4472,73 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="104.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>498</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>501</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>504</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="C4" s="23" t="s">
+        <v>497</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>500</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>503</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="26" t="s">
-        <v>494</v>
+      <c r="I4" s="24" t="s">
+        <v>493</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>492</v>
+        <v>522</v>
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="61.25" x14ac:dyDescent="0.75">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:11" ht="73.5" x14ac:dyDescent="0.75">
+      <c r="A5" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="23" t="s">
         <v>481</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="23" t="s">
         <v>482</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>493</v>
-      </c>
-      <c r="J5" s="27" t="s">
-        <v>520</v>
+      <c r="H5" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>518</v>
       </c>
       <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="4">
@@ -4541,12 +4565,12 @@
       <c r="I6" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="20" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="36.75" x14ac:dyDescent="0.75">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4">
@@ -4573,12 +4597,12 @@
       <c r="I7" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="20" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="25" x14ac:dyDescent="0.75">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B8" s="4">
@@ -4610,7 +4634,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="25" x14ac:dyDescent="0.75">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="4">
@@ -4637,12 +4661,12 @@
       <c r="I9" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="18" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="25" x14ac:dyDescent="0.75">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B10" s="4">
@@ -4652,10 +4676,10 @@
         <v>15</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>13</v>
@@ -4669,12 +4693,12 @@
       <c r="I10" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="18" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="73.5" x14ac:dyDescent="0.75">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B11" s="4">
@@ -4684,10 +4708,10 @@
         <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>4</v>
@@ -4701,12 +4725,12 @@
       <c r="I11" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="19" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="25" x14ac:dyDescent="0.75">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:11" ht="37.25" x14ac:dyDescent="0.75">
+      <c r="A12" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B12" s="4">
@@ -4716,7 +4740,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>134</v>
@@ -4738,108 +4762,108 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="36.75" x14ac:dyDescent="0.75">
-      <c r="A13" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="25">
+      <c r="A13" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="23">
         <v>11</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="D13" s="25" t="s">
+      <c r="C13" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>501</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>502</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>503</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="25" t="s">
+      <c r="F13" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>495</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="122.5" x14ac:dyDescent="0.75">
-      <c r="A14" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="25">
+      <c r="H13" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>494</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="134.75" x14ac:dyDescent="0.75">
+      <c r="A14" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="23">
         <v>12</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="F14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>493</v>
-      </c>
-      <c r="J14" s="27" t="s">
-        <v>522</v>
+      <c r="H14" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>520</v>
       </c>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" ht="61.25" x14ac:dyDescent="0.75">
-      <c r="A15" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="25">
+      <c r="A15" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="23">
         <v>13</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="23" t="s">
         <v>457</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="23" t="s">
         <v>458</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="23" t="s">
         <v>459</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="4" t="s">
+      <c r="F15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="23" t="s">
         <v>464</v>
       </c>
-      <c r="J15" s="25" t="s">
-        <v>507</v>
-      </c>
-      <c r="K15" s="12"/>
+      <c r="J15" s="23" t="s">
+        <v>506</v>
+      </c>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:11" ht="37.25" x14ac:dyDescent="0.75">
-      <c r="A16" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="25">
+      <c r="A16" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="23">
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -4871,7 +4895,7 @@
       <c r="A17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="23">
         <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -4903,7 +4927,7 @@
       <c r="A18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="23">
         <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -4935,7 +4959,7 @@
       <c r="A19" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="23">
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -4964,10 +4988,10 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="36.75" x14ac:dyDescent="0.75">
-      <c r="A20" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="25">
+      <c r="A20" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="23">
         <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -4996,10 +5020,10 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="49.5" x14ac:dyDescent="0.75">
-      <c r="A21" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="25">
+      <c r="A21" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="23">
         <v>19</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -5009,7 +5033,7 @@
         <v>462</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>4</v>
@@ -5029,10 +5053,10 @@
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" s="1" customFormat="1" ht="36.75" x14ac:dyDescent="0.75">
-      <c r="A22" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="25">
+      <c r="A22" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="23">
         <v>20</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -5062,10 +5086,10 @@
       <c r="L22"/>
     </row>
     <row r="23" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A23" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="25">
+      <c r="A23" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="23">
         <v>21</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -5094,10 +5118,10 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="36.75" x14ac:dyDescent="0.75">
-      <c r="A24" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="25">
+      <c r="A24" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="23">
         <v>22</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -5126,10 +5150,10 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="37.25" x14ac:dyDescent="0.75">
-      <c r="A25" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="25">
+      <c r="A25" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="23">
         <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -5158,10 +5182,10 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A26" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="25">
+      <c r="A26" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="23">
         <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -5191,10 +5215,10 @@
       <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A27" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="25">
+      <c r="A27" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="23">
         <v>25</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -5218,15 +5242,15 @@
       <c r="I27" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="J27" s="14" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="36.75" x14ac:dyDescent="0.75">
-      <c r="A28" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="25">
+      <c r="A28" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="23">
         <v>26</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -5255,10 +5279,10 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="61.25" x14ac:dyDescent="0.75">
-      <c r="A29" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="25">
+      <c r="A29" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="23">
         <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -5267,7 +5291,7 @@
       <c r="D29" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="16" t="s">
         <v>433</v>
       </c>
       <c r="F29" s="4" t="s">
@@ -5279,7 +5303,7 @@
       <c r="H29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I29" s="17" t="s">
+      <c r="I29" s="16" t="s">
         <v>467</v>
       </c>
       <c r="J29" s="4" t="s">
@@ -5287,10 +5311,10 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="98" x14ac:dyDescent="0.75">
-      <c r="A30" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="25">
+      <c r="A30" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="23">
         <v>28</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -5319,10 +5343,10 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="61.25" x14ac:dyDescent="0.75">
-      <c r="A31" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="25">
+      <c r="A31" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="23">
         <v>29</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -5351,10 +5375,10 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="39.4" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A32" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="25">
+      <c r="A32" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="23">
         <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -5378,14 +5402,14 @@
       <c r="I32" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="J32" s="21" t="s">
+      <c r="J32" s="20" t="s">
         <v>185</v>
       </c>
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="1:12" ht="39.4" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A33" s="19"/>
-      <c r="B33" s="25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="23">
         <v>31</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -5407,14 +5431,14 @@
         <v>44</v>
       </c>
       <c r="I33" s="4"/>
-      <c r="J33" s="21" t="s">
+      <c r="J33" s="20" t="s">
         <v>456</v>
       </c>
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:12" ht="107.65" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A34" s="19"/>
-      <c r="B34" s="25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="23">
         <v>32</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -5435,14 +5459,14 @@
       <c r="H34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I34" s="19"/>
-      <c r="J34" s="21" t="s">
+      <c r="I34" s="18"/>
+      <c r="J34" s="20" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A35" s="19"/>
-      <c r="B35" s="25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="23">
         <v>33</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -5463,15 +5487,15 @@
       <c r="H35" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I35" s="19"/>
-      <c r="J35" s="21" t="s">
+      <c r="I35" s="18"/>
+      <c r="J35" s="20" t="s">
         <v>255</v>
       </c>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A36" s="19"/>
-      <c r="B36" s="25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="23">
         <v>34</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -5492,24 +5516,24 @@
       <c r="H36" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I36" s="19"/>
-      <c r="J36" s="21" t="s">
+      <c r="I36" s="18"/>
+      <c r="J36" s="20" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A37" s="19"/>
-      <c r="B37" s="25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="23">
         <v>35</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D37" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>513</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>514</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>402</v>
@@ -5520,15 +5544,15 @@
       <c r="H37" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I37" s="19"/>
-      <c r="J37" s="21" t="s">
+      <c r="I37" s="18"/>
+      <c r="J37" s="20" t="s">
         <v>167</v>
       </c>
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A38" s="19"/>
-      <c r="B38" s="25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="23">
         <v>36</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -5549,15 +5573,15 @@
       <c r="H38" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I38" s="19"/>
-      <c r="J38" s="21" t="s">
+      <c r="I38" s="18"/>
+      <c r="J38" s="20" t="s">
         <v>237</v>
       </c>
       <c r="L38" s="2"/>
     </row>
     <row r="39" spans="1:12" ht="36.75" x14ac:dyDescent="0.75">
-      <c r="A39" s="19"/>
-      <c r="B39" s="25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="23">
         <v>37</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -5578,14 +5602,14 @@
       <c r="H39" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I39" s="19"/>
-      <c r="J39" s="21" t="s">
+      <c r="I39" s="18"/>
+      <c r="J39" s="20" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A40" s="19"/>
-      <c r="B40" s="25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="23">
         <v>38</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -5606,21 +5630,21 @@
       <c r="H40" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I40" s="19"/>
-      <c r="J40" s="21" t="s">
+      <c r="I40" s="18"/>
+      <c r="J40" s="20" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A41" s="19"/>
-      <c r="B41" s="25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="23">
         <v>39</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>188</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>191</v>
@@ -5634,14 +5658,14 @@
       <c r="H41" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I41" s="19"/>
-      <c r="J41" s="21" t="s">
+      <c r="I41" s="18"/>
+      <c r="J41" s="20" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="49" x14ac:dyDescent="0.75">
-      <c r="A42" s="19"/>
-      <c r="B42" s="25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="23">
         <v>40</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -5662,14 +5686,14 @@
       <c r="H42" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I42" s="19"/>
-      <c r="J42" s="21" t="s">
+      <c r="I42" s="18"/>
+      <c r="J42" s="20" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="36.75" x14ac:dyDescent="0.75">
-      <c r="A43" s="19"/>
-      <c r="B43" s="25">
+    <row r="43" spans="1:12" ht="49" x14ac:dyDescent="0.75">
+      <c r="A43" s="18"/>
+      <c r="B43" s="23">
         <v>41</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -5690,14 +5714,14 @@
       <c r="H43" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I43" s="19"/>
-      <c r="J43" s="21" t="s">
+      <c r="I43" s="18"/>
+      <c r="J43" s="20" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="36.75" x14ac:dyDescent="0.75">
-      <c r="A44" s="19"/>
-      <c r="B44" s="25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="23">
         <v>42</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -5718,14 +5742,14 @@
       <c r="H44" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="I44" s="19"/>
-      <c r="J44" s="23" t="s">
+      <c r="I44" s="18"/>
+      <c r="J44" s="22" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A45" s="19"/>
-      <c r="B45" s="25">
+    <row r="45" spans="1:12" ht="36.75" x14ac:dyDescent="0.75">
+      <c r="A45" s="18"/>
+      <c r="B45" s="23">
         <v>43</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -5746,14 +5770,14 @@
       <c r="H45" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="I45" s="19"/>
-      <c r="J45" s="23" t="s">
+      <c r="I45" s="18"/>
+      <c r="J45" s="22" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A46" s="19"/>
-      <c r="B46" s="25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="23">
         <v>44</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -5774,14 +5798,14 @@
       <c r="H46" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I46" s="19"/>
-      <c r="J46" s="21" t="s">
+      <c r="I46" s="18"/>
+      <c r="J46" s="20" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A47" s="19"/>
-      <c r="B47" s="25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="23">
         <v>45</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -5802,14 +5826,14 @@
       <c r="H47" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I47" s="19"/>
-      <c r="J47" s="21" t="s">
+      <c r="I47" s="18"/>
+      <c r="J47" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A48" s="19"/>
-      <c r="B48" s="25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="23">
         <v>46</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -5830,14 +5854,14 @@
       <c r="H48" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I48" s="19"/>
-      <c r="J48" s="21" t="s">
+      <c r="I48" s="18"/>
+      <c r="J48" s="20" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="37.4" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A49" s="19"/>
-      <c r="B49" s="25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="23">
         <v>47</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -5858,21 +5882,21 @@
       <c r="H49" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I49" s="19"/>
-      <c r="J49" s="21" t="s">
+      <c r="I49" s="18"/>
+      <c r="J49" s="20" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="31.9" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A50" s="19"/>
-      <c r="B50" s="25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="23">
         <v>48</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>243</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>203</v>
@@ -5886,14 +5910,14 @@
       <c r="H50" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="I50" s="19"/>
-      <c r="J50" s="21" t="s">
+      <c r="I50" s="18"/>
+      <c r="J50" s="20" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A51" s="19"/>
-      <c r="B51" s="25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="23">
         <v>49</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -5914,14 +5938,14 @@
       <c r="H51" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I51" s="19"/>
-      <c r="J51" s="21" t="s">
+      <c r="I51" s="18"/>
+      <c r="J51" s="20" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A52" s="19"/>
-      <c r="B52" s="25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="23">
         <v>50</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -5942,14 +5966,14 @@
       <c r="H52" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I52" s="19"/>
-      <c r="J52" s="21" t="s">
+      <c r="I52" s="18"/>
+      <c r="J52" s="20" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A53" s="19"/>
-      <c r="B53" s="25">
+      <c r="A53" s="18"/>
+      <c r="B53" s="23">
         <v>51</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -5970,14 +5994,14 @@
       <c r="H53" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I53" s="19"/>
-      <c r="J53" s="21" t="s">
+      <c r="I53" s="18"/>
+      <c r="J53" s="20" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A54" s="19"/>
-      <c r="B54" s="25">
+      <c r="A54" s="18"/>
+      <c r="B54" s="23">
         <v>52</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -5998,14 +6022,14 @@
       <c r="H54" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="I54" s="19"/>
-      <c r="J54" s="21" t="s">
+      <c r="I54" s="18"/>
+      <c r="J54" s="20" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A55" s="19"/>
-      <c r="B55" s="25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="23">
         <v>53</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -6026,14 +6050,14 @@
       <c r="H55" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I55" s="19"/>
-      <c r="J55" s="21" t="s">
+      <c r="I55" s="18"/>
+      <c r="J55" s="20" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="61.25" x14ac:dyDescent="0.75">
-      <c r="A56" s="19"/>
-      <c r="B56" s="25">
+      <c r="A56" s="18"/>
+      <c r="B56" s="23">
         <v>54</v>
       </c>
       <c r="C56" s="4" t="s">
@@ -6054,14 +6078,14 @@
       <c r="H56" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="I56" s="19"/>
-      <c r="J56" s="21" t="s">
+      <c r="I56" s="18"/>
+      <c r="J56" s="20" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="24.5" x14ac:dyDescent="0.75">
-      <c r="A57" s="19"/>
-      <c r="B57" s="25">
+      <c r="A57" s="18"/>
+      <c r="B57" s="23">
         <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -6082,14 +6106,14 @@
       <c r="H57" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="I57" s="19"/>
-      <c r="J57" s="21" t="s">
+      <c r="I57" s="18"/>
+      <c r="J57" s="20" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="1" customFormat="1" ht="24.5" x14ac:dyDescent="0.65">
-      <c r="A58" s="19"/>
-      <c r="B58" s="25">
+    <row r="58" spans="1:10" s="1" customFormat="1" ht="36.75" x14ac:dyDescent="0.65">
+      <c r="A58" s="18"/>
+      <c r="B58" s="23">
         <v>56</v>
       </c>
       <c r="C58" s="4" t="s">
@@ -6110,14 +6134,14 @@
       <c r="H58" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="I58" s="19"/>
-      <c r="J58" s="21" t="s">
+      <c r="I58" s="18"/>
+      <c r="J58" s="20" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="1" customFormat="1" ht="73.5" x14ac:dyDescent="0.65">
       <c r="A59" s="3"/>
-      <c r="B59" s="25">
+      <c r="B59" s="23">
         <v>57</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -6147,7 +6171,7 @@
     </row>
     <row r="60" spans="1:10" s="1" customFormat="1" ht="49" x14ac:dyDescent="0.65">
       <c r="A60" s="3"/>
-      <c r="B60" s="25">
+      <c r="B60" s="23">
         <v>58</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -6175,7 +6199,7 @@
     </row>
     <row r="61" spans="1:10" ht="49" x14ac:dyDescent="0.75">
       <c r="A61" s="3"/>
-      <c r="B61" s="25">
+      <c r="B61" s="23">
         <v>59</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -6202,8 +6226,8 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="36.75" x14ac:dyDescent="0.75">
-      <c r="A62" s="19"/>
-      <c r="B62" s="25">
+      <c r="A62" s="18"/>
+      <c r="B62" s="23">
         <v>60</v>
       </c>
       <c r="C62" s="4" t="s">
@@ -6232,8 +6256,8 @@
       </c>
     </row>
     <row r="63" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A63" s="19"/>
-      <c r="B63" s="25">
+      <c r="A63" s="18"/>
+      <c r="B63" s="23">
         <v>61</v>
       </c>
       <c r="C63" s="4" t="s">
@@ -6255,20 +6279,20 @@
       <c r="I63" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="J63" s="20" t="s">
+      <c r="J63" s="19" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="73.5" x14ac:dyDescent="0.75">
-      <c r="A64" s="19"/>
-      <c r="B64" s="25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="23">
         <v>62</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>290</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>295</v>
@@ -6281,9 +6305,12 @@
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="5"/>
-      <c r="J64" s="20" t="s">
+      <c r="J64" s="19" t="s">
         <v>296</v>
       </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.75">
+      <c r="B65" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>